<commit_message>
Vorbereitung Treffen mit Hans Rudin - Stundenachweis versioniert und PDF erstellt (Rev. C) - Stundennachweis grafisch erfasst und PDF erstellt (Rev. C) - Dokumenten Status Liste nachgeführt.
</commit_message>
<xml_diff>
--- a/ProjektManagement/NuvoControl_0011_StundenNachweis_Grafisch.xlsx
+++ b/ProjektManagement/NuvoControl_0011_StundenNachweis_Grafisch.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="33">
   <si>
     <t>Die Werte in diesem Sheet wurden mit dem Dokument "NuvoControl_0010_StundenNachweis" erfasst.</t>
   </si>
@@ -143,6 +143,12 @@
   </si>
   <si>
     <t>Version an HSR verschickt für Zwischenbewertung</t>
+  </si>
+  <si>
+    <t>c / 24-Mai-2009</t>
+  </si>
+  <si>
+    <t>Version an Hans Rudin Zwecks Zwischenbesprechung</t>
   </si>
 </sst>
 </file>
@@ -642,69 +648,69 @@
                   <c:v>54.75</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>54.75</c:v>
+                  <c:v>66</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>54.75</c:v>
+                  <c:v>84.75</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>54.75</c:v>
+                  <c:v>99.75</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>54.75</c:v>
+                  <c:v>128.75</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>54.75</c:v>
+                  <c:v>128.75</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>54.75</c:v>
+                  <c:v>128.75</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>54.75</c:v>
+                  <c:v>128.75</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>54.75</c:v>
+                  <c:v>128.75</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>54.75</c:v>
+                  <c:v>128.75</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>54.75</c:v>
+                  <c:v>128.75</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>54.75</c:v>
+                  <c:v>128.75</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>54.75</c:v>
+                  <c:v>128.75</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>54.75</c:v>
+                  <c:v>128.75</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>54.75</c:v>
+                  <c:v>128.75</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>54.75</c:v>
+                  <c:v>128.75</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>54.75</c:v>
+                  <c:v>128.75</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>54.75</c:v>
+                  <c:v>128.75</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>54.75</c:v>
+                  <c:v>128.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="113177728"/>
-        <c:axId val="113179264"/>
+        <c:axId val="133083904"/>
+        <c:axId val="133085440"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="113177728"/>
+        <c:axId val="133083904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -722,13 +728,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="113179264"/>
+        <c:crossAx val="133085440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="113179264"/>
+        <c:axId val="133085440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -760,7 +766,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="113177728"/>
+        <c:crossAx val="133083904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -783,7 +789,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.7000000000000004" r="0.7000000000000004" t="0.78740157499999996" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000051" r="0.70000000000000051" t="0.78740157499999996" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1144,69 +1150,69 @@
                   <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>49</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>49</c:v>
+                  <c:v>60.75</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>49</c:v>
+                  <c:v>74.75</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>49</c:v>
+                  <c:v>90.25</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>49</c:v>
+                  <c:v>90.25</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>49</c:v>
+                  <c:v>90.25</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>49</c:v>
+                  <c:v>90.25</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>49</c:v>
+                  <c:v>90.25</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>49</c:v>
+                  <c:v>90.25</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>49</c:v>
+                  <c:v>90.25</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>49</c:v>
+                  <c:v>90.25</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>49</c:v>
+                  <c:v>90.25</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>49</c:v>
+                  <c:v>90.25</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>49</c:v>
+                  <c:v>90.25</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>49</c:v>
+                  <c:v>90.25</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>49</c:v>
+                  <c:v>90.25</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>49</c:v>
+                  <c:v>90.25</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>49</c:v>
+                  <c:v>90.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="113283072"/>
-        <c:axId val="113284608"/>
+        <c:axId val="133111168"/>
+        <c:axId val="133129344"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="113283072"/>
+        <c:axId val="133111168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1224,13 +1230,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="113284608"/>
+        <c:crossAx val="133129344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="113284608"/>
+        <c:axId val="133129344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1262,7 +1268,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="113283072"/>
+        <c:crossAx val="133111168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1285,7 +1291,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.7000000000000004" r="0.7000000000000004" t="0.78740157499999996" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000051" r="0.70000000000000051" t="0.78740157499999996" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1646,69 +1652,69 @@
                   <c:v>103.75</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>103.75</c:v>
+                  <c:v>122</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>103.75</c:v>
+                  <c:v>145.5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>103.75</c:v>
+                  <c:v>174.5</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>103.75</c:v>
+                  <c:v>219</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>103.75</c:v>
+                  <c:v>219</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>103.75</c:v>
+                  <c:v>219</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>103.75</c:v>
+                  <c:v>219</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>103.75</c:v>
+                  <c:v>219</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>103.75</c:v>
+                  <c:v>219</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>103.75</c:v>
+                  <c:v>219</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>103.75</c:v>
+                  <c:v>219</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>103.75</c:v>
+                  <c:v>219</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>103.75</c:v>
+                  <c:v>219</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>103.75</c:v>
+                  <c:v>219</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>103.75</c:v>
+                  <c:v>219</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>103.75</c:v>
+                  <c:v>219</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>103.75</c:v>
+                  <c:v>219</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>103.75</c:v>
+                  <c:v>219</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="113842432"/>
-        <c:axId val="113844224"/>
+        <c:axId val="133166976"/>
+        <c:axId val="133168512"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="113842432"/>
+        <c:axId val="133166976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1726,13 +1732,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="113844224"/>
+        <c:crossAx val="133168512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="113844224"/>
+        <c:axId val="133168512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1764,7 +1770,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="113842432"/>
+        <c:crossAx val="133166976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1924,6 +1930,9 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="28"/>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2033,6 +2042,18 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="28"/>
+                <c:pt idx="10">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>28</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2142,6 +2163,15 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="28"/>
+                <c:pt idx="10">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2278,6 +2308,9 @@
                 <c:pt idx="9">
                   <c:v>3.5</c:v>
                 </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2402,16 +2435,28 @@
                 <c:pt idx="7">
                   <c:v>4</c:v>
                 </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.25</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.75</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="114102272"/>
-        <c:axId val="114103808"/>
+        <c:axId val="133598208"/>
+        <c:axId val="133620480"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="114102272"/>
+        <c:axId val="133598208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2429,13 +2474,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="114103808"/>
+        <c:crossAx val="133620480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="114103808"/>
+        <c:axId val="133620480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2480,7 +2525,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="114102272"/>
+        <c:crossAx val="133598208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2503,7 +2548,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.7000000000000004" r="0.7000000000000004" t="0.78740157499999996" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000051" r="0.70000000000000051" t="0.78740157499999996" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2640,6 +2685,9 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="28"/>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2749,6 +2797,12 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="28"/>
+                <c:pt idx="12">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>12</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2858,6 +2912,18 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="28"/>
+                <c:pt idx="10">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3106,16 +3172,22 @@
                 <c:pt idx="7">
                   <c:v>1.5</c:v>
                 </c:pt>
+                <c:pt idx="10">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.75</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="114144000"/>
-        <c:axId val="114145536"/>
+        <c:axId val="133537792"/>
+        <c:axId val="133539328"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="114144000"/>
+        <c:axId val="133537792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3133,13 +3205,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="114145536"/>
+        <c:crossAx val="133539328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="114145536"/>
+        <c:axId val="133539328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3184,7 +3256,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="114144000"/>
+        <c:crossAx val="133537792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3207,7 +3279,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.7000000000000004" r="0.7000000000000004" t="0.78740157499999996" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000051" r="0.70000000000000051" t="0.78740157499999996" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3383,55 +3455,55 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3573,58 +3645,58 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3766,58 +3838,58 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>11.5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>18.5</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>18.5</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>18.5</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>18.5</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>18.5</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>18.5</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>18.5</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>18.5</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0</c:v>
+                  <c:v>18.5</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0</c:v>
+                  <c:v>18.5</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0</c:v>
+                  <c:v>18.5</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0</c:v>
+                  <c:v>18.5</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0</c:v>
+                  <c:v>18.5</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0</c:v>
+                  <c:v>18.5</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0</c:v>
+                  <c:v>18.5</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0</c:v>
+                  <c:v>18.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3959,58 +4031,58 @@
                   <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43</c:v>
+                  <c:v>43.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43</c:v>
+                  <c:v>43.5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43</c:v>
+                  <c:v>43.5</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43</c:v>
+                  <c:v>43.5</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43</c:v>
+                  <c:v>43.5</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>43</c:v>
+                  <c:v>43.5</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>43</c:v>
+                  <c:v>43.5</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>43</c:v>
+                  <c:v>43.5</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>43</c:v>
+                  <c:v>43.5</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>43</c:v>
+                  <c:v>43.5</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>43</c:v>
+                  <c:v>43.5</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>43</c:v>
+                  <c:v>43.5</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>43</c:v>
+                  <c:v>43.5</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>43</c:v>
+                  <c:v>43.5</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>43</c:v>
+                  <c:v>43.5</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>43</c:v>
+                  <c:v>43.5</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>43</c:v>
+                  <c:v>43.5</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>43</c:v>
+                  <c:v>43.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4152,69 +4224,69 @@
                   <c:v>11.75</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>11.75</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11.75</c:v>
+                  <c:v>20.75</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>11.75</c:v>
+                  <c:v>21.75</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>11.75</c:v>
+                  <c:v>22.75</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>11.75</c:v>
+                  <c:v>22.75</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>11.75</c:v>
+                  <c:v>22.75</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>11.75</c:v>
+                  <c:v>22.75</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>11.75</c:v>
+                  <c:v>22.75</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>11.75</c:v>
+                  <c:v>22.75</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>11.75</c:v>
+                  <c:v>22.75</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>11.75</c:v>
+                  <c:v>22.75</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>11.75</c:v>
+                  <c:v>22.75</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>11.75</c:v>
+                  <c:v>22.75</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>11.75</c:v>
+                  <c:v>22.75</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>11.75</c:v>
+                  <c:v>22.75</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>11.75</c:v>
+                  <c:v>22.75</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>11.75</c:v>
+                  <c:v>22.75</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>11.75</c:v>
+                  <c:v>22.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="114210688"/>
-        <c:axId val="114212224"/>
+        <c:axId val="133665920"/>
+        <c:axId val="133667456"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="114210688"/>
+        <c:axId val="133665920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4232,13 +4304,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="114212224"/>
+        <c:crossAx val="133667456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="114212224"/>
+        <c:axId val="133667456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4283,7 +4355,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="114210688"/>
+        <c:crossAx val="133665920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4488,49 +4560,49 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4678,52 +4750,52 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4865,58 +4937,58 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>17.5</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>17.5</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>17.5</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>17.5</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>17.5</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>17.5</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>17.5</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0</c:v>
+                  <c:v>17.5</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0</c:v>
+                  <c:v>17.5</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0</c:v>
+                  <c:v>17.5</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0</c:v>
+                  <c:v>17.5</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0</c:v>
+                  <c:v>17.5</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0</c:v>
+                  <c:v>17.5</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0</c:v>
+                  <c:v>17.5</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0</c:v>
+                  <c:v>17.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5251,69 +5323,69 @@
                   <c:v>4.5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.5</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.5</c:v>
+                  <c:v>8.25</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4.5</c:v>
+                  <c:v>8.25</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4.5</c:v>
+                  <c:v>8.25</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>4.5</c:v>
+                  <c:v>8.25</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4.5</c:v>
+                  <c:v>8.25</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4.5</c:v>
+                  <c:v>8.25</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4.5</c:v>
+                  <c:v>8.25</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4.5</c:v>
+                  <c:v>8.25</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4.5</c:v>
+                  <c:v>8.25</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>4.5</c:v>
+                  <c:v>8.25</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>4.5</c:v>
+                  <c:v>8.25</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>4.5</c:v>
+                  <c:v>8.25</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>4.5</c:v>
+                  <c:v>8.25</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>4.5</c:v>
+                  <c:v>8.25</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>4.5</c:v>
+                  <c:v>8.25</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>4.5</c:v>
+                  <c:v>8.25</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>4.5</c:v>
+                  <c:v>8.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="114247936"/>
-        <c:axId val="114262016"/>
+        <c:axId val="133838336"/>
+        <c:axId val="133839872"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="114247936"/>
+        <c:axId val="133838336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5331,13 +5403,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="114262016"/>
+        <c:crossAx val="133839872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="114262016"/>
+        <c:axId val="133839872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5382,7 +5454,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="114247936"/>
+        <c:crossAx val="133838336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5919,10 +5991,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B3:E5"/>
+  <dimension ref="B3:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -5952,6 +6024,14 @@
       </c>
       <c r="E5" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5">
+      <c r="C6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -5971,7 +6051,7 @@
   <dimension ref="B2:O39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -6320,16 +6400,34 @@
         <f t="shared" si="1"/>
         <v>39936</v>
       </c>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
+      <c r="E16" s="9">
+        <f>0.5</f>
+        <v>0.5</v>
+      </c>
+      <c r="F16" s="9">
+        <f>1.5+2+2.5+1</f>
+        <v>7</v>
+      </c>
+      <c r="G16" s="9">
+        <f>0.5</f>
+        <v>0.5</v>
+      </c>
       <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
+      <c r="I16" s="9">
+        <f>2+0.25+1</f>
+        <v>3.25</v>
+      </c>
       <c r="K16" s="9"/>
-      <c r="L16" s="9"/>
+      <c r="L16" s="9">
+        <f>1.5+2.5+1</f>
+        <v>5</v>
+      </c>
       <c r="M16" s="9"/>
       <c r="N16" s="9"/>
-      <c r="O16" s="9"/>
+      <c r="O16" s="9">
+        <f>2</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="17" spans="2:15">
       <c r="B17" s="2">
@@ -6341,15 +6439,33 @@
         <v>39943</v>
       </c>
       <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
+      <c r="F17" s="9">
+        <f>3+1.5</f>
+        <v>4.5</v>
+      </c>
+      <c r="G17" s="9">
+        <f>1+4.5+2</f>
+        <v>7.5</v>
+      </c>
+      <c r="H17" s="9">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="I17" s="9">
+        <f>1.75+4</f>
+        <v>5.75</v>
+      </c>
       <c r="K17" s="9"/>
-      <c r="L17" s="9"/>
+      <c r="L17" s="9">
+        <f>3</f>
+        <v>3</v>
+      </c>
       <c r="M17" s="9"/>
       <c r="N17" s="9"/>
-      <c r="O17" s="9"/>
+      <c r="O17" s="9">
+        <f>1.75</f>
+        <v>1.75</v>
+      </c>
     </row>
     <row r="18" spans="2:15">
       <c r="B18" s="2">
@@ -6361,13 +6477,28 @@
         <v>39950</v>
       </c>
       <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
+      <c r="F18" s="9">
+        <f>1+2.5+3.5</f>
+        <v>7</v>
+      </c>
+      <c r="G18" s="9">
+        <f>3+0.5+1.5+0.5+1.5</f>
+        <v>7</v>
+      </c>
       <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
+      <c r="I18" s="9">
+        <f>0.5+0.5</f>
+        <v>1</v>
+      </c>
       <c r="K18" s="9"/>
-      <c r="L18" s="9"/>
-      <c r="M18" s="9"/>
+      <c r="L18" s="9">
+        <f>1+2+4</f>
+        <v>7</v>
+      </c>
+      <c r="M18" s="9">
+        <f>3+2+2</f>
+        <v>7</v>
+      </c>
       <c r="N18" s="9"/>
       <c r="O18" s="9"/>
     </row>
@@ -6382,13 +6513,28 @@
       </c>
       <c r="E19" s="9"/>
       <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
+      <c r="G19" s="9">
+        <f>3+3+5+1.5+6+7+2.5</f>
+        <v>28</v>
+      </c>
       <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
+      <c r="I19" s="9">
+        <f>1</f>
+        <v>1</v>
+      </c>
       <c r="K19" s="9"/>
-      <c r="L19" s="9"/>
-      <c r="M19" s="9"/>
-      <c r="N19" s="9"/>
+      <c r="L19" s="9">
+        <f>2.5</f>
+        <v>2.5</v>
+      </c>
+      <c r="M19" s="9">
+        <f>2+3+4+3</f>
+        <v>12</v>
+      </c>
+      <c r="N19" s="9">
+        <f>1</f>
+        <v>1</v>
+      </c>
       <c r="O19" s="9"/>
     </row>
     <row r="20" spans="2:15">
@@ -6678,23 +6824,23 @@
       <c r="C35" s="5"/>
       <c r="E35" s="6">
         <f>SUM(E6:E33)</f>
-        <v>43</v>
+        <v>43.5</v>
       </c>
       <c r="F35" s="6">
         <f>SUM(F6:F33)</f>
-        <v>0</v>
+        <v>18.5</v>
       </c>
       <c r="G35" s="6">
         <f>SUM(G6:G33)</f>
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="H35" s="6">
         <f>SUM(H6:H33)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I35" s="6">
         <f>SUM(I6:I33)</f>
-        <v>11.75</v>
+        <v>22.75</v>
       </c>
       <c r="K35" s="6">
         <f>SUM(K6:K33)</f>
@@ -6702,19 +6848,19 @@
       </c>
       <c r="L35" s="6">
         <f>SUM(L6:L33)</f>
-        <v>0</v>
+        <v>17.5</v>
       </c>
       <c r="M35" s="6">
         <f>SUM(M6:M33)</f>
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="N35" s="6">
         <f>SUM(N6:N33)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O35" s="6">
         <f>SUM(O6:O33)</f>
-        <v>4.5</v>
+        <v>8.25</v>
       </c>
     </row>
     <row r="36" spans="2:15">
@@ -6724,7 +6870,7 @@
       <c r="C36" s="5"/>
       <c r="E36" s="6">
         <f>SUM(E35:I35)</f>
-        <v>54.75</v>
+        <v>128.75</v>
       </c>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
@@ -6732,7 +6878,7 @@
       <c r="I36" s="7"/>
       <c r="K36" s="6">
         <f>SUM(K35:O35)</f>
-        <v>49</v>
+        <v>90.25</v>
       </c>
       <c r="L36" s="7"/>
       <c r="M36" s="7"/>
@@ -6746,23 +6892,23 @@
       <c r="C38" s="5"/>
       <c r="E38" s="6">
         <f>E35+K35</f>
-        <v>87.5</v>
+        <v>88</v>
       </c>
       <c r="F38" s="6">
         <f>F35+L35</f>
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="G38" s="6">
         <f>G35+M35</f>
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="H38" s="6">
         <f>H35+N35</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I38" s="6">
         <f>I35+O35</f>
-        <v>16.25</v>
+        <v>31</v>
       </c>
     </row>
     <row r="39" spans="2:15">
@@ -6772,7 +6918,7 @@
       <c r="C39" s="5"/>
       <c r="E39" s="6">
         <f>SUM(E38:I38)</f>
-        <v>103.75</v>
+        <v>219</v>
       </c>
     </row>
   </sheetData>
@@ -6796,7 +6942,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="A4" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="N43" sqref="N43"/>
     </sheetView>
   </sheetViews>
@@ -8812,15 +8958,15 @@
       </c>
       <c r="E16" s="10">
         <f>Eingabedaten!E16+Eingabedaten!K16</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F16" s="10">
         <f>Eingabedaten!F16+Eingabedaten!L16</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="G16" s="10">
         <f>Eingabedaten!G16+Eingabedaten!M16</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H16" s="10">
         <f>Eingabedaten!H16+Eingabedaten!N16</f>
@@ -8828,47 +8974,47 @@
       </c>
       <c r="I16" s="10">
         <f>Eingabedaten!I16+Eingabedaten!O16</f>
-        <v>0</v>
+        <v>5.25</v>
       </c>
       <c r="J16" s="10">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>18.25</v>
       </c>
       <c r="L16" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="M16" s="10">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>12.5</v>
       </c>
       <c r="N16" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="O16" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="P16" s="10">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>18.25</v>
       </c>
       <c r="Q16" s="10">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>57.25</v>
       </c>
       <c r="S16" s="10">
         <f>Eingabedaten!E16+'Eingabedaten (berechnet)'!S15</f>
-        <v>43</v>
+        <v>43.5</v>
       </c>
       <c r="T16" s="10">
         <f>Eingabedaten!F16+'Eingabedaten (berechnet)'!T15</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="U16" s="10">
         <f>Eingabedaten!G16+'Eingabedaten (berechnet)'!U15</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="V16" s="10">
         <f>Eingabedaten!H16+'Eingabedaten (berechnet)'!V15</f>
@@ -8876,11 +9022,11 @@
       </c>
       <c r="W16" s="10">
         <f>Eingabedaten!I16+'Eingabedaten (berechnet)'!W15</f>
-        <v>11.75</v>
+        <v>15</v>
       </c>
       <c r="X16" s="10">
         <f t="shared" si="7"/>
-        <v>54.75</v>
+        <v>66</v>
       </c>
       <c r="Z16" s="10">
         <f>Z15+Eingabedaten!K16</f>
@@ -8888,7 +9034,7 @@
       </c>
       <c r="AA16" s="10">
         <f>AA15+Eingabedaten!L16</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AB16" s="10">
         <f>AB15+Eingabedaten!M16</f>
@@ -8900,15 +9046,15 @@
       </c>
       <c r="AD16" s="10">
         <f>AD15+Eingabedaten!O16</f>
-        <v>4.5</v>
+        <v>6.5</v>
       </c>
       <c r="AE16" s="10">
         <f t="shared" si="8"/>
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="AG16" s="10">
         <f t="shared" si="9"/>
-        <v>103.75</v>
+        <v>122</v>
       </c>
     </row>
     <row r="17" spans="2:33">
@@ -8926,23 +9072,23 @@
       </c>
       <c r="F17" s="10">
         <f>Eingabedaten!F17+Eingabedaten!L17</f>
-        <v>0</v>
+        <v>7.5</v>
       </c>
       <c r="G17" s="10">
         <f>Eingabedaten!G17+Eingabedaten!M17</f>
-        <v>0</v>
+        <v>7.5</v>
       </c>
       <c r="H17" s="10">
         <f>Eingabedaten!H17+Eingabedaten!N17</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I17" s="10">
         <f>Eingabedaten!I17+Eingabedaten!O17</f>
-        <v>0</v>
+        <v>7.5</v>
       </c>
       <c r="J17" s="10">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>23.5</v>
       </c>
       <c r="L17" s="10">
         <f t="shared" si="0"/>
@@ -8950,47 +9096,47 @@
       </c>
       <c r="M17" s="10">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>7.5</v>
       </c>
       <c r="N17" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="O17" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="P17" s="10">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>23.5</v>
       </c>
       <c r="Q17" s="10">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="S17" s="10">
         <f>Eingabedaten!E17+'Eingabedaten (berechnet)'!S16</f>
-        <v>43</v>
+        <v>43.5</v>
       </c>
       <c r="T17" s="10">
         <f>Eingabedaten!F17+'Eingabedaten (berechnet)'!T16</f>
-        <v>0</v>
+        <v>11.5</v>
       </c>
       <c r="U17" s="10">
         <f>Eingabedaten!G17+'Eingabedaten (berechnet)'!U16</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="V17" s="10">
         <f>Eingabedaten!H17+'Eingabedaten (berechnet)'!V16</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W17" s="10">
         <f>Eingabedaten!I17+'Eingabedaten (berechnet)'!W16</f>
-        <v>11.75</v>
+        <v>20.75</v>
       </c>
       <c r="X17" s="10">
         <f t="shared" si="7"/>
-        <v>54.75</v>
+        <v>84.75</v>
       </c>
       <c r="Z17" s="10">
         <f>Z16+Eingabedaten!K17</f>
@@ -8998,7 +9144,7 @@
       </c>
       <c r="AA17" s="10">
         <f>AA16+Eingabedaten!L17</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AB17" s="10">
         <f>AB16+Eingabedaten!M17</f>
@@ -9010,15 +9156,15 @@
       </c>
       <c r="AD17" s="10">
         <f>AD16+Eingabedaten!O17</f>
-        <v>4.5</v>
+        <v>8.25</v>
       </c>
       <c r="AE17" s="10">
         <f t="shared" si="8"/>
-        <v>49</v>
+        <v>60.75</v>
       </c>
       <c r="AG17" s="10">
         <f t="shared" si="9"/>
-        <v>103.75</v>
+        <v>145.5</v>
       </c>
     </row>
     <row r="18" spans="2:33">
@@ -9036,11 +9182,11 @@
       </c>
       <c r="F18" s="10">
         <f>Eingabedaten!F18+Eingabedaten!L18</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="G18" s="10">
         <f>Eingabedaten!G18+Eingabedaten!M18</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="H18" s="10">
         <f>Eingabedaten!H18+Eingabedaten!N18</f>
@@ -9048,11 +9194,11 @@
       </c>
       <c r="I18" s="10">
         <f>Eingabedaten!I18+Eingabedaten!O18</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J18" s="10">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="L18" s="10">
         <f t="shared" si="0"/>
@@ -9060,47 +9206,47 @@
       </c>
       <c r="M18" s="10">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="N18" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="O18" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="P18" s="10">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="Q18" s="10">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>99</v>
       </c>
       <c r="S18" s="10">
         <f>Eingabedaten!E18+'Eingabedaten (berechnet)'!S17</f>
-        <v>43</v>
+        <v>43.5</v>
       </c>
       <c r="T18" s="10">
         <f>Eingabedaten!F18+'Eingabedaten (berechnet)'!T17</f>
-        <v>0</v>
+        <v>18.5</v>
       </c>
       <c r="U18" s="10">
         <f>Eingabedaten!G18+'Eingabedaten (berechnet)'!U17</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="V18" s="10">
         <f>Eingabedaten!H18+'Eingabedaten (berechnet)'!V17</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W18" s="10">
         <f>Eingabedaten!I18+'Eingabedaten (berechnet)'!W17</f>
-        <v>11.75</v>
+        <v>21.75</v>
       </c>
       <c r="X18" s="10">
         <f t="shared" si="7"/>
-        <v>54.75</v>
+        <v>99.75</v>
       </c>
       <c r="Z18" s="10">
         <f>Z17+Eingabedaten!K18</f>
@@ -9108,11 +9254,11 @@
       </c>
       <c r="AA18" s="10">
         <f>AA17+Eingabedaten!L18</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AB18" s="10">
         <f>AB17+Eingabedaten!M18</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AC18" s="10">
         <f>AC17+Eingabedaten!N18</f>
@@ -9120,15 +9266,15 @@
       </c>
       <c r="AD18" s="10">
         <f>AD17+Eingabedaten!O18</f>
-        <v>4.5</v>
+        <v>8.25</v>
       </c>
       <c r="AE18" s="10">
         <f t="shared" si="8"/>
-        <v>49</v>
+        <v>74.75</v>
       </c>
       <c r="AG18" s="10">
         <f t="shared" si="9"/>
-        <v>103.75</v>
+        <v>174.5</v>
       </c>
     </row>
     <row r="19" spans="2:33">
@@ -9146,23 +9292,23 @@
       </c>
       <c r="F19" s="10">
         <f>Eingabedaten!F19+Eingabedaten!L19</f>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="G19" s="10">
         <f>Eingabedaten!G19+Eingabedaten!M19</f>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="H19" s="10">
         <f>Eingabedaten!H19+Eingabedaten!N19</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I19" s="10">
         <f>Eingabedaten!I19+Eingabedaten!O19</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J19" s="10">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>44.5</v>
       </c>
       <c r="L19" s="10">
         <f t="shared" si="0"/>
@@ -9170,47 +9316,47 @@
       </c>
       <c r="M19" s="10">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="N19" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>42.5</v>
       </c>
       <c r="O19" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>43.5</v>
       </c>
       <c r="P19" s="10">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>44.5</v>
       </c>
       <c r="Q19" s="10">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>133</v>
       </c>
       <c r="S19" s="10">
         <f>Eingabedaten!E19+'Eingabedaten (berechnet)'!S18</f>
-        <v>43</v>
+        <v>43.5</v>
       </c>
       <c r="T19" s="10">
         <f>Eingabedaten!F19+'Eingabedaten (berechnet)'!T18</f>
-        <v>0</v>
+        <v>18.5</v>
       </c>
       <c r="U19" s="10">
         <f>Eingabedaten!G19+'Eingabedaten (berechnet)'!U18</f>
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="V19" s="10">
         <f>Eingabedaten!H19+'Eingabedaten (berechnet)'!V18</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W19" s="10">
         <f>Eingabedaten!I19+'Eingabedaten (berechnet)'!W18</f>
-        <v>11.75</v>
+        <v>22.75</v>
       </c>
       <c r="X19" s="10">
         <f t="shared" si="7"/>
-        <v>54.75</v>
+        <v>128.75</v>
       </c>
       <c r="Z19" s="10">
         <f>Z18+Eingabedaten!K19</f>
@@ -9218,27 +9364,27 @@
       </c>
       <c r="AA19" s="10">
         <f>AA18+Eingabedaten!L19</f>
-        <v>0</v>
+        <v>17.5</v>
       </c>
       <c r="AB19" s="10">
         <f>AB18+Eingabedaten!M19</f>
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="AC19" s="10">
         <f>AC18+Eingabedaten!N19</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD19" s="10">
         <f>AD18+Eingabedaten!O19</f>
-        <v>4.5</v>
+        <v>8.25</v>
       </c>
       <c r="AE19" s="10">
         <f t="shared" si="8"/>
-        <v>49</v>
+        <v>90.25</v>
       </c>
       <c r="AG19" s="10">
         <f t="shared" si="9"/>
-        <v>103.75</v>
+        <v>219</v>
       </c>
     </row>
     <row r="20" spans="2:33">
@@ -9300,27 +9446,27 @@
       </c>
       <c r="S20" s="10">
         <f>Eingabedaten!E20+'Eingabedaten (berechnet)'!S19</f>
-        <v>43</v>
+        <v>43.5</v>
       </c>
       <c r="T20" s="10">
         <f>Eingabedaten!F20+'Eingabedaten (berechnet)'!T19</f>
-        <v>0</v>
+        <v>18.5</v>
       </c>
       <c r="U20" s="10">
         <f>Eingabedaten!G20+'Eingabedaten (berechnet)'!U19</f>
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="V20" s="10">
         <f>Eingabedaten!H20+'Eingabedaten (berechnet)'!V19</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W20" s="10">
         <f>Eingabedaten!I20+'Eingabedaten (berechnet)'!W19</f>
-        <v>11.75</v>
+        <v>22.75</v>
       </c>
       <c r="X20" s="10">
         <f t="shared" si="7"/>
-        <v>54.75</v>
+        <v>128.75</v>
       </c>
       <c r="Z20" s="10">
         <f>Z19+Eingabedaten!K20</f>
@@ -9328,27 +9474,27 @@
       </c>
       <c r="AA20" s="10">
         <f>AA19+Eingabedaten!L20</f>
-        <v>0</v>
+        <v>17.5</v>
       </c>
       <c r="AB20" s="10">
         <f>AB19+Eingabedaten!M20</f>
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="AC20" s="10">
         <f>AC19+Eingabedaten!N20</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD20" s="10">
         <f>AD19+Eingabedaten!O20</f>
-        <v>4.5</v>
+        <v>8.25</v>
       </c>
       <c r="AE20" s="10">
         <f t="shared" si="8"/>
-        <v>49</v>
+        <v>90.25</v>
       </c>
       <c r="AG20" s="10">
         <f t="shared" si="9"/>
-        <v>103.75</v>
+        <v>219</v>
       </c>
     </row>
     <row r="21" spans="2:33">
@@ -9410,27 +9556,27 @@
       </c>
       <c r="S21" s="10">
         <f>Eingabedaten!E21+'Eingabedaten (berechnet)'!S20</f>
-        <v>43</v>
+        <v>43.5</v>
       </c>
       <c r="T21" s="10">
         <f>Eingabedaten!F21+'Eingabedaten (berechnet)'!T20</f>
-        <v>0</v>
+        <v>18.5</v>
       </c>
       <c r="U21" s="10">
         <f>Eingabedaten!G21+'Eingabedaten (berechnet)'!U20</f>
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="V21" s="10">
         <f>Eingabedaten!H21+'Eingabedaten (berechnet)'!V20</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W21" s="10">
         <f>Eingabedaten!I21+'Eingabedaten (berechnet)'!W20</f>
-        <v>11.75</v>
+        <v>22.75</v>
       </c>
       <c r="X21" s="10">
         <f t="shared" si="7"/>
-        <v>54.75</v>
+        <v>128.75</v>
       </c>
       <c r="Z21" s="10">
         <f>Z20+Eingabedaten!K21</f>
@@ -9438,27 +9584,27 @@
       </c>
       <c r="AA21" s="10">
         <f>AA20+Eingabedaten!L21</f>
-        <v>0</v>
+        <v>17.5</v>
       </c>
       <c r="AB21" s="10">
         <f>AB20+Eingabedaten!M21</f>
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="AC21" s="10">
         <f>AC20+Eingabedaten!N21</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD21" s="10">
         <f>AD20+Eingabedaten!O21</f>
-        <v>4.5</v>
+        <v>8.25</v>
       </c>
       <c r="AE21" s="10">
         <f t="shared" si="8"/>
-        <v>49</v>
+        <v>90.25</v>
       </c>
       <c r="AG21" s="10">
         <f t="shared" si="9"/>
-        <v>103.75</v>
+        <v>219</v>
       </c>
     </row>
     <row r="22" spans="2:33">
@@ -9520,27 +9666,27 @@
       </c>
       <c r="S22" s="10">
         <f>Eingabedaten!E22+'Eingabedaten (berechnet)'!S21</f>
-        <v>43</v>
+        <v>43.5</v>
       </c>
       <c r="T22" s="10">
         <f>Eingabedaten!F22+'Eingabedaten (berechnet)'!T21</f>
-        <v>0</v>
+        <v>18.5</v>
       </c>
       <c r="U22" s="10">
         <f>Eingabedaten!G22+'Eingabedaten (berechnet)'!U21</f>
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="V22" s="10">
         <f>Eingabedaten!H22+'Eingabedaten (berechnet)'!V21</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W22" s="10">
         <f>Eingabedaten!I22+'Eingabedaten (berechnet)'!W21</f>
-        <v>11.75</v>
+        <v>22.75</v>
       </c>
       <c r="X22" s="10">
         <f t="shared" si="7"/>
-        <v>54.75</v>
+        <v>128.75</v>
       </c>
       <c r="Z22" s="10">
         <f>Z21+Eingabedaten!K22</f>
@@ -9548,27 +9694,27 @@
       </c>
       <c r="AA22" s="10">
         <f>AA21+Eingabedaten!L22</f>
-        <v>0</v>
+        <v>17.5</v>
       </c>
       <c r="AB22" s="10">
         <f>AB21+Eingabedaten!M22</f>
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="AC22" s="10">
         <f>AC21+Eingabedaten!N22</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD22" s="10">
         <f>AD21+Eingabedaten!O22</f>
-        <v>4.5</v>
+        <v>8.25</v>
       </c>
       <c r="AE22" s="10">
         <f t="shared" si="8"/>
-        <v>49</v>
+        <v>90.25</v>
       </c>
       <c r="AG22" s="10">
         <f t="shared" si="9"/>
-        <v>103.75</v>
+        <v>219</v>
       </c>
     </row>
     <row r="23" spans="2:33">
@@ -9630,27 +9776,27 @@
       </c>
       <c r="S23" s="10">
         <f>Eingabedaten!E23+'Eingabedaten (berechnet)'!S22</f>
-        <v>43</v>
+        <v>43.5</v>
       </c>
       <c r="T23" s="10">
         <f>Eingabedaten!F23+'Eingabedaten (berechnet)'!T22</f>
-        <v>0</v>
+        <v>18.5</v>
       </c>
       <c r="U23" s="10">
         <f>Eingabedaten!G23+'Eingabedaten (berechnet)'!U22</f>
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="V23" s="10">
         <f>Eingabedaten!H23+'Eingabedaten (berechnet)'!V22</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W23" s="10">
         <f>Eingabedaten!I23+'Eingabedaten (berechnet)'!W22</f>
-        <v>11.75</v>
+        <v>22.75</v>
       </c>
       <c r="X23" s="10">
         <f t="shared" si="7"/>
-        <v>54.75</v>
+        <v>128.75</v>
       </c>
       <c r="Z23" s="10">
         <f>Z22+Eingabedaten!K23</f>
@@ -9658,27 +9804,27 @@
       </c>
       <c r="AA23" s="10">
         <f>AA22+Eingabedaten!L23</f>
-        <v>0</v>
+        <v>17.5</v>
       </c>
       <c r="AB23" s="10">
         <f>AB22+Eingabedaten!M23</f>
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="AC23" s="10">
         <f>AC22+Eingabedaten!N23</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD23" s="10">
         <f>AD22+Eingabedaten!O23</f>
-        <v>4.5</v>
+        <v>8.25</v>
       </c>
       <c r="AE23" s="10">
         <f t="shared" si="8"/>
-        <v>49</v>
+        <v>90.25</v>
       </c>
       <c r="AG23" s="10">
         <f t="shared" si="9"/>
-        <v>103.75</v>
+        <v>219</v>
       </c>
     </row>
     <row r="24" spans="2:33">
@@ -9740,27 +9886,27 @@
       </c>
       <c r="S24" s="10">
         <f>Eingabedaten!E24+'Eingabedaten (berechnet)'!S23</f>
-        <v>43</v>
+        <v>43.5</v>
       </c>
       <c r="T24" s="10">
         <f>Eingabedaten!F24+'Eingabedaten (berechnet)'!T23</f>
-        <v>0</v>
+        <v>18.5</v>
       </c>
       <c r="U24" s="10">
         <f>Eingabedaten!G24+'Eingabedaten (berechnet)'!U23</f>
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="V24" s="10">
         <f>Eingabedaten!H24+'Eingabedaten (berechnet)'!V23</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W24" s="10">
         <f>Eingabedaten!I24+'Eingabedaten (berechnet)'!W23</f>
-        <v>11.75</v>
+        <v>22.75</v>
       </c>
       <c r="X24" s="10">
         <f t="shared" si="7"/>
-        <v>54.75</v>
+        <v>128.75</v>
       </c>
       <c r="Z24" s="10">
         <f>Z23+Eingabedaten!K24</f>
@@ -9768,27 +9914,27 @@
       </c>
       <c r="AA24" s="10">
         <f>AA23+Eingabedaten!L24</f>
-        <v>0</v>
+        <v>17.5</v>
       </c>
       <c r="AB24" s="10">
         <f>AB23+Eingabedaten!M24</f>
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="AC24" s="10">
         <f>AC23+Eingabedaten!N24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD24" s="10">
         <f>AD23+Eingabedaten!O24</f>
-        <v>4.5</v>
+        <v>8.25</v>
       </c>
       <c r="AE24" s="10">
         <f t="shared" si="8"/>
-        <v>49</v>
+        <v>90.25</v>
       </c>
       <c r="AG24" s="10">
         <f t="shared" si="9"/>
-        <v>103.75</v>
+        <v>219</v>
       </c>
     </row>
     <row r="25" spans="2:33">
@@ -9850,27 +9996,27 @@
       </c>
       <c r="S25" s="10">
         <f>Eingabedaten!E25+'Eingabedaten (berechnet)'!S24</f>
-        <v>43</v>
+        <v>43.5</v>
       </c>
       <c r="T25" s="10">
         <f>Eingabedaten!F25+'Eingabedaten (berechnet)'!T24</f>
-        <v>0</v>
+        <v>18.5</v>
       </c>
       <c r="U25" s="10">
         <f>Eingabedaten!G25+'Eingabedaten (berechnet)'!U24</f>
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="V25" s="10">
         <f>Eingabedaten!H25+'Eingabedaten (berechnet)'!V24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W25" s="10">
         <f>Eingabedaten!I25+'Eingabedaten (berechnet)'!W24</f>
-        <v>11.75</v>
+        <v>22.75</v>
       </c>
       <c r="X25" s="10">
         <f t="shared" si="7"/>
-        <v>54.75</v>
+        <v>128.75</v>
       </c>
       <c r="Z25" s="10">
         <f>Z24+Eingabedaten!K25</f>
@@ -9878,27 +10024,27 @@
       </c>
       <c r="AA25" s="10">
         <f>AA24+Eingabedaten!L25</f>
-        <v>0</v>
+        <v>17.5</v>
       </c>
       <c r="AB25" s="10">
         <f>AB24+Eingabedaten!M25</f>
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="AC25" s="10">
         <f>AC24+Eingabedaten!N25</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD25" s="10">
         <f>AD24+Eingabedaten!O25</f>
-        <v>4.5</v>
+        <v>8.25</v>
       </c>
       <c r="AE25" s="10">
         <f t="shared" si="8"/>
-        <v>49</v>
+        <v>90.25</v>
       </c>
       <c r="AG25" s="10">
         <f t="shared" si="9"/>
-        <v>103.75</v>
+        <v>219</v>
       </c>
     </row>
     <row r="26" spans="2:33">
@@ -9960,27 +10106,27 @@
       </c>
       <c r="S26" s="10">
         <f>Eingabedaten!E26+'Eingabedaten (berechnet)'!S25</f>
-        <v>43</v>
+        <v>43.5</v>
       </c>
       <c r="T26" s="10">
         <f>Eingabedaten!F26+'Eingabedaten (berechnet)'!T25</f>
-        <v>0</v>
+        <v>18.5</v>
       </c>
       <c r="U26" s="10">
         <f>Eingabedaten!G26+'Eingabedaten (berechnet)'!U25</f>
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="V26" s="10">
         <f>Eingabedaten!H26+'Eingabedaten (berechnet)'!V25</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W26" s="10">
         <f>Eingabedaten!I26+'Eingabedaten (berechnet)'!W25</f>
-        <v>11.75</v>
+        <v>22.75</v>
       </c>
       <c r="X26" s="10">
         <f t="shared" si="7"/>
-        <v>54.75</v>
+        <v>128.75</v>
       </c>
       <c r="Z26" s="10">
         <f>Z25+Eingabedaten!K26</f>
@@ -9988,27 +10134,27 @@
       </c>
       <c r="AA26" s="10">
         <f>AA25+Eingabedaten!L26</f>
-        <v>0</v>
+        <v>17.5</v>
       </c>
       <c r="AB26" s="10">
         <f>AB25+Eingabedaten!M26</f>
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="AC26" s="10">
         <f>AC25+Eingabedaten!N26</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD26" s="10">
         <f>AD25+Eingabedaten!O26</f>
-        <v>4.5</v>
+        <v>8.25</v>
       </c>
       <c r="AE26" s="10">
         <f t="shared" si="8"/>
-        <v>49</v>
+        <v>90.25</v>
       </c>
       <c r="AG26" s="10">
         <f t="shared" si="9"/>
-        <v>103.75</v>
+        <v>219</v>
       </c>
     </row>
     <row r="27" spans="2:33">
@@ -10070,27 +10216,27 @@
       </c>
       <c r="S27" s="10">
         <f>Eingabedaten!E27+'Eingabedaten (berechnet)'!S26</f>
-        <v>43</v>
+        <v>43.5</v>
       </c>
       <c r="T27" s="10">
         <f>Eingabedaten!F27+'Eingabedaten (berechnet)'!T26</f>
-        <v>0</v>
+        <v>18.5</v>
       </c>
       <c r="U27" s="10">
         <f>Eingabedaten!G27+'Eingabedaten (berechnet)'!U26</f>
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="V27" s="10">
         <f>Eingabedaten!H27+'Eingabedaten (berechnet)'!V26</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W27" s="10">
         <f>Eingabedaten!I27+'Eingabedaten (berechnet)'!W26</f>
-        <v>11.75</v>
+        <v>22.75</v>
       </c>
       <c r="X27" s="10">
         <f t="shared" si="7"/>
-        <v>54.75</v>
+        <v>128.75</v>
       </c>
       <c r="Z27" s="10">
         <f>Z26+Eingabedaten!K27</f>
@@ -10098,27 +10244,27 @@
       </c>
       <c r="AA27" s="10">
         <f>AA26+Eingabedaten!L27</f>
-        <v>0</v>
+        <v>17.5</v>
       </c>
       <c r="AB27" s="10">
         <f>AB26+Eingabedaten!M27</f>
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="AC27" s="10">
         <f>AC26+Eingabedaten!N27</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD27" s="10">
         <f>AD26+Eingabedaten!O27</f>
-        <v>4.5</v>
+        <v>8.25</v>
       </c>
       <c r="AE27" s="10">
         <f t="shared" si="8"/>
-        <v>49</v>
+        <v>90.25</v>
       </c>
       <c r="AG27" s="10">
         <f t="shared" si="9"/>
-        <v>103.75</v>
+        <v>219</v>
       </c>
     </row>
     <row r="28" spans="2:33">
@@ -10180,27 +10326,27 @@
       </c>
       <c r="S28" s="10">
         <f>Eingabedaten!E28+'Eingabedaten (berechnet)'!S27</f>
-        <v>43</v>
+        <v>43.5</v>
       </c>
       <c r="T28" s="10">
         <f>Eingabedaten!F28+'Eingabedaten (berechnet)'!T27</f>
-        <v>0</v>
+        <v>18.5</v>
       </c>
       <c r="U28" s="10">
         <f>Eingabedaten!G28+'Eingabedaten (berechnet)'!U27</f>
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="V28" s="10">
         <f>Eingabedaten!H28+'Eingabedaten (berechnet)'!V27</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W28" s="10">
         <f>Eingabedaten!I28+'Eingabedaten (berechnet)'!W27</f>
-        <v>11.75</v>
+        <v>22.75</v>
       </c>
       <c r="X28" s="10">
         <f t="shared" si="7"/>
-        <v>54.75</v>
+        <v>128.75</v>
       </c>
       <c r="Z28" s="10">
         <f>Z27+Eingabedaten!K28</f>
@@ -10208,27 +10354,27 @@
       </c>
       <c r="AA28" s="10">
         <f>AA27+Eingabedaten!L28</f>
-        <v>0</v>
+        <v>17.5</v>
       </c>
       <c r="AB28" s="10">
         <f>AB27+Eingabedaten!M28</f>
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="AC28" s="10">
         <f>AC27+Eingabedaten!N28</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD28" s="10">
         <f>AD27+Eingabedaten!O28</f>
-        <v>4.5</v>
+        <v>8.25</v>
       </c>
       <c r="AE28" s="10">
         <f t="shared" si="8"/>
-        <v>49</v>
+        <v>90.25</v>
       </c>
       <c r="AG28" s="10">
         <f t="shared" si="9"/>
-        <v>103.75</v>
+        <v>219</v>
       </c>
     </row>
     <row r="29" spans="2:33">
@@ -10290,27 +10436,27 @@
       </c>
       <c r="S29" s="10">
         <f>Eingabedaten!E29+'Eingabedaten (berechnet)'!S28</f>
-        <v>43</v>
+        <v>43.5</v>
       </c>
       <c r="T29" s="10">
         <f>Eingabedaten!F29+'Eingabedaten (berechnet)'!T28</f>
-        <v>0</v>
+        <v>18.5</v>
       </c>
       <c r="U29" s="10">
         <f>Eingabedaten!G29+'Eingabedaten (berechnet)'!U28</f>
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="V29" s="10">
         <f>Eingabedaten!H29+'Eingabedaten (berechnet)'!V28</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W29" s="10">
         <f>Eingabedaten!I29+'Eingabedaten (berechnet)'!W28</f>
-        <v>11.75</v>
+        <v>22.75</v>
       </c>
       <c r="X29" s="10">
         <f t="shared" si="7"/>
-        <v>54.75</v>
+        <v>128.75</v>
       </c>
       <c r="Z29" s="10">
         <f>Z28+Eingabedaten!K29</f>
@@ -10318,27 +10464,27 @@
       </c>
       <c r="AA29" s="10">
         <f>AA28+Eingabedaten!L29</f>
-        <v>0</v>
+        <v>17.5</v>
       </c>
       <c r="AB29" s="10">
         <f>AB28+Eingabedaten!M29</f>
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="AC29" s="10">
         <f>AC28+Eingabedaten!N29</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD29" s="10">
         <f>AD28+Eingabedaten!O29</f>
-        <v>4.5</v>
+        <v>8.25</v>
       </c>
       <c r="AE29" s="10">
         <f t="shared" si="8"/>
-        <v>49</v>
+        <v>90.25</v>
       </c>
       <c r="AG29" s="10">
         <f t="shared" si="9"/>
-        <v>103.75</v>
+        <v>219</v>
       </c>
     </row>
     <row r="30" spans="2:33">
@@ -10400,27 +10546,27 @@
       </c>
       <c r="S30" s="10">
         <f>Eingabedaten!E30+'Eingabedaten (berechnet)'!S29</f>
-        <v>43</v>
+        <v>43.5</v>
       </c>
       <c r="T30" s="10">
         <f>Eingabedaten!F30+'Eingabedaten (berechnet)'!T29</f>
-        <v>0</v>
+        <v>18.5</v>
       </c>
       <c r="U30" s="10">
         <f>Eingabedaten!G30+'Eingabedaten (berechnet)'!U29</f>
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="V30" s="10">
         <f>Eingabedaten!H30+'Eingabedaten (berechnet)'!V29</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W30" s="10">
         <f>Eingabedaten!I30+'Eingabedaten (berechnet)'!W29</f>
-        <v>11.75</v>
+        <v>22.75</v>
       </c>
       <c r="X30" s="10">
         <f t="shared" si="7"/>
-        <v>54.75</v>
+        <v>128.75</v>
       </c>
       <c r="Z30" s="10">
         <f>Z29+Eingabedaten!K30</f>
@@ -10428,27 +10574,27 @@
       </c>
       <c r="AA30" s="10">
         <f>AA29+Eingabedaten!L30</f>
-        <v>0</v>
+        <v>17.5</v>
       </c>
       <c r="AB30" s="10">
         <f>AB29+Eingabedaten!M30</f>
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="AC30" s="10">
         <f>AC29+Eingabedaten!N30</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD30" s="10">
         <f>AD29+Eingabedaten!O30</f>
-        <v>4.5</v>
+        <v>8.25</v>
       </c>
       <c r="AE30" s="10">
         <f t="shared" si="8"/>
-        <v>49</v>
+        <v>90.25</v>
       </c>
       <c r="AG30" s="10">
         <f t="shared" si="9"/>
-        <v>103.75</v>
+        <v>219</v>
       </c>
     </row>
     <row r="31" spans="2:33">
@@ -10510,27 +10656,27 @@
       </c>
       <c r="S31" s="10">
         <f>Eingabedaten!E31+'Eingabedaten (berechnet)'!S30</f>
-        <v>43</v>
+        <v>43.5</v>
       </c>
       <c r="T31" s="10">
         <f>Eingabedaten!F31+'Eingabedaten (berechnet)'!T30</f>
-        <v>0</v>
+        <v>18.5</v>
       </c>
       <c r="U31" s="10">
         <f>Eingabedaten!G31+'Eingabedaten (berechnet)'!U30</f>
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="V31" s="10">
         <f>Eingabedaten!H31+'Eingabedaten (berechnet)'!V30</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W31" s="10">
         <f>Eingabedaten!I31+'Eingabedaten (berechnet)'!W30</f>
-        <v>11.75</v>
+        <v>22.75</v>
       </c>
       <c r="X31" s="10">
         <f t="shared" si="7"/>
-        <v>54.75</v>
+        <v>128.75</v>
       </c>
       <c r="Z31" s="10">
         <f>Z30+Eingabedaten!K31</f>
@@ -10538,27 +10684,27 @@
       </c>
       <c r="AA31" s="10">
         <f>AA30+Eingabedaten!L31</f>
-        <v>0</v>
+        <v>17.5</v>
       </c>
       <c r="AB31" s="10">
         <f>AB30+Eingabedaten!M31</f>
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="AC31" s="10">
         <f>AC30+Eingabedaten!N31</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD31" s="10">
         <f>AD30+Eingabedaten!O31</f>
-        <v>4.5</v>
+        <v>8.25</v>
       </c>
       <c r="AE31" s="10">
         <f t="shared" si="8"/>
-        <v>49</v>
+        <v>90.25</v>
       </c>
       <c r="AG31" s="10">
         <f t="shared" si="9"/>
-        <v>103.75</v>
+        <v>219</v>
       </c>
     </row>
     <row r="32" spans="2:33">
@@ -10620,27 +10766,27 @@
       </c>
       <c r="S32" s="10">
         <f>Eingabedaten!E32+'Eingabedaten (berechnet)'!S31</f>
-        <v>43</v>
+        <v>43.5</v>
       </c>
       <c r="T32" s="10">
         <f>Eingabedaten!F32+'Eingabedaten (berechnet)'!T31</f>
-        <v>0</v>
+        <v>18.5</v>
       </c>
       <c r="U32" s="10">
         <f>Eingabedaten!G32+'Eingabedaten (berechnet)'!U31</f>
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="V32" s="10">
         <f>Eingabedaten!H32+'Eingabedaten (berechnet)'!V31</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W32" s="10">
         <f>Eingabedaten!I32+'Eingabedaten (berechnet)'!W31</f>
-        <v>11.75</v>
+        <v>22.75</v>
       </c>
       <c r="X32" s="10">
         <f t="shared" si="7"/>
-        <v>54.75</v>
+        <v>128.75</v>
       </c>
       <c r="Z32" s="10">
         <f>Z31+Eingabedaten!K32</f>
@@ -10648,27 +10794,27 @@
       </c>
       <c r="AA32" s="10">
         <f>AA31+Eingabedaten!L32</f>
-        <v>0</v>
+        <v>17.5</v>
       </c>
       <c r="AB32" s="10">
         <f>AB31+Eingabedaten!M32</f>
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="AC32" s="10">
         <f>AC31+Eingabedaten!N32</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD32" s="10">
         <f>AD31+Eingabedaten!O32</f>
-        <v>4.5</v>
+        <v>8.25</v>
       </c>
       <c r="AE32" s="10">
         <f t="shared" si="8"/>
-        <v>49</v>
+        <v>90.25</v>
       </c>
       <c r="AG32" s="10">
         <f t="shared" si="9"/>
-        <v>103.75</v>
+        <v>219</v>
       </c>
     </row>
     <row r="33" spans="2:33">
@@ -10730,27 +10876,27 @@
       </c>
       <c r="S33" s="10">
         <f>Eingabedaten!E33+'Eingabedaten (berechnet)'!S32</f>
-        <v>43</v>
+        <v>43.5</v>
       </c>
       <c r="T33" s="10">
         <f>Eingabedaten!F33+'Eingabedaten (berechnet)'!T32</f>
-        <v>0</v>
+        <v>18.5</v>
       </c>
       <c r="U33" s="10">
         <f>Eingabedaten!G33+'Eingabedaten (berechnet)'!U32</f>
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="V33" s="10">
         <f>Eingabedaten!H33+'Eingabedaten (berechnet)'!V32</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W33" s="10">
         <f>Eingabedaten!I33+'Eingabedaten (berechnet)'!W32</f>
-        <v>11.75</v>
+        <v>22.75</v>
       </c>
       <c r="X33" s="10">
         <f t="shared" si="7"/>
-        <v>54.75</v>
+        <v>128.75</v>
       </c>
       <c r="Z33" s="10">
         <f>Z32+Eingabedaten!K33</f>
@@ -10758,59 +10904,59 @@
       </c>
       <c r="AA33" s="10">
         <f>AA32+Eingabedaten!L33</f>
-        <v>0</v>
+        <v>17.5</v>
       </c>
       <c r="AB33" s="10">
         <f>AB32+Eingabedaten!M33</f>
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="AC33" s="10">
         <f>AC32+Eingabedaten!N33</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD33" s="10">
         <f>AD32+Eingabedaten!O33</f>
-        <v>4.5</v>
+        <v>8.25</v>
       </c>
       <c r="AE33" s="10">
         <f t="shared" si="8"/>
-        <v>49</v>
+        <v>90.25</v>
       </c>
       <c r="AG33" s="10">
         <f t="shared" si="9"/>
-        <v>103.75</v>
+        <v>219</v>
       </c>
     </row>
     <row r="35" spans="2:33">
       <c r="E35" s="6">
         <f t="shared" ref="E35:J35" si="12">SUM(E6:E33)</f>
-        <v>87.5</v>
+        <v>88</v>
       </c>
       <c r="F35" s="6">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="G35" s="6">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="H35" s="6">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I35" s="6">
         <f t="shared" si="12"/>
-        <v>16.25</v>
+        <v>31</v>
       </c>
       <c r="J35" s="6">
         <f t="shared" si="12"/>
-        <v>103.75</v>
+        <v>219</v>
       </c>
     </row>
     <row r="36" spans="2:33">
       <c r="E36" s="6">
         <f>SUM(E35:I35)</f>
-        <v>103.75</v>
+        <v>219</v>
       </c>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>

</xml_diff>

<commit_message>
Prepare for Meeting at Tuesday, 30-June-2009
</commit_message>
<xml_diff>
--- a/ProjektManagement/NuvoControl_0011_StundenNachweis_Grafisch.xlsx
+++ b/ProjektManagement/NuvoControl_0011_StundenNachweis_Grafisch.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="34">
   <si>
     <t>Die Werte in diesem Sheet wurden mit dem Dokument "NuvoControl_0010_StundenNachweis" erfasst.</t>
   </si>
@@ -149,6 +149,9 @@
   </si>
   <si>
     <t>Version an Hans Rudin Zwecks Zwischenbesprechung</t>
+  </si>
+  <si>
+    <t>d / 29-Mai-2009</t>
   </si>
 </sst>
 </file>
@@ -660,57 +663,57 @@
                   <c:v>128.75</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>128.75</c:v>
+                  <c:v>158.25</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>128.75</c:v>
+                  <c:v>165.25</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>128.75</c:v>
+                  <c:v>196.75</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>128.75</c:v>
+                  <c:v>220.25</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>128.75</c:v>
+                  <c:v>237.75</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>128.75</c:v>
+                  <c:v>237.75</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>128.75</c:v>
+                  <c:v>237.75</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>128.75</c:v>
+                  <c:v>237.75</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>128.75</c:v>
+                  <c:v>237.75</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>128.75</c:v>
+                  <c:v>237.75</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>128.75</c:v>
+                  <c:v>237.75</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>128.75</c:v>
+                  <c:v>237.75</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>128.75</c:v>
+                  <c:v>237.75</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>128.75</c:v>
+                  <c:v>237.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="133083904"/>
-        <c:axId val="133085440"/>
+        <c:axId val="127190144"/>
+        <c:axId val="127191680"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="133083904"/>
+        <c:axId val="127190144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -728,13 +731,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="133085440"/>
+        <c:crossAx val="127191680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="133085440"/>
+        <c:axId val="127191680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -766,7 +769,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="133083904"/>
+        <c:crossAx val="127190144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -789,7 +792,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.70000000000000051" r="0.70000000000000051" t="0.78740157499999996" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000062" r="0.70000000000000062" t="0.78740157499999996" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1159,60 +1162,60 @@
                   <c:v>74.75</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>90.25</c:v>
+                  <c:v>93.25</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>90.25</c:v>
+                  <c:v>109.25</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>90.25</c:v>
+                  <c:v>109.25</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>90.25</c:v>
+                  <c:v>139.25</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>90.25</c:v>
+                  <c:v>165.75</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>90.25</c:v>
+                  <c:v>173.75</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>90.25</c:v>
+                  <c:v>173.75</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>90.25</c:v>
+                  <c:v>173.75</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>90.25</c:v>
+                  <c:v>173.75</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>90.25</c:v>
+                  <c:v>173.75</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>90.25</c:v>
+                  <c:v>173.75</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>90.25</c:v>
+                  <c:v>173.75</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>90.25</c:v>
+                  <c:v>173.75</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>90.25</c:v>
+                  <c:v>173.75</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>90.25</c:v>
+                  <c:v>173.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="133111168"/>
-        <c:axId val="133129344"/>
+        <c:axId val="127229952"/>
+        <c:axId val="127231488"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="133111168"/>
+        <c:axId val="127229952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1230,13 +1233,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="133129344"/>
+        <c:crossAx val="127231488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="133129344"/>
+        <c:axId val="127231488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1268,7 +1271,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="133111168"/>
+        <c:crossAx val="127229952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1291,7 +1294,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.70000000000000051" r="0.70000000000000051" t="0.78740157499999996" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000062" r="0.70000000000000062" t="0.78740157499999996" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1661,60 +1664,60 @@
                   <c:v>174.5</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>219</c:v>
+                  <c:v>222</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>219</c:v>
+                  <c:v>267.5</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>219</c:v>
+                  <c:v>274.5</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>219</c:v>
+                  <c:v>336</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>219</c:v>
+                  <c:v>386</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>219</c:v>
+                  <c:v>411.5</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>219</c:v>
+                  <c:v>411.5</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>219</c:v>
+                  <c:v>411.5</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>219</c:v>
+                  <c:v>411.5</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>219</c:v>
+                  <c:v>411.5</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>219</c:v>
+                  <c:v>411.5</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>219</c:v>
+                  <c:v>411.5</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>219</c:v>
+                  <c:v>411.5</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>219</c:v>
+                  <c:v>411.5</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>219</c:v>
+                  <c:v>411.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="133166976"/>
-        <c:axId val="133168512"/>
+        <c:axId val="127260928"/>
+        <c:axId val="127266816"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="133166976"/>
+        <c:axId val="127260928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1732,13 +1735,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="133168512"/>
+        <c:crossAx val="127266816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="133168512"/>
+        <c:axId val="127266816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1770,7 +1773,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="133166976"/>
+        <c:crossAx val="127260928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1933,6 +1936,18 @@
                 <c:pt idx="11">
                   <c:v>1</c:v>
                 </c:pt>
+                <c:pt idx="14">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6.5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2054,6 +2069,21 @@
                 <c:pt idx="13">
                   <c:v>28</c:v>
                 </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>10</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2172,6 +2202,12 @@
                 <c:pt idx="12">
                   <c:v>7</c:v>
                 </c:pt>
+                <c:pt idx="14">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2447,16 +2483,28 @@
                 <c:pt idx="13">
                   <c:v>1</c:v>
                 </c:pt>
+                <c:pt idx="14">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="133598208"/>
-        <c:axId val="133620480"/>
+        <c:axId val="128748928"/>
+        <c:axId val="128763008"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="133598208"/>
+        <c:axId val="128748928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2474,13 +2522,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="133620480"/>
+        <c:crossAx val="128763008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="133620480"/>
+        <c:axId val="128763008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2525,7 +2573,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="133598208"/>
+        <c:crossAx val="128748928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2548,7 +2596,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.70000000000000051" r="0.70000000000000051" t="0.78740157499999996" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000062" r="0.70000000000000062" t="0.78740157499999996" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2688,6 +2736,12 @@
                 <c:pt idx="13">
                   <c:v>1</c:v>
                 </c:pt>
+                <c:pt idx="17">
+                  <c:v>10.5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2803,6 +2857,15 @@
                 <c:pt idx="13">
                   <c:v>12</c:v>
                 </c:pt>
+                <c:pt idx="14">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2922,7 +2985,19 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.5</c:v>
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3178,16 +3253,22 @@
                 <c:pt idx="11">
                   <c:v>1.75</c:v>
                 </c:pt>
+                <c:pt idx="14">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="133537792"/>
-        <c:axId val="133539328"/>
+        <c:axId val="128692608"/>
+        <c:axId val="128694144"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="133537792"/>
+        <c:axId val="128692608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3205,13 +3286,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="133539328"/>
+        <c:crossAx val="128694144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="133539328"/>
+        <c:axId val="128694144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3256,7 +3337,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="133537792"/>
+        <c:crossAx val="128692608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3279,7 +3360,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.70000000000000051" r="0.70000000000000051" t="0.78740157499999996" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000062" r="0.70000000000000062" t="0.78740157499999996" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3464,46 +3545,46 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1</c:v>
+                  <c:v>10.5</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1</c:v>
+                  <c:v>27.5</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3657,46 +3738,46 @@
                   <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43</c:v>
+                  <c:v>44.5</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>43</c:v>
+                  <c:v>51.5</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>43</c:v>
+                  <c:v>65.5</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>43</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>43</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>43</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>43</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>43</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>43</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>43</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>43</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>43</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>43</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>43</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3850,46 +3931,46 @@
                   <c:v>18.5</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>18.5</c:v>
+                  <c:v>23.5</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>18.5</c:v>
+                  <c:v>23.5</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>18.5</c:v>
+                  <c:v>27.5</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>18.5</c:v>
+                  <c:v>27.5</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>18.5</c:v>
+                  <c:v>27.5</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>18.5</c:v>
+                  <c:v>27.5</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>18.5</c:v>
+                  <c:v>27.5</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>18.5</c:v>
+                  <c:v>27.5</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>18.5</c:v>
+                  <c:v>27.5</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>18.5</c:v>
+                  <c:v>27.5</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>18.5</c:v>
+                  <c:v>27.5</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>18.5</c:v>
+                  <c:v>27.5</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>18.5</c:v>
+                  <c:v>27.5</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>18.5</c:v>
+                  <c:v>27.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4236,57 +4317,57 @@
                   <c:v>22.75</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>22.75</c:v>
+                  <c:v>40.75</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>22.75</c:v>
+                  <c:v>40.75</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>22.75</c:v>
+                  <c:v>49.75</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>22.75</c:v>
+                  <c:v>51.75</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>22.75</c:v>
+                  <c:v>52.75</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>22.75</c:v>
+                  <c:v>52.75</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>22.75</c:v>
+                  <c:v>52.75</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>22.75</c:v>
+                  <c:v>52.75</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>22.75</c:v>
+                  <c:v>52.75</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>22.75</c:v>
+                  <c:v>52.75</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>22.75</c:v>
+                  <c:v>52.75</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>22.75</c:v>
+                  <c:v>52.75</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>22.75</c:v>
+                  <c:v>52.75</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>22.75</c:v>
+                  <c:v>52.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="133665920"/>
-        <c:axId val="133667456"/>
+        <c:axId val="128947712"/>
+        <c:axId val="128949248"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="133665920"/>
+        <c:axId val="128947712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4304,13 +4385,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="133667456"/>
+        <c:crossAx val="128949248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="133667456"/>
+        <c:axId val="128949248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4355,7 +4436,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="133665920"/>
+        <c:crossAx val="128947712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4572,37 +4653,37 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1</c:v>
+                  <c:v>11.5</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4756,46 +4837,46 @@
                   <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>19</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>19</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>19</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>19</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>19</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>19</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>19</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>19</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>19</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>19</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>19</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>19</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>19</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>19</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4946,49 +5027,49 @@
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>17.5</c:v>
+                  <c:v>20.5</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>17.5</c:v>
+                  <c:v>30.5</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>17.5</c:v>
+                  <c:v>30.5</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>17.5</c:v>
+                  <c:v>46.5</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>17.5</c:v>
+                  <c:v>56.5</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>17.5</c:v>
+                  <c:v>63.5</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>17.5</c:v>
+                  <c:v>63.5</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>17.5</c:v>
+                  <c:v>63.5</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>17.5</c:v>
+                  <c:v>63.5</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>17.5</c:v>
+                  <c:v>63.5</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>17.5</c:v>
+                  <c:v>63.5</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>17.5</c:v>
+                  <c:v>63.5</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>17.5</c:v>
+                  <c:v>63.5</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>17.5</c:v>
+                  <c:v>63.5</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>17.5</c:v>
+                  <c:v>63.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5335,57 +5416,57 @@
                   <c:v>8.25</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>8.25</c:v>
+                  <c:v>12.25</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>8.25</c:v>
+                  <c:v>12.25</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>8.25</c:v>
+                  <c:v>12.25</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>8.25</c:v>
+                  <c:v>14.25</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>8.25</c:v>
+                  <c:v>14.25</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>8.25</c:v>
+                  <c:v>14.25</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>8.25</c:v>
+                  <c:v>14.25</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>8.25</c:v>
+                  <c:v>14.25</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>8.25</c:v>
+                  <c:v>14.25</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>8.25</c:v>
+                  <c:v>14.25</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>8.25</c:v>
+                  <c:v>14.25</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>8.25</c:v>
+                  <c:v>14.25</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>8.25</c:v>
+                  <c:v>14.25</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>8.25</c:v>
+                  <c:v>14.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="133838336"/>
-        <c:axId val="133839872"/>
+        <c:axId val="128984960"/>
+        <c:axId val="128986496"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="133838336"/>
+        <c:axId val="128984960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5403,13 +5484,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="133839872"/>
+        <c:crossAx val="128986496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="133839872"/>
+        <c:axId val="128986496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5454,7 +5535,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="133838336"/>
+        <c:crossAx val="128984960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5991,11 +6072,9 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B3:E6"/>
+  <dimension ref="B3:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
@@ -6031,6 +6110,14 @@
         <v>31</v>
       </c>
       <c r="E6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5">
+      <c r="C7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" t="s">
         <v>32</v>
       </c>
     </row>
@@ -6051,7 +6138,8 @@
   <dimension ref="B2:O39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <pane ySplit="5" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -6524,8 +6612,8 @@
       </c>
       <c r="K19" s="9"/>
       <c r="L19" s="9">
-        <f>2.5</f>
-        <v>2.5</v>
+        <f>2.5+3</f>
+        <v>5.5</v>
       </c>
       <c r="M19" s="9">
         <f>2+3+4+3</f>
@@ -6547,15 +6635,36 @@
         <v>39964</v>
       </c>
       <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
+      <c r="F20" s="9">
+        <f>5</f>
+        <v>5</v>
+      </c>
+      <c r="G20" s="9">
+        <f>1.5</f>
+        <v>1.5</v>
+      </c>
+      <c r="H20" s="9">
+        <f>1.5+3.5</f>
+        <v>5</v>
+      </c>
+      <c r="I20" s="9">
+        <f>1+3+1+13</f>
+        <v>18</v>
+      </c>
       <c r="K20" s="9"/>
-      <c r="L20" s="9"/>
-      <c r="M20" s="9"/>
+      <c r="L20" s="9">
+        <f>2+8</f>
+        <v>10</v>
+      </c>
+      <c r="M20" s="9">
+        <f>2</f>
+        <v>2</v>
+      </c>
       <c r="N20" s="9"/>
-      <c r="O20" s="9"/>
+      <c r="O20" s="9">
+        <f>1+3</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="21" spans="2:15">
       <c r="B21" s="2">
@@ -6568,7 +6677,10 @@
       </c>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
+      <c r="G21" s="9">
+        <f>7</f>
+        <v>7</v>
+      </c>
       <c r="H21" s="9"/>
       <c r="I21" s="9"/>
       <c r="K21" s="9"/>
@@ -6587,13 +6699,31 @@
         <v>39978</v>
       </c>
       <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
+      <c r="F22" s="9">
+        <f>4</f>
+        <v>4</v>
+      </c>
+      <c r="G22" s="9">
+        <f>5+2+1+5+1</f>
+        <v>14</v>
+      </c>
+      <c r="H22" s="9">
+        <f>0.5+4</f>
+        <v>4.5</v>
+      </c>
+      <c r="I22" s="9">
+        <f>0.5+0.5+1+1+1+5</f>
+        <v>9</v>
+      </c>
       <c r="K22" s="9"/>
-      <c r="L22" s="9"/>
-      <c r="M22" s="9"/>
+      <c r="L22" s="9">
+        <f>4+12</f>
+        <v>16</v>
+      </c>
+      <c r="M22" s="9">
+        <f>2+7+3+2</f>
+        <v>14</v>
+      </c>
       <c r="N22" s="9"/>
       <c r="O22" s="9"/>
     </row>
@@ -6608,14 +6738,35 @@
       </c>
       <c r="E23" s="9"/>
       <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
+      <c r="G23" s="9">
+        <f>3+1.5</f>
+        <v>4.5</v>
+      </c>
+      <c r="H23" s="9">
+        <f>2.5+2+4+6+2.5</f>
+        <v>17</v>
+      </c>
+      <c r="I23" s="9">
+        <f>2</f>
+        <v>2</v>
+      </c>
       <c r="K23" s="9"/>
-      <c r="L23" s="9"/>
-      <c r="M23" s="9"/>
-      <c r="N23" s="9"/>
-      <c r="O23" s="9"/>
+      <c r="L23" s="9">
+        <f>2+8</f>
+        <v>10</v>
+      </c>
+      <c r="M23" s="9">
+        <f>2+2</f>
+        <v>4</v>
+      </c>
+      <c r="N23" s="9">
+        <f>2+2.5+6</f>
+        <v>10.5</v>
+      </c>
+      <c r="O23" s="9">
+        <f>2</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="24" spans="2:15">
       <c r="B24" s="2">
@@ -6628,13 +6779,28 @@
       </c>
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
+      <c r="G24" s="9">
+        <f>5+2+3</f>
+        <v>10</v>
+      </c>
+      <c r="H24" s="9">
+        <f>1.5+4+1</f>
+        <v>6.5</v>
+      </c>
+      <c r="I24" s="9">
+        <f>1</f>
+        <v>1</v>
+      </c>
       <c r="K24" s="9"/>
-      <c r="L24" s="9"/>
+      <c r="L24" s="9">
+        <f>4+3</f>
+        <v>7</v>
+      </c>
       <c r="M24" s="9"/>
-      <c r="N24" s="9"/>
+      <c r="N24" s="9">
+        <f>1</f>
+        <v>1</v>
+      </c>
       <c r="O24" s="9"/>
     </row>
     <row r="25" spans="2:15">
@@ -6828,19 +6994,19 @@
       </c>
       <c r="F35" s="6">
         <f>SUM(F6:F33)</f>
-        <v>18.5</v>
+        <v>27.5</v>
       </c>
       <c r="G35" s="6">
         <f>SUM(G6:G33)</f>
-        <v>43</v>
+        <v>80</v>
       </c>
       <c r="H35" s="6">
         <f>SUM(H6:H33)</f>
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="I35" s="6">
         <f>SUM(I6:I33)</f>
-        <v>22.75</v>
+        <v>52.75</v>
       </c>
       <c r="K35" s="6">
         <f>SUM(K6:K33)</f>
@@ -6848,19 +7014,19 @@
       </c>
       <c r="L35" s="6">
         <f>SUM(L6:L33)</f>
-        <v>17.5</v>
+        <v>63.5</v>
       </c>
       <c r="M35" s="6">
         <f>SUM(M6:M33)</f>
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="N35" s="6">
         <f>SUM(N6:N33)</f>
-        <v>1</v>
+        <v>12.5</v>
       </c>
       <c r="O35" s="6">
         <f>SUM(O6:O33)</f>
-        <v>8.25</v>
+        <v>14.25</v>
       </c>
     </row>
     <row r="36" spans="2:15">
@@ -6870,7 +7036,7 @@
       <c r="C36" s="5"/>
       <c r="E36" s="6">
         <f>SUM(E35:I35)</f>
-        <v>128.75</v>
+        <v>237.75</v>
       </c>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
@@ -6878,7 +7044,7 @@
       <c r="I36" s="7"/>
       <c r="K36" s="6">
         <f>SUM(K35:O35)</f>
-        <v>90.25</v>
+        <v>173.75</v>
       </c>
       <c r="L36" s="7"/>
       <c r="M36" s="7"/>
@@ -6896,19 +7062,19 @@
       </c>
       <c r="F38" s="6">
         <f>F35+L35</f>
-        <v>36</v>
+        <v>91</v>
       </c>
       <c r="G38" s="6">
         <f>G35+M35</f>
-        <v>62</v>
+        <v>119</v>
       </c>
       <c r="H38" s="6">
         <f>H35+N35</f>
-        <v>2</v>
+        <v>46.5</v>
       </c>
       <c r="I38" s="6">
         <f>I35+O35</f>
-        <v>31</v>
+        <v>67</v>
       </c>
     </row>
     <row r="39" spans="2:15">
@@ -6918,7 +7084,7 @@
       <c r="C39" s="5"/>
       <c r="E39" s="6">
         <f>SUM(E38:I38)</f>
-        <v>219</v>
+        <v>411.5</v>
       </c>
     </row>
   </sheetData>
@@ -6942,7 +7108,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A4" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="N43" sqref="N43"/>
     </sheetView>
   </sheetViews>
@@ -9292,7 +9458,7 @@
       </c>
       <c r="F19" s="10">
         <f>Eingabedaten!F19+Eingabedaten!L19</f>
-        <v>2.5</v>
+        <v>5.5</v>
       </c>
       <c r="G19" s="10">
         <f>Eingabedaten!G19+Eingabedaten!M19</f>
@@ -9308,7 +9474,7 @@
       </c>
       <c r="J19" s="10">
         <f t="shared" si="5"/>
-        <v>44.5</v>
+        <v>47.5</v>
       </c>
       <c r="L19" s="10">
         <f t="shared" si="0"/>
@@ -9316,23 +9482,23 @@
       </c>
       <c r="M19" s="10">
         <f t="shared" si="1"/>
-        <v>2.5</v>
+        <v>5.5</v>
       </c>
       <c r="N19" s="10">
         <f t="shared" si="2"/>
-        <v>42.5</v>
+        <v>45.5</v>
       </c>
       <c r="O19" s="10">
         <f t="shared" si="3"/>
-        <v>43.5</v>
+        <v>46.5</v>
       </c>
       <c r="P19" s="10">
         <f t="shared" si="4"/>
-        <v>44.5</v>
+        <v>47.5</v>
       </c>
       <c r="Q19" s="10">
         <f t="shared" si="6"/>
-        <v>133</v>
+        <v>145</v>
       </c>
       <c r="S19" s="10">
         <f>Eingabedaten!E19+'Eingabedaten (berechnet)'!S18</f>
@@ -9364,7 +9530,7 @@
       </c>
       <c r="AA19" s="10">
         <f>AA18+Eingabedaten!L19</f>
-        <v>17.5</v>
+        <v>20.5</v>
       </c>
       <c r="AB19" s="10">
         <f>AB18+Eingabedaten!M19</f>
@@ -9380,11 +9546,11 @@
       </c>
       <c r="AE19" s="10">
         <f t="shared" si="8"/>
-        <v>90.25</v>
+        <v>93.25</v>
       </c>
       <c r="AG19" s="10">
         <f t="shared" si="9"/>
-        <v>219</v>
+        <v>222</v>
       </c>
     </row>
     <row r="20" spans="2:33">
@@ -9402,23 +9568,23 @@
       </c>
       <c r="F20" s="10">
         <f>Eingabedaten!F20+Eingabedaten!L20</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="G20" s="10">
         <f>Eingabedaten!G20+Eingabedaten!M20</f>
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="H20" s="10">
         <f>Eingabedaten!H20+Eingabedaten!N20</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I20" s="10">
         <f>Eingabedaten!I20+Eingabedaten!O20</f>
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="J20" s="10">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>45.5</v>
       </c>
       <c r="L20" s="10">
         <f t="shared" si="0"/>
@@ -9426,23 +9592,23 @@
       </c>
       <c r="M20" s="10">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="N20" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>18.5</v>
       </c>
       <c r="O20" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>23.5</v>
       </c>
       <c r="P20" s="10">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>45.5</v>
       </c>
       <c r="Q20" s="10">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>102.5</v>
       </c>
       <c r="S20" s="10">
         <f>Eingabedaten!E20+'Eingabedaten (berechnet)'!S19</f>
@@ -9450,23 +9616,23 @@
       </c>
       <c r="T20" s="10">
         <f>Eingabedaten!F20+'Eingabedaten (berechnet)'!T19</f>
-        <v>18.5</v>
+        <v>23.5</v>
       </c>
       <c r="U20" s="10">
         <f>Eingabedaten!G20+'Eingabedaten (berechnet)'!U19</f>
-        <v>43</v>
+        <v>44.5</v>
       </c>
       <c r="V20" s="10">
         <f>Eingabedaten!H20+'Eingabedaten (berechnet)'!V19</f>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="W20" s="10">
         <f>Eingabedaten!I20+'Eingabedaten (berechnet)'!W19</f>
-        <v>22.75</v>
+        <v>40.75</v>
       </c>
       <c r="X20" s="10">
         <f t="shared" si="7"/>
-        <v>128.75</v>
+        <v>158.25</v>
       </c>
       <c r="Z20" s="10">
         <f>Z19+Eingabedaten!K20</f>
@@ -9474,11 +9640,11 @@
       </c>
       <c r="AA20" s="10">
         <f>AA19+Eingabedaten!L20</f>
-        <v>17.5</v>
+        <v>30.5</v>
       </c>
       <c r="AB20" s="10">
         <f>AB19+Eingabedaten!M20</f>
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="AC20" s="10">
         <f>AC19+Eingabedaten!N20</f>
@@ -9486,15 +9652,15 @@
       </c>
       <c r="AD20" s="10">
         <f>AD19+Eingabedaten!O20</f>
-        <v>8.25</v>
+        <v>12.25</v>
       </c>
       <c r="AE20" s="10">
         <f t="shared" si="8"/>
-        <v>90.25</v>
+        <v>109.25</v>
       </c>
       <c r="AG20" s="10">
         <f t="shared" si="9"/>
-        <v>219</v>
+        <v>267.5</v>
       </c>
     </row>
     <row r="21" spans="2:33">
@@ -9516,7 +9682,7 @@
       </c>
       <c r="G21" s="10">
         <f>Eingabedaten!G21+Eingabedaten!M21</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H21" s="10">
         <f>Eingabedaten!H21+Eingabedaten!N21</f>
@@ -9528,7 +9694,7 @@
       </c>
       <c r="J21" s="10">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="L21" s="10">
         <f t="shared" si="0"/>
@@ -9540,19 +9706,19 @@
       </c>
       <c r="N21" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="O21" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="P21" s="10">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="Q21" s="10">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="S21" s="10">
         <f>Eingabedaten!E21+'Eingabedaten (berechnet)'!S20</f>
@@ -9560,23 +9726,23 @@
       </c>
       <c r="T21" s="10">
         <f>Eingabedaten!F21+'Eingabedaten (berechnet)'!T20</f>
-        <v>18.5</v>
+        <v>23.5</v>
       </c>
       <c r="U21" s="10">
         <f>Eingabedaten!G21+'Eingabedaten (berechnet)'!U20</f>
-        <v>43</v>
+        <v>51.5</v>
       </c>
       <c r="V21" s="10">
         <f>Eingabedaten!H21+'Eingabedaten (berechnet)'!V20</f>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="W21" s="10">
         <f>Eingabedaten!I21+'Eingabedaten (berechnet)'!W20</f>
-        <v>22.75</v>
+        <v>40.75</v>
       </c>
       <c r="X21" s="10">
         <f t="shared" si="7"/>
-        <v>128.75</v>
+        <v>165.25</v>
       </c>
       <c r="Z21" s="10">
         <f>Z20+Eingabedaten!K21</f>
@@ -9584,11 +9750,11 @@
       </c>
       <c r="AA21" s="10">
         <f>AA20+Eingabedaten!L21</f>
-        <v>17.5</v>
+        <v>30.5</v>
       </c>
       <c r="AB21" s="10">
         <f>AB20+Eingabedaten!M21</f>
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="AC21" s="10">
         <f>AC20+Eingabedaten!N21</f>
@@ -9596,15 +9762,15 @@
       </c>
       <c r="AD21" s="10">
         <f>AD20+Eingabedaten!O21</f>
-        <v>8.25</v>
+        <v>12.25</v>
       </c>
       <c r="AE21" s="10">
         <f t="shared" si="8"/>
-        <v>90.25</v>
+        <v>109.25</v>
       </c>
       <c r="AG21" s="10">
         <f t="shared" si="9"/>
-        <v>219</v>
+        <v>274.5</v>
       </c>
     </row>
     <row r="22" spans="2:33">
@@ -9622,23 +9788,23 @@
       </c>
       <c r="F22" s="10">
         <f>Eingabedaten!F22+Eingabedaten!L22</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G22" s="10">
         <f>Eingabedaten!G22+Eingabedaten!M22</f>
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="H22" s="10">
         <f>Eingabedaten!H22+Eingabedaten!N22</f>
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="I22" s="10">
         <f>Eingabedaten!I22+Eingabedaten!O22</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J22" s="10">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>61.5</v>
       </c>
       <c r="L22" s="10">
         <f t="shared" si="0"/>
@@ -9646,23 +9812,23 @@
       </c>
       <c r="M22" s="10">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="N22" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="O22" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>52.5</v>
       </c>
       <c r="P22" s="10">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>61.5</v>
       </c>
       <c r="Q22" s="10">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>182</v>
       </c>
       <c r="S22" s="10">
         <f>Eingabedaten!E22+'Eingabedaten (berechnet)'!S21</f>
@@ -9670,23 +9836,23 @@
       </c>
       <c r="T22" s="10">
         <f>Eingabedaten!F22+'Eingabedaten (berechnet)'!T21</f>
-        <v>18.5</v>
+        <v>27.5</v>
       </c>
       <c r="U22" s="10">
         <f>Eingabedaten!G22+'Eingabedaten (berechnet)'!U21</f>
-        <v>43</v>
+        <v>65.5</v>
       </c>
       <c r="V22" s="10">
         <f>Eingabedaten!H22+'Eingabedaten (berechnet)'!V21</f>
-        <v>1</v>
+        <v>10.5</v>
       </c>
       <c r="W22" s="10">
         <f>Eingabedaten!I22+'Eingabedaten (berechnet)'!W21</f>
-        <v>22.75</v>
+        <v>49.75</v>
       </c>
       <c r="X22" s="10">
         <f t="shared" si="7"/>
-        <v>128.75</v>
+        <v>196.75</v>
       </c>
       <c r="Z22" s="10">
         <f>Z21+Eingabedaten!K22</f>
@@ -9694,11 +9860,11 @@
       </c>
       <c r="AA22" s="10">
         <f>AA21+Eingabedaten!L22</f>
-        <v>17.5</v>
+        <v>46.5</v>
       </c>
       <c r="AB22" s="10">
         <f>AB21+Eingabedaten!M22</f>
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="AC22" s="10">
         <f>AC21+Eingabedaten!N22</f>
@@ -9706,15 +9872,15 @@
       </c>
       <c r="AD22" s="10">
         <f>AD21+Eingabedaten!O22</f>
-        <v>8.25</v>
+        <v>12.25</v>
       </c>
       <c r="AE22" s="10">
         <f t="shared" si="8"/>
-        <v>90.25</v>
+        <v>139.25</v>
       </c>
       <c r="AG22" s="10">
         <f t="shared" si="9"/>
-        <v>219</v>
+        <v>336</v>
       </c>
     </row>
     <row r="23" spans="2:33">
@@ -9732,23 +9898,23 @@
       </c>
       <c r="F23" s="10">
         <f>Eingabedaten!F23+Eingabedaten!L23</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G23" s="10">
         <f>Eingabedaten!G23+Eingabedaten!M23</f>
-        <v>0</v>
+        <v>8.5</v>
       </c>
       <c r="H23" s="10">
         <f>Eingabedaten!H23+Eingabedaten!N23</f>
-        <v>0</v>
+        <v>27.5</v>
       </c>
       <c r="I23" s="10">
         <f>Eingabedaten!I23+Eingabedaten!O23</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J23" s="10">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="L23" s="10">
         <f t="shared" si="0"/>
@@ -9756,23 +9922,23 @@
       </c>
       <c r="M23" s="10">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="N23" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>18.5</v>
       </c>
       <c r="O23" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="P23" s="10">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="Q23" s="10">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>124.5</v>
       </c>
       <c r="S23" s="10">
         <f>Eingabedaten!E23+'Eingabedaten (berechnet)'!S22</f>
@@ -9780,23 +9946,23 @@
       </c>
       <c r="T23" s="10">
         <f>Eingabedaten!F23+'Eingabedaten (berechnet)'!T22</f>
-        <v>18.5</v>
+        <v>27.5</v>
       </c>
       <c r="U23" s="10">
         <f>Eingabedaten!G23+'Eingabedaten (berechnet)'!U22</f>
-        <v>43</v>
+        <v>70</v>
       </c>
       <c r="V23" s="10">
         <f>Eingabedaten!H23+'Eingabedaten (berechnet)'!V22</f>
-        <v>1</v>
+        <v>27.5</v>
       </c>
       <c r="W23" s="10">
         <f>Eingabedaten!I23+'Eingabedaten (berechnet)'!W22</f>
-        <v>22.75</v>
+        <v>51.75</v>
       </c>
       <c r="X23" s="10">
         <f t="shared" si="7"/>
-        <v>128.75</v>
+        <v>220.25</v>
       </c>
       <c r="Z23" s="10">
         <f>Z22+Eingabedaten!K23</f>
@@ -9804,27 +9970,27 @@
       </c>
       <c r="AA23" s="10">
         <f>AA22+Eingabedaten!L23</f>
-        <v>17.5</v>
+        <v>56.5</v>
       </c>
       <c r="AB23" s="10">
         <f>AB22+Eingabedaten!M23</f>
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="AC23" s="10">
         <f>AC22+Eingabedaten!N23</f>
-        <v>1</v>
+        <v>11.5</v>
       </c>
       <c r="AD23" s="10">
         <f>AD22+Eingabedaten!O23</f>
-        <v>8.25</v>
+        <v>14.25</v>
       </c>
       <c r="AE23" s="10">
         <f t="shared" si="8"/>
-        <v>90.25</v>
+        <v>165.75</v>
       </c>
       <c r="AG23" s="10">
         <f t="shared" si="9"/>
-        <v>219</v>
+        <v>386</v>
       </c>
     </row>
     <row r="24" spans="2:33">
@@ -9842,23 +10008,23 @@
       </c>
       <c r="F24" s="10">
         <f>Eingabedaten!F24+Eingabedaten!L24</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G24" s="10">
         <f>Eingabedaten!G24+Eingabedaten!M24</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H24" s="10">
         <f>Eingabedaten!H24+Eingabedaten!N24</f>
-        <v>0</v>
+        <v>7.5</v>
       </c>
       <c r="I24" s="10">
         <f>Eingabedaten!I24+Eingabedaten!O24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J24" s="10">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>25.5</v>
       </c>
       <c r="L24" s="10">
         <f t="shared" si="0"/>
@@ -9866,23 +10032,23 @@
       </c>
       <c r="M24" s="10">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="N24" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="O24" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>24.5</v>
       </c>
       <c r="P24" s="10">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>25.5</v>
       </c>
       <c r="Q24" s="10">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>74</v>
       </c>
       <c r="S24" s="10">
         <f>Eingabedaten!E24+'Eingabedaten (berechnet)'!S23</f>
@@ -9890,23 +10056,23 @@
       </c>
       <c r="T24" s="10">
         <f>Eingabedaten!F24+'Eingabedaten (berechnet)'!T23</f>
-        <v>18.5</v>
+        <v>27.5</v>
       </c>
       <c r="U24" s="10">
         <f>Eingabedaten!G24+'Eingabedaten (berechnet)'!U23</f>
-        <v>43</v>
+        <v>80</v>
       </c>
       <c r="V24" s="10">
         <f>Eingabedaten!H24+'Eingabedaten (berechnet)'!V23</f>
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="W24" s="10">
         <f>Eingabedaten!I24+'Eingabedaten (berechnet)'!W23</f>
-        <v>22.75</v>
+        <v>52.75</v>
       </c>
       <c r="X24" s="10">
         <f t="shared" si="7"/>
-        <v>128.75</v>
+        <v>237.75</v>
       </c>
       <c r="Z24" s="10">
         <f>Z23+Eingabedaten!K24</f>
@@ -9914,27 +10080,27 @@
       </c>
       <c r="AA24" s="10">
         <f>AA23+Eingabedaten!L24</f>
-        <v>17.5</v>
+        <v>63.5</v>
       </c>
       <c r="AB24" s="10">
         <f>AB23+Eingabedaten!M24</f>
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="AC24" s="10">
         <f>AC23+Eingabedaten!N24</f>
-        <v>1</v>
+        <v>12.5</v>
       </c>
       <c r="AD24" s="10">
         <f>AD23+Eingabedaten!O24</f>
-        <v>8.25</v>
+        <v>14.25</v>
       </c>
       <c r="AE24" s="10">
         <f t="shared" si="8"/>
-        <v>90.25</v>
+        <v>173.75</v>
       </c>
       <c r="AG24" s="10">
         <f t="shared" si="9"/>
-        <v>219</v>
+        <v>411.5</v>
       </c>
     </row>
     <row r="25" spans="2:33">
@@ -10000,23 +10166,23 @@
       </c>
       <c r="T25" s="10">
         <f>Eingabedaten!F25+'Eingabedaten (berechnet)'!T24</f>
-        <v>18.5</v>
+        <v>27.5</v>
       </c>
       <c r="U25" s="10">
         <f>Eingabedaten!G25+'Eingabedaten (berechnet)'!U24</f>
-        <v>43</v>
+        <v>80</v>
       </c>
       <c r="V25" s="10">
         <f>Eingabedaten!H25+'Eingabedaten (berechnet)'!V24</f>
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="W25" s="10">
         <f>Eingabedaten!I25+'Eingabedaten (berechnet)'!W24</f>
-        <v>22.75</v>
+        <v>52.75</v>
       </c>
       <c r="X25" s="10">
         <f t="shared" si="7"/>
-        <v>128.75</v>
+        <v>237.75</v>
       </c>
       <c r="Z25" s="10">
         <f>Z24+Eingabedaten!K25</f>
@@ -10024,27 +10190,27 @@
       </c>
       <c r="AA25" s="10">
         <f>AA24+Eingabedaten!L25</f>
-        <v>17.5</v>
+        <v>63.5</v>
       </c>
       <c r="AB25" s="10">
         <f>AB24+Eingabedaten!M25</f>
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="AC25" s="10">
         <f>AC24+Eingabedaten!N25</f>
-        <v>1</v>
+        <v>12.5</v>
       </c>
       <c r="AD25" s="10">
         <f>AD24+Eingabedaten!O25</f>
-        <v>8.25</v>
+        <v>14.25</v>
       </c>
       <c r="AE25" s="10">
         <f t="shared" si="8"/>
-        <v>90.25</v>
+        <v>173.75</v>
       </c>
       <c r="AG25" s="10">
         <f t="shared" si="9"/>
-        <v>219</v>
+        <v>411.5</v>
       </c>
     </row>
     <row r="26" spans="2:33">
@@ -10110,23 +10276,23 @@
       </c>
       <c r="T26" s="10">
         <f>Eingabedaten!F26+'Eingabedaten (berechnet)'!T25</f>
-        <v>18.5</v>
+        <v>27.5</v>
       </c>
       <c r="U26" s="10">
         <f>Eingabedaten!G26+'Eingabedaten (berechnet)'!U25</f>
-        <v>43</v>
+        <v>80</v>
       </c>
       <c r="V26" s="10">
         <f>Eingabedaten!H26+'Eingabedaten (berechnet)'!V25</f>
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="W26" s="10">
         <f>Eingabedaten!I26+'Eingabedaten (berechnet)'!W25</f>
-        <v>22.75</v>
+        <v>52.75</v>
       </c>
       <c r="X26" s="10">
         <f t="shared" si="7"/>
-        <v>128.75</v>
+        <v>237.75</v>
       </c>
       <c r="Z26" s="10">
         <f>Z25+Eingabedaten!K26</f>
@@ -10134,27 +10300,27 @@
       </c>
       <c r="AA26" s="10">
         <f>AA25+Eingabedaten!L26</f>
-        <v>17.5</v>
+        <v>63.5</v>
       </c>
       <c r="AB26" s="10">
         <f>AB25+Eingabedaten!M26</f>
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="AC26" s="10">
         <f>AC25+Eingabedaten!N26</f>
-        <v>1</v>
+        <v>12.5</v>
       </c>
       <c r="AD26" s="10">
         <f>AD25+Eingabedaten!O26</f>
-        <v>8.25</v>
+        <v>14.25</v>
       </c>
       <c r="AE26" s="10">
         <f t="shared" si="8"/>
-        <v>90.25</v>
+        <v>173.75</v>
       </c>
       <c r="AG26" s="10">
         <f t="shared" si="9"/>
-        <v>219</v>
+        <v>411.5</v>
       </c>
     </row>
     <row r="27" spans="2:33">
@@ -10220,23 +10386,23 @@
       </c>
       <c r="T27" s="10">
         <f>Eingabedaten!F27+'Eingabedaten (berechnet)'!T26</f>
-        <v>18.5</v>
+        <v>27.5</v>
       </c>
       <c r="U27" s="10">
         <f>Eingabedaten!G27+'Eingabedaten (berechnet)'!U26</f>
-        <v>43</v>
+        <v>80</v>
       </c>
       <c r="V27" s="10">
         <f>Eingabedaten!H27+'Eingabedaten (berechnet)'!V26</f>
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="W27" s="10">
         <f>Eingabedaten!I27+'Eingabedaten (berechnet)'!W26</f>
-        <v>22.75</v>
+        <v>52.75</v>
       </c>
       <c r="X27" s="10">
         <f t="shared" si="7"/>
-        <v>128.75</v>
+        <v>237.75</v>
       </c>
       <c r="Z27" s="10">
         <f>Z26+Eingabedaten!K27</f>
@@ -10244,27 +10410,27 @@
       </c>
       <c r="AA27" s="10">
         <f>AA26+Eingabedaten!L27</f>
-        <v>17.5</v>
+        <v>63.5</v>
       </c>
       <c r="AB27" s="10">
         <f>AB26+Eingabedaten!M27</f>
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="AC27" s="10">
         <f>AC26+Eingabedaten!N27</f>
-        <v>1</v>
+        <v>12.5</v>
       </c>
       <c r="AD27" s="10">
         <f>AD26+Eingabedaten!O27</f>
-        <v>8.25</v>
+        <v>14.25</v>
       </c>
       <c r="AE27" s="10">
         <f t="shared" si="8"/>
-        <v>90.25</v>
+        <v>173.75</v>
       </c>
       <c r="AG27" s="10">
         <f t="shared" si="9"/>
-        <v>219</v>
+        <v>411.5</v>
       </c>
     </row>
     <row r="28" spans="2:33">
@@ -10330,23 +10496,23 @@
       </c>
       <c r="T28" s="10">
         <f>Eingabedaten!F28+'Eingabedaten (berechnet)'!T27</f>
-        <v>18.5</v>
+        <v>27.5</v>
       </c>
       <c r="U28" s="10">
         <f>Eingabedaten!G28+'Eingabedaten (berechnet)'!U27</f>
-        <v>43</v>
+        <v>80</v>
       </c>
       <c r="V28" s="10">
         <f>Eingabedaten!H28+'Eingabedaten (berechnet)'!V27</f>
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="W28" s="10">
         <f>Eingabedaten!I28+'Eingabedaten (berechnet)'!W27</f>
-        <v>22.75</v>
+        <v>52.75</v>
       </c>
       <c r="X28" s="10">
         <f t="shared" si="7"/>
-        <v>128.75</v>
+        <v>237.75</v>
       </c>
       <c r="Z28" s="10">
         <f>Z27+Eingabedaten!K28</f>
@@ -10354,27 +10520,27 @@
       </c>
       <c r="AA28" s="10">
         <f>AA27+Eingabedaten!L28</f>
-        <v>17.5</v>
+        <v>63.5</v>
       </c>
       <c r="AB28" s="10">
         <f>AB27+Eingabedaten!M28</f>
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="AC28" s="10">
         <f>AC27+Eingabedaten!N28</f>
-        <v>1</v>
+        <v>12.5</v>
       </c>
       <c r="AD28" s="10">
         <f>AD27+Eingabedaten!O28</f>
-        <v>8.25</v>
+        <v>14.25</v>
       </c>
       <c r="AE28" s="10">
         <f t="shared" si="8"/>
-        <v>90.25</v>
+        <v>173.75</v>
       </c>
       <c r="AG28" s="10">
         <f t="shared" si="9"/>
-        <v>219</v>
+        <v>411.5</v>
       </c>
     </row>
     <row r="29" spans="2:33">
@@ -10440,23 +10606,23 @@
       </c>
       <c r="T29" s="10">
         <f>Eingabedaten!F29+'Eingabedaten (berechnet)'!T28</f>
-        <v>18.5</v>
+        <v>27.5</v>
       </c>
       <c r="U29" s="10">
         <f>Eingabedaten!G29+'Eingabedaten (berechnet)'!U28</f>
-        <v>43</v>
+        <v>80</v>
       </c>
       <c r="V29" s="10">
         <f>Eingabedaten!H29+'Eingabedaten (berechnet)'!V28</f>
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="W29" s="10">
         <f>Eingabedaten!I29+'Eingabedaten (berechnet)'!W28</f>
-        <v>22.75</v>
+        <v>52.75</v>
       </c>
       <c r="X29" s="10">
         <f t="shared" si="7"/>
-        <v>128.75</v>
+        <v>237.75</v>
       </c>
       <c r="Z29" s="10">
         <f>Z28+Eingabedaten!K29</f>
@@ -10464,27 +10630,27 @@
       </c>
       <c r="AA29" s="10">
         <f>AA28+Eingabedaten!L29</f>
-        <v>17.5</v>
+        <v>63.5</v>
       </c>
       <c r="AB29" s="10">
         <f>AB28+Eingabedaten!M29</f>
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="AC29" s="10">
         <f>AC28+Eingabedaten!N29</f>
-        <v>1</v>
+        <v>12.5</v>
       </c>
       <c r="AD29" s="10">
         <f>AD28+Eingabedaten!O29</f>
-        <v>8.25</v>
+        <v>14.25</v>
       </c>
       <c r="AE29" s="10">
         <f t="shared" si="8"/>
-        <v>90.25</v>
+        <v>173.75</v>
       </c>
       <c r="AG29" s="10">
         <f t="shared" si="9"/>
-        <v>219</v>
+        <v>411.5</v>
       </c>
     </row>
     <row r="30" spans="2:33">
@@ -10550,23 +10716,23 @@
       </c>
       <c r="T30" s="10">
         <f>Eingabedaten!F30+'Eingabedaten (berechnet)'!T29</f>
-        <v>18.5</v>
+        <v>27.5</v>
       </c>
       <c r="U30" s="10">
         <f>Eingabedaten!G30+'Eingabedaten (berechnet)'!U29</f>
-        <v>43</v>
+        <v>80</v>
       </c>
       <c r="V30" s="10">
         <f>Eingabedaten!H30+'Eingabedaten (berechnet)'!V29</f>
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="W30" s="10">
         <f>Eingabedaten!I30+'Eingabedaten (berechnet)'!W29</f>
-        <v>22.75</v>
+        <v>52.75</v>
       </c>
       <c r="X30" s="10">
         <f t="shared" si="7"/>
-        <v>128.75</v>
+        <v>237.75</v>
       </c>
       <c r="Z30" s="10">
         <f>Z29+Eingabedaten!K30</f>
@@ -10574,27 +10740,27 @@
       </c>
       <c r="AA30" s="10">
         <f>AA29+Eingabedaten!L30</f>
-        <v>17.5</v>
+        <v>63.5</v>
       </c>
       <c r="AB30" s="10">
         <f>AB29+Eingabedaten!M30</f>
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="AC30" s="10">
         <f>AC29+Eingabedaten!N30</f>
-        <v>1</v>
+        <v>12.5</v>
       </c>
       <c r="AD30" s="10">
         <f>AD29+Eingabedaten!O30</f>
-        <v>8.25</v>
+        <v>14.25</v>
       </c>
       <c r="AE30" s="10">
         <f t="shared" si="8"/>
-        <v>90.25</v>
+        <v>173.75</v>
       </c>
       <c r="AG30" s="10">
         <f t="shared" si="9"/>
-        <v>219</v>
+        <v>411.5</v>
       </c>
     </row>
     <row r="31" spans="2:33">
@@ -10660,23 +10826,23 @@
       </c>
       <c r="T31" s="10">
         <f>Eingabedaten!F31+'Eingabedaten (berechnet)'!T30</f>
-        <v>18.5</v>
+        <v>27.5</v>
       </c>
       <c r="U31" s="10">
         <f>Eingabedaten!G31+'Eingabedaten (berechnet)'!U30</f>
-        <v>43</v>
+        <v>80</v>
       </c>
       <c r="V31" s="10">
         <f>Eingabedaten!H31+'Eingabedaten (berechnet)'!V30</f>
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="W31" s="10">
         <f>Eingabedaten!I31+'Eingabedaten (berechnet)'!W30</f>
-        <v>22.75</v>
+        <v>52.75</v>
       </c>
       <c r="X31" s="10">
         <f t="shared" si="7"/>
-        <v>128.75</v>
+        <v>237.75</v>
       </c>
       <c r="Z31" s="10">
         <f>Z30+Eingabedaten!K31</f>
@@ -10684,27 +10850,27 @@
       </c>
       <c r="AA31" s="10">
         <f>AA30+Eingabedaten!L31</f>
-        <v>17.5</v>
+        <v>63.5</v>
       </c>
       <c r="AB31" s="10">
         <f>AB30+Eingabedaten!M31</f>
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="AC31" s="10">
         <f>AC30+Eingabedaten!N31</f>
-        <v>1</v>
+        <v>12.5</v>
       </c>
       <c r="AD31" s="10">
         <f>AD30+Eingabedaten!O31</f>
-        <v>8.25</v>
+        <v>14.25</v>
       </c>
       <c r="AE31" s="10">
         <f t="shared" si="8"/>
-        <v>90.25</v>
+        <v>173.75</v>
       </c>
       <c r="AG31" s="10">
         <f t="shared" si="9"/>
-        <v>219</v>
+        <v>411.5</v>
       </c>
     </row>
     <row r="32" spans="2:33">
@@ -10770,23 +10936,23 @@
       </c>
       <c r="T32" s="10">
         <f>Eingabedaten!F32+'Eingabedaten (berechnet)'!T31</f>
-        <v>18.5</v>
+        <v>27.5</v>
       </c>
       <c r="U32" s="10">
         <f>Eingabedaten!G32+'Eingabedaten (berechnet)'!U31</f>
-        <v>43</v>
+        <v>80</v>
       </c>
       <c r="V32" s="10">
         <f>Eingabedaten!H32+'Eingabedaten (berechnet)'!V31</f>
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="W32" s="10">
         <f>Eingabedaten!I32+'Eingabedaten (berechnet)'!W31</f>
-        <v>22.75</v>
+        <v>52.75</v>
       </c>
       <c r="X32" s="10">
         <f t="shared" si="7"/>
-        <v>128.75</v>
+        <v>237.75</v>
       </c>
       <c r="Z32" s="10">
         <f>Z31+Eingabedaten!K32</f>
@@ -10794,27 +10960,27 @@
       </c>
       <c r="AA32" s="10">
         <f>AA31+Eingabedaten!L32</f>
-        <v>17.5</v>
+        <v>63.5</v>
       </c>
       <c r="AB32" s="10">
         <f>AB31+Eingabedaten!M32</f>
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="AC32" s="10">
         <f>AC31+Eingabedaten!N32</f>
-        <v>1</v>
+        <v>12.5</v>
       </c>
       <c r="AD32" s="10">
         <f>AD31+Eingabedaten!O32</f>
-        <v>8.25</v>
+        <v>14.25</v>
       </c>
       <c r="AE32" s="10">
         <f t="shared" si="8"/>
-        <v>90.25</v>
+        <v>173.75</v>
       </c>
       <c r="AG32" s="10">
         <f t="shared" si="9"/>
-        <v>219</v>
+        <v>411.5</v>
       </c>
     </row>
     <row r="33" spans="2:33">
@@ -10880,23 +11046,23 @@
       </c>
       <c r="T33" s="10">
         <f>Eingabedaten!F33+'Eingabedaten (berechnet)'!T32</f>
-        <v>18.5</v>
+        <v>27.5</v>
       </c>
       <c r="U33" s="10">
         <f>Eingabedaten!G33+'Eingabedaten (berechnet)'!U32</f>
-        <v>43</v>
+        <v>80</v>
       </c>
       <c r="V33" s="10">
         <f>Eingabedaten!H33+'Eingabedaten (berechnet)'!V32</f>
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="W33" s="10">
         <f>Eingabedaten!I33+'Eingabedaten (berechnet)'!W32</f>
-        <v>22.75</v>
+        <v>52.75</v>
       </c>
       <c r="X33" s="10">
         <f t="shared" si="7"/>
-        <v>128.75</v>
+        <v>237.75</v>
       </c>
       <c r="Z33" s="10">
         <f>Z32+Eingabedaten!K33</f>
@@ -10904,27 +11070,27 @@
       </c>
       <c r="AA33" s="10">
         <f>AA32+Eingabedaten!L33</f>
-        <v>17.5</v>
+        <v>63.5</v>
       </c>
       <c r="AB33" s="10">
         <f>AB32+Eingabedaten!M33</f>
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="AC33" s="10">
         <f>AC32+Eingabedaten!N33</f>
-        <v>1</v>
+        <v>12.5</v>
       </c>
       <c r="AD33" s="10">
         <f>AD32+Eingabedaten!O33</f>
-        <v>8.25</v>
+        <v>14.25</v>
       </c>
       <c r="AE33" s="10">
         <f t="shared" si="8"/>
-        <v>90.25</v>
+        <v>173.75</v>
       </c>
       <c r="AG33" s="10">
         <f t="shared" si="9"/>
-        <v>219</v>
+        <v>411.5</v>
       </c>
     </row>
     <row r="35" spans="2:33">
@@ -10934,29 +11100,29 @@
       </c>
       <c r="F35" s="6">
         <f t="shared" si="12"/>
-        <v>36</v>
+        <v>91</v>
       </c>
       <c r="G35" s="6">
         <f t="shared" si="12"/>
-        <v>62</v>
+        <v>119</v>
       </c>
       <c r="H35" s="6">
         <f t="shared" si="12"/>
-        <v>2</v>
+        <v>46.5</v>
       </c>
       <c r="I35" s="6">
         <f t="shared" si="12"/>
-        <v>31</v>
+        <v>67</v>
       </c>
       <c r="J35" s="6">
         <f t="shared" si="12"/>
-        <v>219</v>
+        <v>411.5</v>
       </c>
     </row>
     <row r="36" spans="2:33">
       <c r="E36" s="6">
         <f>SUM(E35:I35)</f>
-        <v>219</v>
+        <v>411.5</v>
       </c>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>

</xml_diff>

<commit_message>
Set new revision E, as 'running' version.
</commit_message>
<xml_diff>
--- a/ProjektManagement/NuvoControl_0011_StundenNachweis_Grafisch.xlsx
+++ b/ProjektManagement/NuvoControl_0011_StundenNachweis_Grafisch.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="36">
   <si>
     <t>Die Werte in diesem Sheet wurden mit dem Dokument "NuvoControl_0010_StundenNachweis" erfasst.</t>
   </si>
@@ -152,6 +152,12 @@
   </si>
   <si>
     <t>d / 29-Mai-2009</t>
+  </si>
+  <si>
+    <t>e / ??</t>
+  </si>
+  <si>
+    <t>in work</t>
   </si>
 </sst>
 </file>
@@ -709,11 +715,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="127190144"/>
-        <c:axId val="127191680"/>
+        <c:axId val="128304256"/>
+        <c:axId val="128305792"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="127190144"/>
+        <c:axId val="128304256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -731,13 +737,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="127191680"/>
+        <c:crossAx val="128305792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="127191680"/>
+        <c:axId val="128305792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -769,7 +775,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="127190144"/>
+        <c:crossAx val="128304256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1211,11 +1217,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="127229952"/>
-        <c:axId val="127231488"/>
+        <c:axId val="128356352"/>
+        <c:axId val="128357888"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="127229952"/>
+        <c:axId val="128356352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1233,13 +1239,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="127231488"/>
+        <c:crossAx val="128357888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="127231488"/>
+        <c:axId val="128357888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1271,7 +1277,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="127229952"/>
+        <c:crossAx val="128356352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1713,11 +1719,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="127260928"/>
-        <c:axId val="127266816"/>
+        <c:axId val="128379136"/>
+        <c:axId val="128651264"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="127260928"/>
+        <c:axId val="128379136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1735,13 +1741,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="127266816"/>
+        <c:crossAx val="128651264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="127266816"/>
+        <c:axId val="128651264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1773,7 +1779,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="127260928"/>
+        <c:crossAx val="128379136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1822,7 +1828,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -2500,11 +2505,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="128748928"/>
-        <c:axId val="128763008"/>
+        <c:axId val="128822656"/>
+        <c:axId val="128713856"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="128748928"/>
+        <c:axId val="128822656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2522,13 +2527,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="128763008"/>
+        <c:crossAx val="128713856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="128763008"/>
+        <c:axId val="128713856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2558,7 +2563,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -2573,14 +2577,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="128748928"/>
+        <c:crossAx val="128822656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:txPr>
         <a:bodyPr/>
         <a:lstStyle/>
@@ -2622,7 +2625,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -3264,11 +3266,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="128692608"/>
-        <c:axId val="128694144"/>
+        <c:axId val="128758144"/>
+        <c:axId val="128759680"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="128692608"/>
+        <c:axId val="128758144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3286,13 +3288,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="128694144"/>
+        <c:crossAx val="128759680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="128694144"/>
+        <c:axId val="128759680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3322,7 +3324,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -3337,14 +3338,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="128692608"/>
+        <c:crossAx val="128758144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:txPr>
         <a:bodyPr/>
         <a:lstStyle/>
@@ -3391,7 +3391,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -4363,11 +4362,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="128947712"/>
-        <c:axId val="128949248"/>
+        <c:axId val="128886272"/>
+        <c:axId val="128887808"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="128947712"/>
+        <c:axId val="128886272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4385,13 +4384,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="128949248"/>
+        <c:crossAx val="128887808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="128949248"/>
+        <c:axId val="128887808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4421,7 +4420,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -4436,14 +4434,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="128947712"/>
+        <c:crossAx val="128886272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:txPr>
         <a:bodyPr/>
         <a:lstStyle/>
@@ -4490,7 +4487,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -5462,11 +5458,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="128984960"/>
-        <c:axId val="128986496"/>
+        <c:axId val="129050496"/>
+        <c:axId val="129052032"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="128984960"/>
+        <c:axId val="129050496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5484,13 +5480,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="128986496"/>
+        <c:crossAx val="129052032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="128986496"/>
+        <c:axId val="129052032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5520,7 +5516,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -5535,14 +5530,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="128984960"/>
+        <c:crossAx val="129050496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:txPr>
         <a:bodyPr/>
         <a:lstStyle/>
@@ -6072,9 +6066,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B3:E7"/>
+  <dimension ref="B3:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
@@ -6119,6 +6115,14 @@
       </c>
       <c r="E7" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5">
+      <c r="C8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Abgabe: RevD - 29-June-2009
</commit_message>
<xml_diff>
--- a/ProjektManagement/NuvoControl_0011_StundenNachweis_Grafisch.xlsx
+++ b/ProjektManagement/NuvoControl_0011_StundenNachweis_Grafisch.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="34">
   <si>
     <t>Die Werte in diesem Sheet wurden mit dem Dokument "NuvoControl_0010_StundenNachweis" erfasst.</t>
   </si>
@@ -151,13 +151,7 @@
     <t>Version an Hans Rudin Zwecks Zwischenbesprechung</t>
   </si>
   <si>
-    <t>d / 29-Mai-2009</t>
-  </si>
-  <si>
-    <t>e / ??</t>
-  </si>
-  <si>
-    <t>in work</t>
+    <t>d / 29-June-2009</t>
   </si>
 </sst>
 </file>
@@ -715,11 +709,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="128304256"/>
-        <c:axId val="128305792"/>
+        <c:axId val="129292544"/>
+        <c:axId val="126730240"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="128304256"/>
+        <c:axId val="129292544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -737,13 +731,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="128305792"/>
+        <c:crossAx val="126730240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="128305792"/>
+        <c:axId val="126730240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -775,7 +769,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="128304256"/>
+        <c:crossAx val="129292544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1217,11 +1211,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="128356352"/>
-        <c:axId val="128357888"/>
+        <c:axId val="127271680"/>
+        <c:axId val="127273216"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="128356352"/>
+        <c:axId val="127271680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1239,13 +1233,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="128357888"/>
+        <c:crossAx val="127273216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="128357888"/>
+        <c:axId val="127273216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1277,7 +1271,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="128356352"/>
+        <c:crossAx val="127271680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1719,11 +1713,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="128379136"/>
-        <c:axId val="128651264"/>
+        <c:axId val="127286272"/>
+        <c:axId val="127296256"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="128379136"/>
+        <c:axId val="127286272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1741,13 +1735,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="128651264"/>
+        <c:crossAx val="127296256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="128651264"/>
+        <c:axId val="127296256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1779,7 +1773,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="128379136"/>
+        <c:crossAx val="127286272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2505,11 +2499,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="128822656"/>
-        <c:axId val="128713856"/>
+        <c:axId val="127324544"/>
+        <c:axId val="127326080"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="128822656"/>
+        <c:axId val="127324544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2527,13 +2521,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="128713856"/>
+        <c:crossAx val="127326080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="128713856"/>
+        <c:axId val="127326080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2577,7 +2571,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="128822656"/>
+        <c:crossAx val="127324544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3266,11 +3260,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="128758144"/>
-        <c:axId val="128759680"/>
+        <c:axId val="127800448"/>
+        <c:axId val="127801984"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="128758144"/>
+        <c:axId val="127800448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3288,13 +3282,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="128759680"/>
+        <c:crossAx val="127801984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="128759680"/>
+        <c:axId val="127801984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3338,7 +3332,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="128758144"/>
+        <c:crossAx val="127800448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4362,11 +4356,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="128886272"/>
-        <c:axId val="128887808"/>
+        <c:axId val="127834368"/>
+        <c:axId val="127844352"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="128886272"/>
+        <c:axId val="127834368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4384,13 +4378,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="128887808"/>
+        <c:crossAx val="127844352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="128887808"/>
+        <c:axId val="127844352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4434,7 +4428,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="128886272"/>
+        <c:crossAx val="127834368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5458,11 +5452,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="129050496"/>
-        <c:axId val="129052032"/>
+        <c:axId val="127883904"/>
+        <c:axId val="127893888"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="129050496"/>
+        <c:axId val="127883904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5480,13 +5474,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="129052032"/>
+        <c:crossAx val="127893888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="129052032"/>
+        <c:axId val="127893888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5530,7 +5524,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="129050496"/>
+        <c:crossAx val="127883904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6066,10 +6060,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B3:E8"/>
+  <dimension ref="B3:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -6115,14 +6109,6 @@
       </c>
       <c r="E7" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5">
-      <c r="C8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E8" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Grafische Erfassung der Aufwaende.
</commit_message>
<xml_diff>
--- a/ProjektManagement/NuvoControl_0011_StundenNachweis_Grafisch.xlsx
+++ b/ProjektManagement/NuvoControl_0011_StundenNachweis_Grafisch.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="37">
   <si>
     <t>Die Werte in diesem Sheet wurden mit dem Dokument "NuvoControl_0010_StundenNachweis" erfasst.</t>
   </si>
@@ -154,10 +154,13 @@
     <t>d / 29-June-2009</t>
   </si>
   <si>
-    <t>e / ??-??-2009</t>
+    <t>in work</t>
   </si>
   <si>
-    <t>in work</t>
+    <t>e / 09-Aug-2009</t>
+  </si>
+  <si>
+    <t>f / xx-xx-2009</t>
   </si>
 </sst>
 </file>
@@ -295,7 +298,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -304,7 +307,7 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+  <c:lang val="de-CH"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -684,42 +687,42 @@
                   <c:v>237.75</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>237.75</c:v>
+                  <c:v>241.25</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>237.75</c:v>
+                  <c:v>241.25</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>237.75</c:v>
+                  <c:v>241.25</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>237.75</c:v>
+                  <c:v>241.25</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>237.75</c:v>
+                  <c:v>246.25</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>237.75</c:v>
+                  <c:v>261.75</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>237.75</c:v>
+                  <c:v>261.75</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>237.75</c:v>
+                  <c:v>261.75</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>237.75</c:v>
+                  <c:v>261.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="122818944"/>
-        <c:axId val="122820480"/>
+        <c:axId val="73112960"/>
+        <c:axId val="73122944"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="122818944"/>
+        <c:axId val="73112960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -734,16 +737,16 @@
             <a:pPr>
               <a:defRPr lang="de-CH"/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="122820480"/>
+        <c:crossAx val="73122944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="122820480"/>
+        <c:axId val="73122944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -758,7 +761,7 @@
               <a:pPr>
                 <a:defRPr lang="de-CH"/>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -772,10 +775,10 @@
             <a:pPr>
               <a:defRPr lang="de-CH"/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="122818944"/>
+        <c:crossAx val="73112960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -790,7 +793,7 @@
           <a:pPr>
             <a:defRPr lang="de-CH"/>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -806,7 +809,7 @@
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+  <c:lang val="de-CH"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1186,42 +1189,42 @@
                   <c:v>173.75</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>173.75</c:v>
+                  <c:v>177.25</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>173.75</c:v>
+                  <c:v>207.25</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>173.75</c:v>
+                  <c:v>236.25</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>173.75</c:v>
+                  <c:v>269.25</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>173.75</c:v>
+                  <c:v>283.75</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>173.75</c:v>
+                  <c:v>293.25</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>173.75</c:v>
+                  <c:v>293.25</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>173.75</c:v>
+                  <c:v>293.25</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>173.75</c:v>
+                  <c:v>293.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="128275584"/>
-        <c:axId val="128277120"/>
+        <c:axId val="73423104"/>
+        <c:axId val="73461760"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="128275584"/>
+        <c:axId val="73423104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1236,16 +1239,16 @@
             <a:pPr>
               <a:defRPr lang="de-CH"/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="128277120"/>
+        <c:crossAx val="73461760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="128277120"/>
+        <c:axId val="73461760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1260,7 +1263,7 @@
               <a:pPr>
                 <a:defRPr lang="de-CH"/>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1274,10 +1277,10 @@
             <a:pPr>
               <a:defRPr lang="de-CH"/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="128275584"/>
+        <c:crossAx val="73423104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1292,7 +1295,7 @@
           <a:pPr>
             <a:defRPr lang="de-CH"/>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1308,7 +1311,7 @@
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+  <c:lang val="de-CH"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1688,42 +1691,42 @@
                   <c:v>411.5</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>411.5</c:v>
+                  <c:v>418.5</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>411.5</c:v>
+                  <c:v>448.5</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>411.5</c:v>
+                  <c:v>477.5</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>411.5</c:v>
+                  <c:v>510.5</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>411.5</c:v>
+                  <c:v>530</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>411.5</c:v>
+                  <c:v>555</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>411.5</c:v>
+                  <c:v>555</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>411.5</c:v>
+                  <c:v>555</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>411.5</c:v>
+                  <c:v>555</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="129291392"/>
-        <c:axId val="129292928"/>
+        <c:axId val="74793728"/>
+        <c:axId val="74795264"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="129291392"/>
+        <c:axId val="74793728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1738,16 +1741,16 @@
             <a:pPr>
               <a:defRPr lang="de-CH"/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="129292928"/>
+        <c:crossAx val="74795264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="129292928"/>
+        <c:axId val="74795264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1762,7 +1765,7 @@
               <a:pPr>
                 <a:defRPr lang="de-CH"/>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1776,10 +1779,10 @@
             <a:pPr>
               <a:defRPr lang="de-CH"/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="129291392"/>
+        <c:crossAx val="74793728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1794,7 +1797,7 @@
           <a:pPr>
             <a:defRPr lang="de-CH"/>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1810,7 +1813,7 @@
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+  <c:lang val="de-CH"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1828,6 +1831,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -1953,6 +1957,12 @@
                 <c:pt idx="18">
                   <c:v>6.5</c:v>
                 </c:pt>
+                <c:pt idx="19">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2089,6 +2099,9 @@
                 <c:pt idx="18">
                   <c:v>10</c:v>
                 </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2352,6 +2365,9 @@
                 <c:pt idx="10">
                   <c:v>0.5</c:v>
                 </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2500,16 +2516,22 @@
                 <c:pt idx="18">
                   <c:v>1</c:v>
                 </c:pt>
+                <c:pt idx="23">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>15</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="136820608"/>
-        <c:axId val="136822144"/>
+        <c:axId val="74913664"/>
+        <c:axId val="74915200"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="136820608"/>
+        <c:axId val="74913664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2524,16 +2546,16 @@
             <a:pPr>
               <a:defRPr lang="de-CH"/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="136822144"/>
+        <c:crossAx val="74915200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="136822144"/>
+        <c:axId val="74915200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2563,6 +2585,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -2574,16 +2597,17 @@
             <a:pPr>
               <a:defRPr lang="de-CH"/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="136820608"/>
+        <c:crossAx val="74913664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:txPr>
         <a:bodyPr/>
         <a:lstStyle/>
@@ -2591,7 +2615,7 @@
           <a:pPr>
             <a:defRPr lang="de-CH"/>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2607,7 +2631,7 @@
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+  <c:lang val="de-CH"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -2625,6 +2649,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -2868,6 +2893,18 @@
                 <c:pt idx="17">
                   <c:v>4</c:v>
                 </c:pt>
+                <c:pt idx="21">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>7</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3001,6 +3038,15 @@
                 <c:pt idx="18">
                   <c:v>7</c:v>
                 </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3261,16 +3307,22 @@
                 <c:pt idx="17">
                   <c:v>2</c:v>
                 </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="49805184"/>
-        <c:axId val="49806720"/>
+        <c:axId val="74951296"/>
+        <c:axId val="74961280"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="49805184"/>
+        <c:axId val="74951296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3285,16 +3337,16 @@
             <a:pPr>
               <a:defRPr lang="de-CH"/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="49806720"/>
+        <c:crossAx val="74961280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="49806720"/>
+        <c:axId val="74961280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3324,6 +3376,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -3335,16 +3388,17 @@
             <a:pPr>
               <a:defRPr lang="de-CH"/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="49805184"/>
+        <c:crossAx val="74951296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:txPr>
         <a:bodyPr/>
         <a:lstStyle/>
@@ -3352,7 +3406,7 @@
           <a:pPr>
             <a:defRPr lang="de-CH"/>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3368,7 +3422,7 @@
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+  <c:lang val="de-CH"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -3391,6 +3445,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -3559,31 +3614,31 @@
                   <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>34</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>34</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>34</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>34</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>34</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>34</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>34</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>34</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>34</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3767,16 +3822,16 @@
                   <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>80</c:v>
+                  <c:v>80.5</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>80</c:v>
+                  <c:v>80.5</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>80</c:v>
+                  <c:v>80.5</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>80</c:v>
+                  <c:v>80.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4138,31 +4193,31 @@
                   <c:v>43.5</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>43.5</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>43.5</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>43.5</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>43.5</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>43.5</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>43.5</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>43.5</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>43.5</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>43.5</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4343,30 +4398,30 @@
                   <c:v>52.75</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>52.75</c:v>
+                  <c:v>55.75</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>52.75</c:v>
+                  <c:v>70.75</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>52.75</c:v>
+                  <c:v>70.75</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>52.75</c:v>
+                  <c:v>70.75</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>52.75</c:v>
+                  <c:v>70.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="122801152"/>
-        <c:axId val="122852096"/>
+        <c:axId val="75030528"/>
+        <c:axId val="75032064"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="122801152"/>
+        <c:axId val="75030528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4381,16 +4436,16 @@
             <a:pPr>
               <a:defRPr lang="de-CH"/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="122852096"/>
+        <c:crossAx val="75032064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="122852096"/>
+        <c:axId val="75032064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4420,6 +4475,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -4431,16 +4487,17 @@
             <a:pPr>
               <a:defRPr lang="de-CH"/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="122801152"/>
+        <c:crossAx val="75030528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:txPr>
         <a:bodyPr/>
         <a:lstStyle/>
@@ -4448,7 +4505,7 @@
           <a:pPr>
             <a:defRPr lang="de-CH"/>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4464,7 +4521,7 @@
 
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+  <c:lang val="de-CH"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -4487,6 +4544,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -4854,25 +4912,25 @@
                   <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>39</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>39</c:v>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>39</c:v>
+                  <c:v>109</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>39</c:v>
+                  <c:v>116</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>39</c:v>
+                  <c:v>116</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>39</c:v>
+                  <c:v>116</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>39</c:v>
+                  <c:v>116</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5041,31 +5099,31 @@
                   <c:v>63.5</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>63.5</c:v>
+                  <c:v>67</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>63.5</c:v>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>63.5</c:v>
+                  <c:v>101</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>63.5</c:v>
+                  <c:v>101</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>63.5</c:v>
+                  <c:v>101</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>63.5</c:v>
+                  <c:v>101</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>63.5</c:v>
+                  <c:v>101</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>63.5</c:v>
+                  <c:v>101</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>63.5</c:v>
+                  <c:v>101</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5439,30 +5497,30 @@
                   <c:v>14.25</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>14.25</c:v>
+                  <c:v>16.75</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>14.25</c:v>
+                  <c:v>19.25</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>14.25</c:v>
+                  <c:v>19.25</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>14.25</c:v>
+                  <c:v>19.25</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>14.25</c:v>
+                  <c:v>19.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="125042048"/>
-        <c:axId val="126731392"/>
+        <c:axId val="75198848"/>
+        <c:axId val="75200384"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="125042048"/>
+        <c:axId val="75198848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5477,16 +5535,16 @@
             <a:pPr>
               <a:defRPr lang="de-CH"/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="126731392"/>
+        <c:crossAx val="75200384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="126731392"/>
+        <c:axId val="75200384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5516,6 +5574,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -5527,16 +5586,17 @@
             <a:pPr>
               <a:defRPr lang="de-CH"/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="125042048"/>
+        <c:crossAx val="75198848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:txPr>
         <a:bodyPr/>
         <a:lstStyle/>
@@ -5544,7 +5604,7 @@
           <a:pPr>
             <a:defRPr lang="de-CH"/>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -5779,9 +5839,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -5819,7 +5879,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -5889,7 +5949,7 @@
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -6066,13 +6126,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B3:E8"/>
+  <dimension ref="B3:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3.7109375" customWidth="1"/>
     <col min="2" max="2" width="6.85546875" customWidth="1"/>
@@ -6119,10 +6179,18 @@
     </row>
     <row r="8" spans="2:5">
       <c r="C8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5">
+      <c r="C9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" t="s">
         <v>34</v>
-      </c>
-      <c r="E8" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -6142,11 +6210,11 @@
   <dimension ref="B2:O39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I25" sqref="I25"/>
+      <pane ySplit="5" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3.140625" customWidth="1"/>
     <col min="2" max="2" width="14.140625" customWidth="1"/>
@@ -6816,13 +6884,22 @@
         <f t="shared" si="1"/>
         <v>39999</v>
       </c>
-      <c r="E25" s="9"/>
+      <c r="E25" s="9">
+        <f>0.5</f>
+        <v>0.5</v>
+      </c>
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
-      <c r="H25" s="9"/>
+      <c r="H25" s="9">
+        <f>3</f>
+        <v>3</v>
+      </c>
       <c r="I25" s="9"/>
       <c r="K25" s="9"/>
-      <c r="L25" s="9"/>
+      <c r="L25" s="9">
+        <f>3.5</f>
+        <v>3.5</v>
+      </c>
       <c r="M25" s="9"/>
       <c r="N25" s="9"/>
       <c r="O25" s="9"/>
@@ -6842,7 +6919,10 @@
       <c r="H26" s="9"/>
       <c r="I26" s="9"/>
       <c r="K26" s="9"/>
-      <c r="L26" s="9"/>
+      <c r="L26" s="9">
+        <f>10+10+10</f>
+        <v>30</v>
+      </c>
       <c r="M26" s="9"/>
       <c r="N26" s="9"/>
       <c r="O26" s="9"/>
@@ -6862,8 +6942,14 @@
       <c r="H27" s="9"/>
       <c r="I27" s="9"/>
       <c r="K27" s="9"/>
-      <c r="L27" s="9"/>
-      <c r="M27" s="9"/>
+      <c r="L27" s="9">
+        <f>4</f>
+        <v>4</v>
+      </c>
+      <c r="M27" s="9">
+        <f>4+4+6+8+3</f>
+        <v>25</v>
+      </c>
       <c r="N27" s="9"/>
       <c r="O27" s="9"/>
     </row>
@@ -6883,7 +6969,10 @@
       <c r="I28" s="9"/>
       <c r="K28" s="9"/>
       <c r="L28" s="9"/>
-      <c r="M28" s="9"/>
+      <c r="M28" s="9">
+        <f>7+5+5+6+10</f>
+        <v>33</v>
+      </c>
       <c r="N28" s="9"/>
       <c r="O28" s="9"/>
     </row>
@@ -6899,13 +6988,25 @@
       <c r="E29" s="9"/>
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
-      <c r="H29" s="9"/>
-      <c r="I29" s="9"/>
+      <c r="H29" s="9">
+        <f>2</f>
+        <v>2</v>
+      </c>
+      <c r="I29" s="9">
+        <f>2.5+0.5</f>
+        <v>3</v>
+      </c>
       <c r="K29" s="9"/>
       <c r="L29" s="9"/>
-      <c r="M29" s="9"/>
+      <c r="M29" s="9">
+        <f>4+4+4</f>
+        <v>12</v>
+      </c>
       <c r="N29" s="9"/>
-      <c r="O29" s="9"/>
+      <c r="O29" s="9">
+        <f>2.5</f>
+        <v>2.5</v>
+      </c>
     </row>
     <row r="30" spans="2:15">
       <c r="B30" s="2">
@@ -6918,14 +7019,26 @@
       </c>
       <c r="E30" s="9"/>
       <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
+      <c r="G30" s="9">
+        <f>0.5</f>
+        <v>0.5</v>
+      </c>
       <c r="H30" s="9"/>
-      <c r="I30" s="9"/>
+      <c r="I30" s="9">
+        <f>3+2.5+1.5+3+2+3</f>
+        <v>15</v>
+      </c>
       <c r="K30" s="9"/>
       <c r="L30" s="9"/>
-      <c r="M30" s="9"/>
+      <c r="M30" s="9">
+        <f>2+5</f>
+        <v>7</v>
+      </c>
       <c r="N30" s="9"/>
-      <c r="O30" s="9"/>
+      <c r="O30" s="9">
+        <f>2.5</f>
+        <v>2.5</v>
+      </c>
     </row>
     <row r="31" spans="2:15">
       <c r="B31" s="2">
@@ -6994,7 +7107,7 @@
       <c r="C35" s="5"/>
       <c r="E35" s="6">
         <f>SUM(E6:E33)</f>
-        <v>43.5</v>
+        <v>44</v>
       </c>
       <c r="F35" s="6">
         <f>SUM(F6:F33)</f>
@@ -7002,15 +7115,15 @@
       </c>
       <c r="G35" s="6">
         <f>SUM(G6:G33)</f>
-        <v>80</v>
+        <v>80.5</v>
       </c>
       <c r="H35" s="6">
         <f>SUM(H6:H33)</f>
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="I35" s="6">
         <f>SUM(I6:I33)</f>
-        <v>52.75</v>
+        <v>70.75</v>
       </c>
       <c r="K35" s="6">
         <f>SUM(K6:K33)</f>
@@ -7018,11 +7131,11 @@
       </c>
       <c r="L35" s="6">
         <f>SUM(L6:L33)</f>
-        <v>63.5</v>
+        <v>101</v>
       </c>
       <c r="M35" s="6">
         <f>SUM(M6:M33)</f>
-        <v>39</v>
+        <v>116</v>
       </c>
       <c r="N35" s="6">
         <f>SUM(N6:N33)</f>
@@ -7030,7 +7143,7 @@
       </c>
       <c r="O35" s="6">
         <f>SUM(O6:O33)</f>
-        <v>14.25</v>
+        <v>19.25</v>
       </c>
     </row>
     <row r="36" spans="2:15">
@@ -7040,7 +7153,7 @@
       <c r="C36" s="5"/>
       <c r="E36" s="6">
         <f>SUM(E35:I35)</f>
-        <v>237.75</v>
+        <v>261.75</v>
       </c>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
@@ -7048,7 +7161,7 @@
       <c r="I36" s="7"/>
       <c r="K36" s="6">
         <f>SUM(K35:O35)</f>
-        <v>173.75</v>
+        <v>293.25</v>
       </c>
       <c r="L36" s="7"/>
       <c r="M36" s="7"/>
@@ -7062,23 +7175,23 @@
       <c r="C38" s="5"/>
       <c r="E38" s="6">
         <f>E35+K35</f>
-        <v>88</v>
+        <v>88.5</v>
       </c>
       <c r="F38" s="6">
         <f>F35+L35</f>
-        <v>91</v>
+        <v>128.5</v>
       </c>
       <c r="G38" s="6">
         <f>G35+M35</f>
-        <v>119</v>
+        <v>196.5</v>
       </c>
       <c r="H38" s="6">
         <f>H35+N35</f>
-        <v>46.5</v>
+        <v>51.5</v>
       </c>
       <c r="I38" s="6">
         <f>I35+O35</f>
-        <v>67</v>
+        <v>90</v>
       </c>
     </row>
     <row r="39" spans="2:15">
@@ -7088,7 +7201,7 @@
       <c r="C39" s="5"/>
       <c r="E39" s="6">
         <f>SUM(E38:I38)</f>
-        <v>411.5</v>
+        <v>555</v>
       </c>
     </row>
   </sheetData>
@@ -7116,10 +7229,10 @@
       <selection activeCell="N43" sqref="N43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="57" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="59" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;L&amp;D / &amp;A&amp;R&amp;F</oddFooter>
   </headerFooter>
@@ -7135,7 +7248,7 @@
       <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="12" max="12" width="11.42578125" customWidth="1"/>
   </cols>
@@ -7163,7 +7276,7 @@
       <selection sqref="A1:J44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3.85546875" customWidth="1"/>
     <col min="5" max="5" width="14.85546875" customWidth="1"/>
@@ -7875,7 +7988,7 @@
       <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="4.28515625" customWidth="1"/>
     <col min="2" max="3" width="12" bestFit="1" customWidth="1"/>
@@ -10118,11 +10231,11 @@
       </c>
       <c r="E25" s="10">
         <f>Eingabedaten!E25+Eingabedaten!K25</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F25" s="10">
         <f>Eingabedaten!F25+Eingabedaten!L25</f>
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="G25" s="10">
         <f>Eingabedaten!G25+Eingabedaten!M25</f>
@@ -10130,7 +10243,7 @@
       </c>
       <c r="H25" s="10">
         <f>Eingabedaten!H25+Eingabedaten!N25</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I25" s="10">
         <f>Eingabedaten!I25+Eingabedaten!O25</f>
@@ -10138,35 +10251,35 @@
       </c>
       <c r="J25" s="10">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="L25" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="M25" s="10">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="N25" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O25" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="P25" s="10">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="Q25" s="10">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>22.5</v>
       </c>
       <c r="S25" s="10">
         <f>Eingabedaten!E25+'Eingabedaten (berechnet)'!S24</f>
-        <v>43.5</v>
+        <v>44</v>
       </c>
       <c r="T25" s="10">
         <f>Eingabedaten!F25+'Eingabedaten (berechnet)'!T24</f>
@@ -10178,7 +10291,7 @@
       </c>
       <c r="V25" s="10">
         <f>Eingabedaten!H25+'Eingabedaten (berechnet)'!V24</f>
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="W25" s="10">
         <f>Eingabedaten!I25+'Eingabedaten (berechnet)'!W24</f>
@@ -10186,7 +10299,7 @@
       </c>
       <c r="X25" s="10">
         <f t="shared" si="7"/>
-        <v>237.75</v>
+        <v>241.25</v>
       </c>
       <c r="Z25" s="10">
         <f>Z24+Eingabedaten!K25</f>
@@ -10194,7 +10307,7 @@
       </c>
       <c r="AA25" s="10">
         <f>AA24+Eingabedaten!L25</f>
-        <v>63.5</v>
+        <v>67</v>
       </c>
       <c r="AB25" s="10">
         <f>AB24+Eingabedaten!M25</f>
@@ -10210,11 +10323,11 @@
       </c>
       <c r="AE25" s="10">
         <f t="shared" si="8"/>
-        <v>173.75</v>
+        <v>177.25</v>
       </c>
       <c r="AG25" s="10">
         <f t="shared" si="9"/>
-        <v>411.5</v>
+        <v>418.5</v>
       </c>
     </row>
     <row r="26" spans="2:33">
@@ -10232,7 +10345,7 @@
       </c>
       <c r="F26" s="10">
         <f>Eingabedaten!F26+Eingabedaten!L26</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="G26" s="10">
         <f>Eingabedaten!G26+Eingabedaten!M26</f>
@@ -10248,7 +10361,7 @@
       </c>
       <c r="J26" s="10">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="L26" s="10">
         <f t="shared" si="0"/>
@@ -10256,27 +10369,27 @@
       </c>
       <c r="M26" s="10">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="N26" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="O26" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="P26" s="10">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="Q26" s="10">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="S26" s="10">
         <f>Eingabedaten!E26+'Eingabedaten (berechnet)'!S25</f>
-        <v>43.5</v>
+        <v>44</v>
       </c>
       <c r="T26" s="10">
         <f>Eingabedaten!F26+'Eingabedaten (berechnet)'!T25</f>
@@ -10288,7 +10401,7 @@
       </c>
       <c r="V26" s="10">
         <f>Eingabedaten!H26+'Eingabedaten (berechnet)'!V25</f>
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="W26" s="10">
         <f>Eingabedaten!I26+'Eingabedaten (berechnet)'!W25</f>
@@ -10296,7 +10409,7 @@
       </c>
       <c r="X26" s="10">
         <f t="shared" si="7"/>
-        <v>237.75</v>
+        <v>241.25</v>
       </c>
       <c r="Z26" s="10">
         <f>Z25+Eingabedaten!K26</f>
@@ -10304,7 +10417,7 @@
       </c>
       <c r="AA26" s="10">
         <f>AA25+Eingabedaten!L26</f>
-        <v>63.5</v>
+        <v>97</v>
       </c>
       <c r="AB26" s="10">
         <f>AB25+Eingabedaten!M26</f>
@@ -10320,11 +10433,11 @@
       </c>
       <c r="AE26" s="10">
         <f t="shared" si="8"/>
-        <v>173.75</v>
+        <v>207.25</v>
       </c>
       <c r="AG26" s="10">
         <f t="shared" si="9"/>
-        <v>411.5</v>
+        <v>448.5</v>
       </c>
     </row>
     <row r="27" spans="2:33">
@@ -10342,11 +10455,11 @@
       </c>
       <c r="F27" s="10">
         <f>Eingabedaten!F27+Eingabedaten!L27</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G27" s="10">
         <f>Eingabedaten!G27+Eingabedaten!M27</f>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="H27" s="10">
         <f>Eingabedaten!H27+Eingabedaten!N27</f>
@@ -10358,7 +10471,7 @@
       </c>
       <c r="J27" s="10">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="L27" s="10">
         <f t="shared" si="0"/>
@@ -10366,27 +10479,27 @@
       </c>
       <c r="M27" s="10">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="N27" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="O27" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="P27" s="10">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="Q27" s="10">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>91</v>
       </c>
       <c r="S27" s="10">
         <f>Eingabedaten!E27+'Eingabedaten (berechnet)'!S26</f>
-        <v>43.5</v>
+        <v>44</v>
       </c>
       <c r="T27" s="10">
         <f>Eingabedaten!F27+'Eingabedaten (berechnet)'!T26</f>
@@ -10398,7 +10511,7 @@
       </c>
       <c r="V27" s="10">
         <f>Eingabedaten!H27+'Eingabedaten (berechnet)'!V26</f>
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="W27" s="10">
         <f>Eingabedaten!I27+'Eingabedaten (berechnet)'!W26</f>
@@ -10406,7 +10519,7 @@
       </c>
       <c r="X27" s="10">
         <f t="shared" si="7"/>
-        <v>237.75</v>
+        <v>241.25</v>
       </c>
       <c r="Z27" s="10">
         <f>Z26+Eingabedaten!K27</f>
@@ -10414,11 +10527,11 @@
       </c>
       <c r="AA27" s="10">
         <f>AA26+Eingabedaten!L27</f>
-        <v>63.5</v>
+        <v>101</v>
       </c>
       <c r="AB27" s="10">
         <f>AB26+Eingabedaten!M27</f>
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="AC27" s="10">
         <f>AC26+Eingabedaten!N27</f>
@@ -10430,11 +10543,11 @@
       </c>
       <c r="AE27" s="10">
         <f t="shared" si="8"/>
-        <v>173.75</v>
+        <v>236.25</v>
       </c>
       <c r="AG27" s="10">
         <f t="shared" si="9"/>
-        <v>411.5</v>
+        <v>477.5</v>
       </c>
     </row>
     <row r="28" spans="2:33">
@@ -10456,7 +10569,7 @@
       </c>
       <c r="G28" s="10">
         <f>Eingabedaten!G28+Eingabedaten!M28</f>
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="H28" s="10">
         <f>Eingabedaten!H28+Eingabedaten!N28</f>
@@ -10468,7 +10581,7 @@
       </c>
       <c r="J28" s="10">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="L28" s="10">
         <f t="shared" si="0"/>
@@ -10480,23 +10593,23 @@
       </c>
       <c r="N28" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="O28" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="P28" s="10">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="Q28" s="10">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>99</v>
       </c>
       <c r="S28" s="10">
         <f>Eingabedaten!E28+'Eingabedaten (berechnet)'!S27</f>
-        <v>43.5</v>
+        <v>44</v>
       </c>
       <c r="T28" s="10">
         <f>Eingabedaten!F28+'Eingabedaten (berechnet)'!T27</f>
@@ -10508,7 +10621,7 @@
       </c>
       <c r="V28" s="10">
         <f>Eingabedaten!H28+'Eingabedaten (berechnet)'!V27</f>
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="W28" s="10">
         <f>Eingabedaten!I28+'Eingabedaten (berechnet)'!W27</f>
@@ -10516,7 +10629,7 @@
       </c>
       <c r="X28" s="10">
         <f t="shared" si="7"/>
-        <v>237.75</v>
+        <v>241.25</v>
       </c>
       <c r="Z28" s="10">
         <f>Z27+Eingabedaten!K28</f>
@@ -10524,11 +10637,11 @@
       </c>
       <c r="AA28" s="10">
         <f>AA27+Eingabedaten!L28</f>
-        <v>63.5</v>
+        <v>101</v>
       </c>
       <c r="AB28" s="10">
         <f>AB27+Eingabedaten!M28</f>
-        <v>39</v>
+        <v>97</v>
       </c>
       <c r="AC28" s="10">
         <f>AC27+Eingabedaten!N28</f>
@@ -10540,11 +10653,11 @@
       </c>
       <c r="AE28" s="10">
         <f t="shared" si="8"/>
-        <v>173.75</v>
+        <v>269.25</v>
       </c>
       <c r="AG28" s="10">
         <f t="shared" si="9"/>
-        <v>411.5</v>
+        <v>510.5</v>
       </c>
     </row>
     <row r="29" spans="2:33">
@@ -10566,19 +10679,19 @@
       </c>
       <c r="G29" s="10">
         <f>Eingabedaten!G29+Eingabedaten!M29</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="H29" s="10">
         <f>Eingabedaten!H29+Eingabedaten!N29</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I29" s="10">
         <f>Eingabedaten!I29+Eingabedaten!O29</f>
-        <v>0</v>
+        <v>5.5</v>
       </c>
       <c r="J29" s="10">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>19.5</v>
       </c>
       <c r="L29" s="10">
         <f t="shared" si="0"/>
@@ -10590,23 +10703,23 @@
       </c>
       <c r="N29" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="O29" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="P29" s="10">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>19.5</v>
       </c>
       <c r="Q29" s="10">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>45.5</v>
       </c>
       <c r="S29" s="10">
         <f>Eingabedaten!E29+'Eingabedaten (berechnet)'!S28</f>
-        <v>43.5</v>
+        <v>44</v>
       </c>
       <c r="T29" s="10">
         <f>Eingabedaten!F29+'Eingabedaten (berechnet)'!T28</f>
@@ -10618,15 +10731,15 @@
       </c>
       <c r="V29" s="10">
         <f>Eingabedaten!H29+'Eingabedaten (berechnet)'!V28</f>
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="W29" s="10">
         <f>Eingabedaten!I29+'Eingabedaten (berechnet)'!W28</f>
-        <v>52.75</v>
+        <v>55.75</v>
       </c>
       <c r="X29" s="10">
         <f t="shared" si="7"/>
-        <v>237.75</v>
+        <v>246.25</v>
       </c>
       <c r="Z29" s="10">
         <f>Z28+Eingabedaten!K29</f>
@@ -10634,11 +10747,11 @@
       </c>
       <c r="AA29" s="10">
         <f>AA28+Eingabedaten!L29</f>
-        <v>63.5</v>
+        <v>101</v>
       </c>
       <c r="AB29" s="10">
         <f>AB28+Eingabedaten!M29</f>
-        <v>39</v>
+        <v>109</v>
       </c>
       <c r="AC29" s="10">
         <f>AC28+Eingabedaten!N29</f>
@@ -10646,15 +10759,15 @@
       </c>
       <c r="AD29" s="10">
         <f>AD28+Eingabedaten!O29</f>
-        <v>14.25</v>
+        <v>16.75</v>
       </c>
       <c r="AE29" s="10">
         <f t="shared" si="8"/>
-        <v>173.75</v>
+        <v>283.75</v>
       </c>
       <c r="AG29" s="10">
         <f t="shared" si="9"/>
-        <v>411.5</v>
+        <v>530</v>
       </c>
     </row>
     <row r="30" spans="2:33">
@@ -10676,7 +10789,7 @@
       </c>
       <c r="G30" s="10">
         <f>Eingabedaten!G30+Eingabedaten!M30</f>
-        <v>0</v>
+        <v>7.5</v>
       </c>
       <c r="H30" s="10">
         <f>Eingabedaten!H30+Eingabedaten!N30</f>
@@ -10684,11 +10797,11 @@
       </c>
       <c r="I30" s="10">
         <f>Eingabedaten!I30+Eingabedaten!O30</f>
-        <v>0</v>
+        <v>17.5</v>
       </c>
       <c r="J30" s="10">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="L30" s="10">
         <f t="shared" si="0"/>
@@ -10700,23 +10813,23 @@
       </c>
       <c r="N30" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>7.5</v>
       </c>
       <c r="O30" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>7.5</v>
       </c>
       <c r="P30" s="10">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="Q30" s="10">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="S30" s="10">
         <f>Eingabedaten!E30+'Eingabedaten (berechnet)'!S29</f>
-        <v>43.5</v>
+        <v>44</v>
       </c>
       <c r="T30" s="10">
         <f>Eingabedaten!F30+'Eingabedaten (berechnet)'!T29</f>
@@ -10724,19 +10837,19 @@
       </c>
       <c r="U30" s="10">
         <f>Eingabedaten!G30+'Eingabedaten (berechnet)'!U29</f>
-        <v>80</v>
+        <v>80.5</v>
       </c>
       <c r="V30" s="10">
         <f>Eingabedaten!H30+'Eingabedaten (berechnet)'!V29</f>
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="W30" s="10">
         <f>Eingabedaten!I30+'Eingabedaten (berechnet)'!W29</f>
-        <v>52.75</v>
+        <v>70.75</v>
       </c>
       <c r="X30" s="10">
         <f t="shared" si="7"/>
-        <v>237.75</v>
+        <v>261.75</v>
       </c>
       <c r="Z30" s="10">
         <f>Z29+Eingabedaten!K30</f>
@@ -10744,11 +10857,11 @@
       </c>
       <c r="AA30" s="10">
         <f>AA29+Eingabedaten!L30</f>
-        <v>63.5</v>
+        <v>101</v>
       </c>
       <c r="AB30" s="10">
         <f>AB29+Eingabedaten!M30</f>
-        <v>39</v>
+        <v>116</v>
       </c>
       <c r="AC30" s="10">
         <f>AC29+Eingabedaten!N30</f>
@@ -10756,15 +10869,15 @@
       </c>
       <c r="AD30" s="10">
         <f>AD29+Eingabedaten!O30</f>
-        <v>14.25</v>
+        <v>19.25</v>
       </c>
       <c r="AE30" s="10">
         <f t="shared" si="8"/>
-        <v>173.75</v>
+        <v>293.25</v>
       </c>
       <c r="AG30" s="10">
         <f t="shared" si="9"/>
-        <v>411.5</v>
+        <v>555</v>
       </c>
     </row>
     <row r="31" spans="2:33">
@@ -10826,7 +10939,7 @@
       </c>
       <c r="S31" s="10">
         <f>Eingabedaten!E31+'Eingabedaten (berechnet)'!S30</f>
-        <v>43.5</v>
+        <v>44</v>
       </c>
       <c r="T31" s="10">
         <f>Eingabedaten!F31+'Eingabedaten (berechnet)'!T30</f>
@@ -10834,19 +10947,19 @@
       </c>
       <c r="U31" s="10">
         <f>Eingabedaten!G31+'Eingabedaten (berechnet)'!U30</f>
-        <v>80</v>
+        <v>80.5</v>
       </c>
       <c r="V31" s="10">
         <f>Eingabedaten!H31+'Eingabedaten (berechnet)'!V30</f>
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="W31" s="10">
         <f>Eingabedaten!I31+'Eingabedaten (berechnet)'!W30</f>
-        <v>52.75</v>
+        <v>70.75</v>
       </c>
       <c r="X31" s="10">
         <f t="shared" si="7"/>
-        <v>237.75</v>
+        <v>261.75</v>
       </c>
       <c r="Z31" s="10">
         <f>Z30+Eingabedaten!K31</f>
@@ -10854,11 +10967,11 @@
       </c>
       <c r="AA31" s="10">
         <f>AA30+Eingabedaten!L31</f>
-        <v>63.5</v>
+        <v>101</v>
       </c>
       <c r="AB31" s="10">
         <f>AB30+Eingabedaten!M31</f>
-        <v>39</v>
+        <v>116</v>
       </c>
       <c r="AC31" s="10">
         <f>AC30+Eingabedaten!N31</f>
@@ -10866,15 +10979,15 @@
       </c>
       <c r="AD31" s="10">
         <f>AD30+Eingabedaten!O31</f>
-        <v>14.25</v>
+        <v>19.25</v>
       </c>
       <c r="AE31" s="10">
         <f t="shared" si="8"/>
-        <v>173.75</v>
+        <v>293.25</v>
       </c>
       <c r="AG31" s="10">
         <f t="shared" si="9"/>
-        <v>411.5</v>
+        <v>555</v>
       </c>
     </row>
     <row r="32" spans="2:33">
@@ -10936,7 +11049,7 @@
       </c>
       <c r="S32" s="10">
         <f>Eingabedaten!E32+'Eingabedaten (berechnet)'!S31</f>
-        <v>43.5</v>
+        <v>44</v>
       </c>
       <c r="T32" s="10">
         <f>Eingabedaten!F32+'Eingabedaten (berechnet)'!T31</f>
@@ -10944,19 +11057,19 @@
       </c>
       <c r="U32" s="10">
         <f>Eingabedaten!G32+'Eingabedaten (berechnet)'!U31</f>
-        <v>80</v>
+        <v>80.5</v>
       </c>
       <c r="V32" s="10">
         <f>Eingabedaten!H32+'Eingabedaten (berechnet)'!V31</f>
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="W32" s="10">
         <f>Eingabedaten!I32+'Eingabedaten (berechnet)'!W31</f>
-        <v>52.75</v>
+        <v>70.75</v>
       </c>
       <c r="X32" s="10">
         <f t="shared" si="7"/>
-        <v>237.75</v>
+        <v>261.75</v>
       </c>
       <c r="Z32" s="10">
         <f>Z31+Eingabedaten!K32</f>
@@ -10964,11 +11077,11 @@
       </c>
       <c r="AA32" s="10">
         <f>AA31+Eingabedaten!L32</f>
-        <v>63.5</v>
+        <v>101</v>
       </c>
       <c r="AB32" s="10">
         <f>AB31+Eingabedaten!M32</f>
-        <v>39</v>
+        <v>116</v>
       </c>
       <c r="AC32" s="10">
         <f>AC31+Eingabedaten!N32</f>
@@ -10976,15 +11089,15 @@
       </c>
       <c r="AD32" s="10">
         <f>AD31+Eingabedaten!O32</f>
-        <v>14.25</v>
+        <v>19.25</v>
       </c>
       <c r="AE32" s="10">
         <f t="shared" si="8"/>
-        <v>173.75</v>
+        <v>293.25</v>
       </c>
       <c r="AG32" s="10">
         <f t="shared" si="9"/>
-        <v>411.5</v>
+        <v>555</v>
       </c>
     </row>
     <row r="33" spans="2:33">
@@ -11046,7 +11159,7 @@
       </c>
       <c r="S33" s="10">
         <f>Eingabedaten!E33+'Eingabedaten (berechnet)'!S32</f>
-        <v>43.5</v>
+        <v>44</v>
       </c>
       <c r="T33" s="10">
         <f>Eingabedaten!F33+'Eingabedaten (berechnet)'!T32</f>
@@ -11054,19 +11167,19 @@
       </c>
       <c r="U33" s="10">
         <f>Eingabedaten!G33+'Eingabedaten (berechnet)'!U32</f>
-        <v>80</v>
+        <v>80.5</v>
       </c>
       <c r="V33" s="10">
         <f>Eingabedaten!H33+'Eingabedaten (berechnet)'!V32</f>
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="W33" s="10">
         <f>Eingabedaten!I33+'Eingabedaten (berechnet)'!W32</f>
-        <v>52.75</v>
+        <v>70.75</v>
       </c>
       <c r="X33" s="10">
         <f t="shared" si="7"/>
-        <v>237.75</v>
+        <v>261.75</v>
       </c>
       <c r="Z33" s="10">
         <f>Z32+Eingabedaten!K33</f>
@@ -11074,11 +11187,11 @@
       </c>
       <c r="AA33" s="10">
         <f>AA32+Eingabedaten!L33</f>
-        <v>63.5</v>
+        <v>101</v>
       </c>
       <c r="AB33" s="10">
         <f>AB32+Eingabedaten!M33</f>
-        <v>39</v>
+        <v>116</v>
       </c>
       <c r="AC33" s="10">
         <f>AC32+Eingabedaten!N33</f>
@@ -11086,47 +11199,47 @@
       </c>
       <c r="AD33" s="10">
         <f>AD32+Eingabedaten!O33</f>
-        <v>14.25</v>
+        <v>19.25</v>
       </c>
       <c r="AE33" s="10">
         <f t="shared" si="8"/>
-        <v>173.75</v>
+        <v>293.25</v>
       </c>
       <c r="AG33" s="10">
         <f t="shared" si="9"/>
-        <v>411.5</v>
+        <v>555</v>
       </c>
     </row>
     <row r="35" spans="2:33">
       <c r="E35" s="6">
         <f t="shared" ref="E35:J35" si="12">SUM(E6:E33)</f>
-        <v>88</v>
+        <v>88.5</v>
       </c>
       <c r="F35" s="6">
         <f t="shared" si="12"/>
-        <v>91</v>
+        <v>128.5</v>
       </c>
       <c r="G35" s="6">
         <f t="shared" si="12"/>
-        <v>119</v>
+        <v>196.5</v>
       </c>
       <c r="H35" s="6">
         <f t="shared" si="12"/>
-        <v>46.5</v>
+        <v>51.5</v>
       </c>
       <c r="I35" s="6">
         <f t="shared" si="12"/>
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="J35" s="6">
         <f t="shared" si="12"/>
-        <v>411.5</v>
+        <v>555</v>
       </c>
     </row>
     <row r="36" spans="2:33">
       <c r="E36" s="6">
         <f>SUM(E35:I35)</f>
-        <v>411.5</v>
+        <v>555</v>
       </c>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
@@ -11148,7 +11261,7 @@
     <mergeCell ref="Z4:AD4"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="33" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="35" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;L&amp;D / &amp;A&amp;R&amp;F</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Revision: e / 10-Aug-2009
</commit_message>
<xml_diff>
--- a/ProjektManagement/NuvoControl_0011_StundenNachweis_Grafisch.xlsx
+++ b/ProjektManagement/NuvoControl_0011_StundenNachweis_Grafisch.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="35">
   <si>
     <t>Die Werte in diesem Sheet wurden mit dem Dokument "NuvoControl_0010_StundenNachweis" erfasst.</t>
   </si>
@@ -154,13 +154,7 @@
     <t>d / 29-June-2009</t>
   </si>
   <si>
-    <t>in work</t>
-  </si>
-  <si>
-    <t>e / 09-Aug-2009</t>
-  </si>
-  <si>
-    <t>f / xx-xx-2009</t>
+    <t>e / 10-Aug-2009</t>
   </si>
 </sst>
 </file>
@@ -298,7 +292,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -307,7 +301,7 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="de-CH"/>
+  <c:lang val="en-US"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -718,11 +712,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="73112960"/>
-        <c:axId val="73122944"/>
+        <c:axId val="128904576"/>
+        <c:axId val="129304064"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="73112960"/>
+        <c:axId val="128904576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -737,16 +731,16 @@
             <a:pPr>
               <a:defRPr lang="de-CH"/>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="73122944"/>
+        <c:crossAx val="129304064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="73122944"/>
+        <c:axId val="129304064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -761,7 +755,7 @@
               <a:pPr>
                 <a:defRPr lang="de-CH"/>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -775,10 +769,10 @@
             <a:pPr>
               <a:defRPr lang="de-CH"/>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="73112960"/>
+        <c:crossAx val="128904576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -793,7 +787,7 @@
           <a:pPr>
             <a:defRPr lang="de-CH"/>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -809,7 +803,7 @@
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="de-CH"/>
+  <c:lang val="en-US"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1220,11 +1214,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="73423104"/>
-        <c:axId val="73461760"/>
+        <c:axId val="130158976"/>
+        <c:axId val="130160512"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="73423104"/>
+        <c:axId val="130158976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1239,16 +1233,16 @@
             <a:pPr>
               <a:defRPr lang="de-CH"/>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="73461760"/>
+        <c:crossAx val="130160512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="73461760"/>
+        <c:axId val="130160512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1263,7 +1257,7 @@
               <a:pPr>
                 <a:defRPr lang="de-CH"/>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1277,10 +1271,10 @@
             <a:pPr>
               <a:defRPr lang="de-CH"/>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="73423104"/>
+        <c:crossAx val="130158976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1295,7 +1289,7 @@
           <a:pPr>
             <a:defRPr lang="de-CH"/>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1311,7 +1305,7 @@
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="de-CH"/>
+  <c:lang val="en-US"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1722,11 +1716,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="74793728"/>
-        <c:axId val="74795264"/>
+        <c:axId val="139499776"/>
+        <c:axId val="139583488"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="74793728"/>
+        <c:axId val="139499776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1741,16 +1735,16 @@
             <a:pPr>
               <a:defRPr lang="de-CH"/>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="74795264"/>
+        <c:crossAx val="139583488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="74795264"/>
+        <c:axId val="139583488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1765,7 +1759,7 @@
               <a:pPr>
                 <a:defRPr lang="de-CH"/>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1779,10 +1773,10 @@
             <a:pPr>
               <a:defRPr lang="de-CH"/>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="74793728"/>
+        <c:crossAx val="139499776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1797,7 +1791,7 @@
           <a:pPr>
             <a:defRPr lang="de-CH"/>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1813,7 +1807,7 @@
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="de-CH"/>
+  <c:lang val="en-US"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1831,7 +1825,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -2527,11 +2520,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="74913664"/>
-        <c:axId val="74915200"/>
+        <c:axId val="139987968"/>
+        <c:axId val="123978496"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="74913664"/>
+        <c:axId val="139987968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2546,16 +2539,16 @@
             <a:pPr>
               <a:defRPr lang="de-CH"/>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="74915200"/>
+        <c:crossAx val="123978496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="74915200"/>
+        <c:axId val="123978496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2585,7 +2578,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -2597,17 +2589,16 @@
             <a:pPr>
               <a:defRPr lang="de-CH"/>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="74913664"/>
+        <c:crossAx val="139987968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:txPr>
         <a:bodyPr/>
         <a:lstStyle/>
@@ -2615,7 +2606,7 @@
           <a:pPr>
             <a:defRPr lang="de-CH"/>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2631,7 +2622,7 @@
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="de-CH"/>
+  <c:lang val="en-US"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -2649,7 +2640,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -3318,11 +3308,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="74951296"/>
-        <c:axId val="74961280"/>
+        <c:axId val="126324736"/>
+        <c:axId val="126326272"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="74951296"/>
+        <c:axId val="126324736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3337,16 +3327,16 @@
             <a:pPr>
               <a:defRPr lang="de-CH"/>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="74961280"/>
+        <c:crossAx val="126326272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="74961280"/>
+        <c:axId val="126326272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3376,7 +3366,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -3388,17 +3377,16 @@
             <a:pPr>
               <a:defRPr lang="de-CH"/>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="74951296"/>
+        <c:crossAx val="126324736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:txPr>
         <a:bodyPr/>
         <a:lstStyle/>
@@ -3406,7 +3394,7 @@
           <a:pPr>
             <a:defRPr lang="de-CH"/>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3422,7 +3410,7 @@
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="de-CH"/>
+  <c:lang val="en-US"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -3445,7 +3433,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -4417,11 +4404,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="75030528"/>
-        <c:axId val="75032064"/>
+        <c:axId val="126346368"/>
+        <c:axId val="126347904"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="75030528"/>
+        <c:axId val="126346368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4436,16 +4423,16 @@
             <a:pPr>
               <a:defRPr lang="de-CH"/>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="75032064"/>
+        <c:crossAx val="126347904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="75032064"/>
+        <c:axId val="126347904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4475,7 +4462,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -4487,17 +4473,16 @@
             <a:pPr>
               <a:defRPr lang="de-CH"/>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="75030528"/>
+        <c:crossAx val="126346368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:txPr>
         <a:bodyPr/>
         <a:lstStyle/>
@@ -4505,7 +4490,7 @@
           <a:pPr>
             <a:defRPr lang="de-CH"/>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4521,7 +4506,7 @@
 
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="de-CH"/>
+  <c:lang val="en-US"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -4544,7 +4529,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -5516,11 +5500,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="75198848"/>
-        <c:axId val="75200384"/>
+        <c:axId val="128427520"/>
+        <c:axId val="128429056"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="75198848"/>
+        <c:axId val="128427520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5535,16 +5519,16 @@
             <a:pPr>
               <a:defRPr lang="de-CH"/>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="75200384"/>
+        <c:crossAx val="128429056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="75200384"/>
+        <c:axId val="128429056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5574,7 +5558,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -5586,17 +5569,16 @@
             <a:pPr>
               <a:defRPr lang="de-CH"/>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="75198848"/>
+        <c:crossAx val="128427520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:txPr>
         <a:bodyPr/>
         <a:lstStyle/>
@@ -5604,7 +5586,7 @@
           <a:pPr>
             <a:defRPr lang="de-CH"/>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -5839,9 +5821,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -5879,7 +5861,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -5949,7 +5931,7 @@
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -6126,13 +6108,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B3:E9"/>
+  <dimension ref="B3:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C9" sqref="C9:E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3.7109375" customWidth="1"/>
     <col min="2" max="2" width="6.85546875" customWidth="1"/>
@@ -6179,18 +6161,10 @@
     </row>
     <row r="8" spans="2:5">
       <c r="C8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E8" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5">
-      <c r="C9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E9" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -6214,7 +6188,7 @@
       <selection pane="bottomLeft" activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3.140625" customWidth="1"/>
     <col min="2" max="2" width="14.140625" customWidth="1"/>
@@ -7229,10 +7203,10 @@
       <selection activeCell="N43" sqref="N43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="59" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="57" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;L&amp;D / &amp;A&amp;R&amp;F</oddFooter>
   </headerFooter>
@@ -7248,7 +7222,7 @@
       <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="12" max="12" width="11.42578125" customWidth="1"/>
   </cols>
@@ -7276,7 +7250,7 @@
       <selection sqref="A1:J44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3.85546875" customWidth="1"/>
     <col min="5" max="5" width="14.85546875" customWidth="1"/>
@@ -7988,7 +7962,7 @@
       <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="4.28515625" customWidth="1"/>
     <col min="2" max="3" width="12" bestFit="1" customWidth="1"/>
@@ -11261,7 +11235,7 @@
     <mergeCell ref="Z4:AD4"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="35" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="33" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;L&amp;D / &amp;A&amp;R&amp;F</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Stunden bis 22.8.2009 nachgetragen (Revision f / 22-Aug-2009)
</commit_message>
<xml_diff>
--- a/ProjektManagement/NuvoControl_0011_StundenNachweis_Grafisch.xlsx
+++ b/ProjektManagement/NuvoControl_0011_StundenNachweis_Grafisch.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="37">
   <si>
     <t>Die Werte in diesem Sheet wurden mit dem Dokument "NuvoControl_0010_StundenNachweis" erfasst.</t>
   </si>
@@ -155,6 +155,12 @@
   </si>
   <si>
     <t>e / 10-Aug-2009</t>
+  </si>
+  <si>
+    <t>f / 22-Aug-2009</t>
+  </si>
+  <si>
+    <t>Zwischenstand kurz vor Abgabe</t>
   </si>
 </sst>
 </file>
@@ -696,27 +702,27 @@
                   <c:v>246.25</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>261.75</c:v>
+                  <c:v>266.25</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>261.75</c:v>
+                  <c:v>296.75</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>261.75</c:v>
+                  <c:v>337.75</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>261.75</c:v>
+                  <c:v>337.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="128904576"/>
-        <c:axId val="129304064"/>
+        <c:axId val="132957312"/>
+        <c:axId val="132958848"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="128904576"/>
+        <c:axId val="132957312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -734,13 +740,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="129304064"/>
+        <c:crossAx val="132958848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="129304064"/>
+        <c:axId val="132958848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -772,7 +778,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="128904576"/>
+        <c:crossAx val="132957312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1198,27 +1204,27 @@
                   <c:v>283.75</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>293.25</c:v>
+                  <c:v>304.25</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>293.25</c:v>
+                  <c:v>328.75</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>293.25</c:v>
+                  <c:v>352.75</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>293.25</c:v>
+                  <c:v>352.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="130158976"/>
-        <c:axId val="130160512"/>
+        <c:axId val="133009408"/>
+        <c:axId val="133010944"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="130158976"/>
+        <c:axId val="133009408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1236,13 +1242,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="130160512"/>
+        <c:crossAx val="133010944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="130160512"/>
+        <c:axId val="133010944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1274,7 +1280,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="130158976"/>
+        <c:crossAx val="133009408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1700,27 +1706,27 @@
                   <c:v>530</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>555</c:v>
+                  <c:v>570.5</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>555</c:v>
+                  <c:v>625.5</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>555</c:v>
+                  <c:v>690.5</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>555</c:v>
+                  <c:v>690.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="139499776"/>
-        <c:axId val="139583488"/>
+        <c:axId val="133032192"/>
+        <c:axId val="125046784"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="139499776"/>
+        <c:axId val="133032192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1738,13 +1744,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="139583488"/>
+        <c:crossAx val="125046784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="139583488"/>
+        <c:axId val="125046784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1776,7 +1782,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="139499776"/>
+        <c:crossAx val="133032192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1825,6 +1831,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -1956,6 +1963,12 @@
                 <c:pt idx="23">
                   <c:v>2</c:v>
                 </c:pt>
+                <c:pt idx="25">
+                  <c:v>10.5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>15</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2093,7 +2106,13 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.5</c:v>
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2513,18 +2532,24 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>15</c:v>
+                  <c:v>15.5</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>16.5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>17</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="139987968"/>
-        <c:axId val="123978496"/>
+        <c:axId val="125218176"/>
+        <c:axId val="125109376"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="139987968"/>
+        <c:axId val="125218176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2542,13 +2567,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="123978496"/>
+        <c:crossAx val="125109376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="123978496"/>
+        <c:axId val="125109376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2578,6 +2603,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -2592,13 +2618,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="139987968"/>
+        <c:crossAx val="125218176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:txPr>
         <a:bodyPr/>
         <a:lstStyle/>
@@ -2640,6 +2667,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -2759,6 +2787,9 @@
                 <c:pt idx="18">
                   <c:v>1</c:v>
                 </c:pt>
+                <c:pt idx="25">
+                  <c:v>4</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2893,7 +2924,13 @@
                   <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>7</c:v>
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3303,16 +3340,22 @@
                 <c:pt idx="24">
                   <c:v>2.5</c:v>
                 </c:pt>
+                <c:pt idx="25">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>12</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="126324736"/>
-        <c:axId val="126326272"/>
+        <c:axId val="125161856"/>
+        <c:axId val="125163392"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="126324736"/>
+        <c:axId val="125161856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3330,13 +3373,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="126326272"/>
+        <c:crossAx val="125163392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="126326272"/>
+        <c:axId val="125163392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3366,6 +3409,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -3380,13 +3424,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="126324736"/>
+        <c:crossAx val="125161856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:txPr>
         <a:bodyPr/>
         <a:lstStyle/>
@@ -3433,6 +3478,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -3619,13 +3665,13 @@
                   <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>39</c:v>
+                  <c:v>49.5</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>39</c:v>
+                  <c:v>64.5</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>39</c:v>
+                  <c:v>64.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3809,16 +3855,16 @@
                   <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>80.5</c:v>
+                  <c:v>84.5</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>80.5</c:v>
+                  <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>80.5</c:v>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>80.5</c:v>
+                  <c:v>97</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4388,27 +4434,27 @@
                   <c:v>55.75</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>70.75</c:v>
+                  <c:v>71.25</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>70.75</c:v>
+                  <c:v>87.75</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>70.75</c:v>
+                  <c:v>104.75</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>70.75</c:v>
+                  <c:v>104.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="126346368"/>
-        <c:axId val="126347904"/>
+        <c:axId val="125281792"/>
+        <c:axId val="125283328"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="126346368"/>
+        <c:axId val="125281792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4426,13 +4472,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="126347904"/>
+        <c:crossAx val="125283328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="126347904"/>
+        <c:axId val="125283328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4462,6 +4508,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -4476,13 +4523,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="126346368"/>
+        <c:crossAx val="125281792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:txPr>
         <a:bodyPr/>
         <a:lstStyle/>
@@ -4529,6 +4577,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -4715,13 +4764,13 @@
                   <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>12.5</c:v>
+                  <c:v>16.5</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>12.5</c:v>
+                  <c:v>16.5</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>12.5</c:v>
+                  <c:v>16.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4905,16 +4954,16 @@
                   <c:v>109</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>116</c:v>
+                  <c:v>127</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>116</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>116</c:v>
+                  <c:v>147</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>116</c:v>
+                  <c:v>147</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5487,24 +5536,24 @@
                   <c:v>19.25</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>19.25</c:v>
+                  <c:v>31.75</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>19.25</c:v>
+                  <c:v>43.75</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>19.25</c:v>
+                  <c:v>43.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="128427520"/>
-        <c:axId val="128429056"/>
+        <c:axId val="125446016"/>
+        <c:axId val="125447552"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="128427520"/>
+        <c:axId val="125446016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5522,13 +5571,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="128429056"/>
+        <c:crossAx val="125447552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="128429056"/>
+        <c:axId val="125447552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5558,6 +5607,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -5572,13 +5622,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="128427520"/>
+        <c:crossAx val="125446016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:txPr>
         <a:bodyPr/>
         <a:lstStyle/>
@@ -6108,10 +6159,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B3:E8"/>
+  <dimension ref="B3:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9:E9"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -6165,6 +6216,14 @@
       </c>
       <c r="E8" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5">
+      <c r="C9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -6184,8 +6243,8 @@
   <dimension ref="B2:O39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F35" sqref="F35"/>
+      <pane ySplit="5" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -6994,19 +7053,19 @@
       <c r="E30" s="9"/>
       <c r="F30" s="9"/>
       <c r="G30" s="9">
-        <f>0.5</f>
-        <v>0.5</v>
+        <f>0.5+4</f>
+        <v>4.5</v>
       </c>
       <c r="H30" s="9"/>
       <c r="I30" s="9">
-        <f>3+2.5+1.5+3+2+3</f>
-        <v>15</v>
+        <f>3+2.5+1.5+3+2+3+0.5</f>
+        <v>15.5</v>
       </c>
       <c r="K30" s="9"/>
       <c r="L30" s="9"/>
       <c r="M30" s="9">
-        <f>2+5</f>
-        <v>7</v>
+        <f>2+5+2+6+3</f>
+        <v>18</v>
       </c>
       <c r="N30" s="9"/>
       <c r="O30" s="9">
@@ -7025,14 +7084,32 @@
       </c>
       <c r="E31" s="9"/>
       <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="9"/>
-      <c r="I31" s="9"/>
+      <c r="G31" s="9">
+        <f>3.5</f>
+        <v>3.5</v>
+      </c>
+      <c r="H31" s="9">
+        <f>2.5+1+4+3</f>
+        <v>10.5</v>
+      </c>
+      <c r="I31" s="9">
+        <f>2+1+2.5+2+4.5+3+1.5</f>
+        <v>16.5</v>
+      </c>
       <c r="K31" s="9"/>
       <c r="L31" s="9"/>
-      <c r="M31" s="9"/>
-      <c r="N31" s="9"/>
-      <c r="O31" s="9"/>
+      <c r="M31" s="9">
+        <f>4+4</f>
+        <v>8</v>
+      </c>
+      <c r="N31" s="9">
+        <f>4</f>
+        <v>4</v>
+      </c>
+      <c r="O31" s="9">
+        <f>1+1.5+10</f>
+        <v>12.5</v>
+      </c>
     </row>
     <row r="32" spans="2:15">
       <c r="B32" s="2">
@@ -7045,14 +7122,29 @@
       </c>
       <c r="E32" s="9"/>
       <c r="F32" s="9"/>
-      <c r="G32" s="9"/>
-      <c r="H32" s="9"/>
-      <c r="I32" s="9"/>
+      <c r="G32" s="9">
+        <f>2.5+6+0.5</f>
+        <v>9</v>
+      </c>
+      <c r="H32" s="9">
+        <f>4+4+7</f>
+        <v>15</v>
+      </c>
+      <c r="I32" s="9">
+        <f>2.5+4.5+6+2+0.5+1.5</f>
+        <v>17</v>
+      </c>
       <c r="K32" s="9"/>
       <c r="L32" s="9"/>
-      <c r="M32" s="9"/>
+      <c r="M32" s="9">
+        <f>4+8</f>
+        <v>12</v>
+      </c>
       <c r="N32" s="9"/>
-      <c r="O32" s="9"/>
+      <c r="O32" s="9">
+        <f>2+3+7</f>
+        <v>12</v>
+      </c>
     </row>
     <row r="33" spans="2:15">
       <c r="B33" s="2">
@@ -7089,15 +7181,15 @@
       </c>
       <c r="G35" s="6">
         <f>SUM(G6:G33)</f>
-        <v>80.5</v>
+        <v>97</v>
       </c>
       <c r="H35" s="6">
         <f>SUM(H6:H33)</f>
-        <v>39</v>
+        <v>64.5</v>
       </c>
       <c r="I35" s="6">
         <f>SUM(I6:I33)</f>
-        <v>70.75</v>
+        <v>104.75</v>
       </c>
       <c r="K35" s="6">
         <f>SUM(K6:K33)</f>
@@ -7109,15 +7201,15 @@
       </c>
       <c r="M35" s="6">
         <f>SUM(M6:M33)</f>
-        <v>116</v>
+        <v>147</v>
       </c>
       <c r="N35" s="6">
         <f>SUM(N6:N33)</f>
-        <v>12.5</v>
+        <v>16.5</v>
       </c>
       <c r="O35" s="6">
         <f>SUM(O6:O33)</f>
-        <v>19.25</v>
+        <v>43.75</v>
       </c>
     </row>
     <row r="36" spans="2:15">
@@ -7127,7 +7219,7 @@
       <c r="C36" s="5"/>
       <c r="E36" s="6">
         <f>SUM(E35:I35)</f>
-        <v>261.75</v>
+        <v>337.75</v>
       </c>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
@@ -7135,7 +7227,7 @@
       <c r="I36" s="7"/>
       <c r="K36" s="6">
         <f>SUM(K35:O35)</f>
-        <v>293.25</v>
+        <v>352.75</v>
       </c>
       <c r="L36" s="7"/>
       <c r="M36" s="7"/>
@@ -7157,15 +7249,15 @@
       </c>
       <c r="G38" s="6">
         <f>G35+M35</f>
-        <v>196.5</v>
+        <v>244</v>
       </c>
       <c r="H38" s="6">
         <f>H35+N35</f>
-        <v>51.5</v>
+        <v>81</v>
       </c>
       <c r="I38" s="6">
         <f>I35+O35</f>
-        <v>90</v>
+        <v>148.5</v>
       </c>
     </row>
     <row r="39" spans="2:15">
@@ -7175,7 +7267,7 @@
       <c r="C39" s="5"/>
       <c r="E39" s="6">
         <f>SUM(E38:I38)</f>
-        <v>555</v>
+        <v>690.5</v>
       </c>
     </row>
   </sheetData>
@@ -10763,7 +10855,7 @@
       </c>
       <c r="G30" s="10">
         <f>Eingabedaten!G30+Eingabedaten!M30</f>
-        <v>7.5</v>
+        <v>22.5</v>
       </c>
       <c r="H30" s="10">
         <f>Eingabedaten!H30+Eingabedaten!N30</f>
@@ -10771,11 +10863,11 @@
       </c>
       <c r="I30" s="10">
         <f>Eingabedaten!I30+Eingabedaten!O30</f>
-        <v>17.5</v>
+        <v>18</v>
       </c>
       <c r="J30" s="10">
         <f t="shared" si="5"/>
-        <v>25</v>
+        <v>40.5</v>
       </c>
       <c r="L30" s="10">
         <f t="shared" si="0"/>
@@ -10787,19 +10879,19 @@
       </c>
       <c r="N30" s="10">
         <f t="shared" si="2"/>
-        <v>7.5</v>
+        <v>22.5</v>
       </c>
       <c r="O30" s="10">
         <f t="shared" si="3"/>
-        <v>7.5</v>
+        <v>22.5</v>
       </c>
       <c r="P30" s="10">
         <f t="shared" si="4"/>
-        <v>25</v>
+        <v>40.5</v>
       </c>
       <c r="Q30" s="10">
         <f t="shared" si="6"/>
-        <v>40</v>
+        <v>85.5</v>
       </c>
       <c r="S30" s="10">
         <f>Eingabedaten!E30+'Eingabedaten (berechnet)'!S29</f>
@@ -10811,7 +10903,7 @@
       </c>
       <c r="U30" s="10">
         <f>Eingabedaten!G30+'Eingabedaten (berechnet)'!U29</f>
-        <v>80.5</v>
+        <v>84.5</v>
       </c>
       <c r="V30" s="10">
         <f>Eingabedaten!H30+'Eingabedaten (berechnet)'!V29</f>
@@ -10819,11 +10911,11 @@
       </c>
       <c r="W30" s="10">
         <f>Eingabedaten!I30+'Eingabedaten (berechnet)'!W29</f>
-        <v>70.75</v>
+        <v>71.25</v>
       </c>
       <c r="X30" s="10">
         <f t="shared" si="7"/>
-        <v>261.75</v>
+        <v>266.25</v>
       </c>
       <c r="Z30" s="10">
         <f>Z29+Eingabedaten!K30</f>
@@ -10835,7 +10927,7 @@
       </c>
       <c r="AB30" s="10">
         <f>AB29+Eingabedaten!M30</f>
-        <v>116</v>
+        <v>127</v>
       </c>
       <c r="AC30" s="10">
         <f>AC29+Eingabedaten!N30</f>
@@ -10847,11 +10939,11 @@
       </c>
       <c r="AE30" s="10">
         <f t="shared" si="8"/>
-        <v>293.25</v>
+        <v>304.25</v>
       </c>
       <c r="AG30" s="10">
         <f t="shared" si="9"/>
-        <v>555</v>
+        <v>570.5</v>
       </c>
     </row>
     <row r="31" spans="2:33">
@@ -10873,19 +10965,19 @@
       </c>
       <c r="G31" s="10">
         <f>Eingabedaten!G31+Eingabedaten!M31</f>
-        <v>0</v>
+        <v>11.5</v>
       </c>
       <c r="H31" s="10">
         <f>Eingabedaten!H31+Eingabedaten!N31</f>
-        <v>0</v>
+        <v>14.5</v>
       </c>
       <c r="I31" s="10">
         <f>Eingabedaten!I31+Eingabedaten!O31</f>
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="J31" s="10">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="L31" s="10">
         <f t="shared" si="0"/>
@@ -10897,19 +10989,19 @@
       </c>
       <c r="N31" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>11.5</v>
       </c>
       <c r="O31" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="P31" s="10">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="Q31" s="10">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>92.5</v>
       </c>
       <c r="S31" s="10">
         <f>Eingabedaten!E31+'Eingabedaten (berechnet)'!S30</f>
@@ -10921,19 +11013,19 @@
       </c>
       <c r="U31" s="10">
         <f>Eingabedaten!G31+'Eingabedaten (berechnet)'!U30</f>
-        <v>80.5</v>
+        <v>88</v>
       </c>
       <c r="V31" s="10">
         <f>Eingabedaten!H31+'Eingabedaten (berechnet)'!V30</f>
-        <v>39</v>
+        <v>49.5</v>
       </c>
       <c r="W31" s="10">
         <f>Eingabedaten!I31+'Eingabedaten (berechnet)'!W30</f>
-        <v>70.75</v>
+        <v>87.75</v>
       </c>
       <c r="X31" s="10">
         <f t="shared" si="7"/>
-        <v>261.75</v>
+        <v>296.75</v>
       </c>
       <c r="Z31" s="10">
         <f>Z30+Eingabedaten!K31</f>
@@ -10945,23 +11037,23 @@
       </c>
       <c r="AB31" s="10">
         <f>AB30+Eingabedaten!M31</f>
-        <v>116</v>
+        <v>135</v>
       </c>
       <c r="AC31" s="10">
         <f>AC30+Eingabedaten!N31</f>
-        <v>12.5</v>
+        <v>16.5</v>
       </c>
       <c r="AD31" s="10">
         <f>AD30+Eingabedaten!O31</f>
-        <v>19.25</v>
+        <v>31.75</v>
       </c>
       <c r="AE31" s="10">
         <f t="shared" si="8"/>
-        <v>293.25</v>
+        <v>328.75</v>
       </c>
       <c r="AG31" s="10">
         <f t="shared" si="9"/>
-        <v>555</v>
+        <v>625.5</v>
       </c>
     </row>
     <row r="32" spans="2:33">
@@ -10983,19 +11075,19 @@
       </c>
       <c r="G32" s="10">
         <f>Eingabedaten!G32+Eingabedaten!M32</f>
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="H32" s="10">
         <f>Eingabedaten!H32+Eingabedaten!N32</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="I32" s="10">
         <f>Eingabedaten!I32+Eingabedaten!O32</f>
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="J32" s="10">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="L32" s="10">
         <f t="shared" si="0"/>
@@ -11007,19 +11099,19 @@
       </c>
       <c r="N32" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="O32" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="P32" s="10">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="Q32" s="10">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>122</v>
       </c>
       <c r="S32" s="10">
         <f>Eingabedaten!E32+'Eingabedaten (berechnet)'!S31</f>
@@ -11031,19 +11123,19 @@
       </c>
       <c r="U32" s="10">
         <f>Eingabedaten!G32+'Eingabedaten (berechnet)'!U31</f>
-        <v>80.5</v>
+        <v>97</v>
       </c>
       <c r="V32" s="10">
         <f>Eingabedaten!H32+'Eingabedaten (berechnet)'!V31</f>
-        <v>39</v>
+        <v>64.5</v>
       </c>
       <c r="W32" s="10">
         <f>Eingabedaten!I32+'Eingabedaten (berechnet)'!W31</f>
-        <v>70.75</v>
+        <v>104.75</v>
       </c>
       <c r="X32" s="10">
         <f t="shared" si="7"/>
-        <v>261.75</v>
+        <v>337.75</v>
       </c>
       <c r="Z32" s="10">
         <f>Z31+Eingabedaten!K32</f>
@@ -11055,23 +11147,23 @@
       </c>
       <c r="AB32" s="10">
         <f>AB31+Eingabedaten!M32</f>
-        <v>116</v>
+        <v>147</v>
       </c>
       <c r="AC32" s="10">
         <f>AC31+Eingabedaten!N32</f>
-        <v>12.5</v>
+        <v>16.5</v>
       </c>
       <c r="AD32" s="10">
         <f>AD31+Eingabedaten!O32</f>
-        <v>19.25</v>
+        <v>43.75</v>
       </c>
       <c r="AE32" s="10">
         <f t="shared" si="8"/>
-        <v>293.25</v>
+        <v>352.75</v>
       </c>
       <c r="AG32" s="10">
         <f t="shared" si="9"/>
-        <v>555</v>
+        <v>690.5</v>
       </c>
     </row>
     <row r="33" spans="2:33">
@@ -11141,19 +11233,19 @@
       </c>
       <c r="U33" s="10">
         <f>Eingabedaten!G33+'Eingabedaten (berechnet)'!U32</f>
-        <v>80.5</v>
+        <v>97</v>
       </c>
       <c r="V33" s="10">
         <f>Eingabedaten!H33+'Eingabedaten (berechnet)'!V32</f>
-        <v>39</v>
+        <v>64.5</v>
       </c>
       <c r="W33" s="10">
         <f>Eingabedaten!I33+'Eingabedaten (berechnet)'!W32</f>
-        <v>70.75</v>
+        <v>104.75</v>
       </c>
       <c r="X33" s="10">
         <f t="shared" si="7"/>
-        <v>261.75</v>
+        <v>337.75</v>
       </c>
       <c r="Z33" s="10">
         <f>Z32+Eingabedaten!K33</f>
@@ -11165,23 +11257,23 @@
       </c>
       <c r="AB33" s="10">
         <f>AB32+Eingabedaten!M33</f>
-        <v>116</v>
+        <v>147</v>
       </c>
       <c r="AC33" s="10">
         <f>AC32+Eingabedaten!N33</f>
-        <v>12.5</v>
+        <v>16.5</v>
       </c>
       <c r="AD33" s="10">
         <f>AD32+Eingabedaten!O33</f>
-        <v>19.25</v>
+        <v>43.75</v>
       </c>
       <c r="AE33" s="10">
         <f t="shared" si="8"/>
-        <v>293.25</v>
+        <v>352.75</v>
       </c>
       <c r="AG33" s="10">
         <f t="shared" si="9"/>
-        <v>555</v>
+        <v>690.5</v>
       </c>
     </row>
     <row r="35" spans="2:33">
@@ -11195,25 +11287,25 @@
       </c>
       <c r="G35" s="6">
         <f t="shared" si="12"/>
-        <v>196.5</v>
+        <v>244</v>
       </c>
       <c r="H35" s="6">
         <f t="shared" si="12"/>
-        <v>51.5</v>
+        <v>81</v>
       </c>
       <c r="I35" s="6">
         <f t="shared" si="12"/>
-        <v>90</v>
+        <v>148.5</v>
       </c>
       <c r="J35" s="6">
         <f t="shared" si="12"/>
-        <v>555</v>
+        <v>690.5</v>
       </c>
     </row>
     <row r="36" spans="2:33">
       <c r="E36" s="6">
         <f>SUM(E35:I35)</f>
-        <v>555</v>
+        <v>690.5</v>
       </c>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>

</xml_diff>

<commit_message>
Add last hours, before 'closing' this document.
</commit_message>
<xml_diff>
--- a/ProjektManagement/NuvoControl_0011_StundenNachweis_Grafisch.xlsx
+++ b/ProjektManagement/NuvoControl_0011_StundenNachweis_Grafisch.xlsx
@@ -157,10 +157,10 @@
     <t>e / 10-Aug-2009</t>
   </si>
   <si>
-    <t>f / 22-Aug-2009</t>
+    <t>Finale Version für die Abgabe</t>
   </si>
   <si>
-    <t>Zwischenstand kurz vor Abgabe</t>
+    <t>f / 24-Aug-2009</t>
   </si>
 </sst>
 </file>
@@ -307,7 +307,7 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+  <c:lang val="de-CH"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -708,21 +708,21 @@
                   <c:v>296.75</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>337.75</c:v>
+                  <c:v>349.75</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>337.75</c:v>
+                  <c:v>360.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="132957312"/>
-        <c:axId val="132958848"/>
+        <c:axId val="129283200"/>
+        <c:axId val="129284736"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="132957312"/>
+        <c:axId val="129283200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -737,16 +737,16 @@
             <a:pPr>
               <a:defRPr lang="de-CH"/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="132958848"/>
+        <c:crossAx val="129284736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="132958848"/>
+        <c:axId val="129284736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -761,7 +761,7 @@
               <a:pPr>
                 <a:defRPr lang="de-CH"/>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -775,10 +775,10 @@
             <a:pPr>
               <a:defRPr lang="de-CH"/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="132957312"/>
+        <c:crossAx val="129283200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -793,7 +793,7 @@
           <a:pPr>
             <a:defRPr lang="de-CH"/>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -809,7 +809,7 @@
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+  <c:lang val="de-CH"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1210,21 +1210,21 @@
                   <c:v>328.75</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>352.75</c:v>
+                  <c:v>358.25</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>352.75</c:v>
+                  <c:v>361.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="133009408"/>
-        <c:axId val="133010944"/>
+        <c:axId val="129335296"/>
+        <c:axId val="129336832"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="133009408"/>
+        <c:axId val="129335296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1239,16 +1239,16 @@
             <a:pPr>
               <a:defRPr lang="de-CH"/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="133010944"/>
+        <c:crossAx val="129336832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="133010944"/>
+        <c:axId val="129336832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1263,7 +1263,7 @@
               <a:pPr>
                 <a:defRPr lang="de-CH"/>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1277,10 +1277,10 @@
             <a:pPr>
               <a:defRPr lang="de-CH"/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="133009408"/>
+        <c:crossAx val="129335296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1295,7 +1295,7 @@
           <a:pPr>
             <a:defRPr lang="de-CH"/>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1311,7 +1311,7 @@
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+  <c:lang val="de-CH"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1712,21 +1712,21 @@
                   <c:v>625.5</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>690.5</c:v>
+                  <c:v>708</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>690.5</c:v>
+                  <c:v>722</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="133032192"/>
-        <c:axId val="125046784"/>
+        <c:axId val="129358080"/>
+        <c:axId val="130678784"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="133032192"/>
+        <c:axId val="129358080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1741,16 +1741,16 @@
             <a:pPr>
               <a:defRPr lang="de-CH"/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="125046784"/>
+        <c:crossAx val="130678784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="125046784"/>
+        <c:axId val="130678784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1765,7 +1765,7 @@
               <a:pPr>
                 <a:defRPr lang="de-CH"/>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1779,10 +1779,10 @@
             <a:pPr>
               <a:defRPr lang="de-CH"/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="133032192"/>
+        <c:crossAx val="129358080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1797,7 +1797,7 @@
           <a:pPr>
             <a:defRPr lang="de-CH"/>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1813,7 +1813,7 @@
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+  <c:lang val="de-CH"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -2112,7 +2112,7 @@
                   <c:v>3.5</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>9</c:v>
+                  <c:v>10.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2538,18 +2538,21 @@
                   <c:v>16.5</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>17</c:v>
+                  <c:v>27.5</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="125218176"/>
-        <c:axId val="125109376"/>
+        <c:axId val="130854272"/>
+        <c:axId val="130745472"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="125218176"/>
+        <c:axId val="130854272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2564,16 +2567,16 @@
             <a:pPr>
               <a:defRPr lang="de-CH"/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="125109376"/>
+        <c:crossAx val="130745472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="125109376"/>
+        <c:axId val="130745472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2615,10 +2618,10 @@
             <a:pPr>
               <a:defRPr lang="de-CH"/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="125218176"/>
+        <c:crossAx val="130854272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2633,7 +2636,7 @@
           <a:pPr>
             <a:defRPr lang="de-CH"/>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2649,7 +2652,7 @@
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+  <c:lang val="de-CH"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -2790,6 +2793,9 @@
                 <c:pt idx="25">
                   <c:v>4</c:v>
                 </c:pt>
+                <c:pt idx="26">
+                  <c:v>3</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3344,18 +3350,21 @@
                   <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>12</c:v>
+                  <c:v>14.5</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="125161856"/>
-        <c:axId val="125163392"/>
+        <c:axId val="130802048"/>
+        <c:axId val="130803584"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="125161856"/>
+        <c:axId val="130802048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3370,16 +3379,16 @@
             <a:pPr>
               <a:defRPr lang="de-CH"/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="125163392"/>
+        <c:crossAx val="130803584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="125163392"/>
+        <c:axId val="130803584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3421,10 +3430,10 @@
             <a:pPr>
               <a:defRPr lang="de-CH"/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="125161856"/>
+        <c:crossAx val="130802048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3439,7 +3448,7 @@
           <a:pPr>
             <a:defRPr lang="de-CH"/>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3455,7 +3464,7 @@
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+  <c:lang val="de-CH"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -3861,10 +3870,10 @@
                   <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>97</c:v>
+                  <c:v>98.5</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>97</c:v>
+                  <c:v>98.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4440,21 +4449,21 @@
                   <c:v>87.75</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>104.75</c:v>
+                  <c:v>115.25</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>104.75</c:v>
+                  <c:v>126.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="125281792"/>
-        <c:axId val="125283328"/>
+        <c:axId val="130917888"/>
+        <c:axId val="130919424"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="125281792"/>
+        <c:axId val="130917888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4469,16 +4478,16 @@
             <a:pPr>
               <a:defRPr lang="de-CH"/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="125283328"/>
+        <c:crossAx val="130919424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="125283328"/>
+        <c:axId val="130919424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4520,10 +4529,10 @@
             <a:pPr>
               <a:defRPr lang="de-CH"/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="125281792"/>
+        <c:crossAx val="130917888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4538,7 +4547,7 @@
           <a:pPr>
             <a:defRPr lang="de-CH"/>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4554,7 +4563,7 @@
 
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+  <c:lang val="de-CH"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -4767,10 +4776,10 @@
                   <c:v>16.5</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>16.5</c:v>
+                  <c:v>19.5</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>16.5</c:v>
+                  <c:v>19.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5539,21 +5548,21 @@
                   <c:v>31.75</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>43.75</c:v>
+                  <c:v>46.25</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>43.75</c:v>
+                  <c:v>49.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="125446016"/>
-        <c:axId val="125447552"/>
+        <c:axId val="131082112"/>
+        <c:axId val="131083648"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="125446016"/>
+        <c:axId val="131082112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5568,16 +5577,16 @@
             <a:pPr>
               <a:defRPr lang="de-CH"/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="125447552"/>
+        <c:crossAx val="131083648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="125447552"/>
+        <c:axId val="131083648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5619,10 +5628,10 @@
             <a:pPr>
               <a:defRPr lang="de-CH"/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="125446016"/>
+        <c:crossAx val="131082112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5637,7 +5646,7 @@
           <a:pPr>
             <a:defRPr lang="de-CH"/>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -6162,7 +6171,7 @@
   <dimension ref="B3:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -6220,10 +6229,10 @@
     </row>
     <row r="9" spans="2:5">
       <c r="C9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" t="s">
         <v>35</v>
-      </c>
-      <c r="E9" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -6243,8 +6252,8 @@
   <dimension ref="B2:O39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G32" sqref="G32"/>
+      <pane ySplit="5" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -7123,16 +7132,16 @@
       <c r="E32" s="9"/>
       <c r="F32" s="9"/>
       <c r="G32" s="9">
-        <f>2.5+6+0.5</f>
-        <v>9</v>
+        <f>2.5+6+0.5+1.5</f>
+        <v>10.5</v>
       </c>
       <c r="H32" s="9">
         <f>4+4+7</f>
         <v>15</v>
       </c>
       <c r="I32" s="9">
-        <f>2.5+4.5+6+2+0.5+1.5</f>
-        <v>17</v>
+        <f>2.5+4.5+6+2+0.5+1.5+1+2.5+1+6</f>
+        <v>27.5</v>
       </c>
       <c r="K32" s="9"/>
       <c r="L32" s="9"/>
@@ -7140,10 +7149,13 @@
         <f>4+8</f>
         <v>12</v>
       </c>
-      <c r="N32" s="9"/>
+      <c r="N32" s="9">
+        <f>3</f>
+        <v>3</v>
+      </c>
       <c r="O32" s="9">
-        <f>2+3+7</f>
-        <v>12</v>
+        <f>2+3+7+2.5</f>
+        <v>14.5</v>
       </c>
     </row>
     <row r="33" spans="2:15">
@@ -7159,12 +7171,18 @@
       <c r="F33" s="9"/>
       <c r="G33" s="9"/>
       <c r="H33" s="9"/>
-      <c r="I33" s="9"/>
+      <c r="I33" s="9">
+        <f>8+3</f>
+        <v>11</v>
+      </c>
       <c r="K33" s="9"/>
       <c r="L33" s="9"/>
       <c r="M33" s="9"/>
       <c r="N33" s="9"/>
-      <c r="O33" s="9"/>
+      <c r="O33" s="9">
+        <f>3</f>
+        <v>3</v>
+      </c>
     </row>
     <row r="35" spans="2:15">
       <c r="B35" s="4" t="s">
@@ -7181,7 +7199,7 @@
       </c>
       <c r="G35" s="6">
         <f>SUM(G6:G33)</f>
-        <v>97</v>
+        <v>98.5</v>
       </c>
       <c r="H35" s="6">
         <f>SUM(H6:H33)</f>
@@ -7189,7 +7207,7 @@
       </c>
       <c r="I35" s="6">
         <f>SUM(I6:I33)</f>
-        <v>104.75</v>
+        <v>126.25</v>
       </c>
       <c r="K35" s="6">
         <f>SUM(K6:K33)</f>
@@ -7205,11 +7223,11 @@
       </c>
       <c r="N35" s="6">
         <f>SUM(N6:N33)</f>
-        <v>16.5</v>
+        <v>19.5</v>
       </c>
       <c r="O35" s="6">
         <f>SUM(O6:O33)</f>
-        <v>43.75</v>
+        <v>49.25</v>
       </c>
     </row>
     <row r="36" spans="2:15">
@@ -7219,7 +7237,7 @@
       <c r="C36" s="5"/>
       <c r="E36" s="6">
         <f>SUM(E35:I35)</f>
-        <v>337.75</v>
+        <v>360.75</v>
       </c>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
@@ -7227,7 +7245,7 @@
       <c r="I36" s="7"/>
       <c r="K36" s="6">
         <f>SUM(K35:O35)</f>
-        <v>352.75</v>
+        <v>361.25</v>
       </c>
       <c r="L36" s="7"/>
       <c r="M36" s="7"/>
@@ -7249,15 +7267,15 @@
       </c>
       <c r="G38" s="6">
         <f>G35+M35</f>
-        <v>244</v>
+        <v>245.5</v>
       </c>
       <c r="H38" s="6">
         <f>H35+N35</f>
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="I38" s="6">
         <f>I35+O35</f>
-        <v>148.5</v>
+        <v>175.5</v>
       </c>
     </row>
     <row r="39" spans="2:15">
@@ -7267,7 +7285,7 @@
       <c r="C39" s="5"/>
       <c r="E39" s="6">
         <f>SUM(E38:I38)</f>
-        <v>690.5</v>
+        <v>722</v>
       </c>
     </row>
   </sheetData>
@@ -7291,7 +7309,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="A12" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="N43" sqref="N43"/>
     </sheetView>
   </sheetViews>
@@ -7311,7 +7329,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScale="60" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="K53" sqref="K53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -11075,19 +11093,19 @@
       </c>
       <c r="G32" s="10">
         <f>Eingabedaten!G32+Eingabedaten!M32</f>
-        <v>21</v>
+        <v>22.5</v>
       </c>
       <c r="H32" s="10">
         <f>Eingabedaten!H32+Eingabedaten!N32</f>
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="I32" s="10">
         <f>Eingabedaten!I32+Eingabedaten!O32</f>
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="J32" s="10">
         <f t="shared" si="5"/>
-        <v>65</v>
+        <v>82.5</v>
       </c>
       <c r="L32" s="10">
         <f t="shared" si="0"/>
@@ -11099,19 +11117,19 @@
       </c>
       <c r="N32" s="10">
         <f t="shared" si="2"/>
-        <v>21</v>
+        <v>22.5</v>
       </c>
       <c r="O32" s="10">
         <f t="shared" si="3"/>
-        <v>36</v>
+        <v>40.5</v>
       </c>
       <c r="P32" s="10">
         <f t="shared" si="4"/>
-        <v>65</v>
+        <v>82.5</v>
       </c>
       <c r="Q32" s="10">
         <f t="shared" si="6"/>
-        <v>122</v>
+        <v>145.5</v>
       </c>
       <c r="S32" s="10">
         <f>Eingabedaten!E32+'Eingabedaten (berechnet)'!S31</f>
@@ -11123,7 +11141,7 @@
       </c>
       <c r="U32" s="10">
         <f>Eingabedaten!G32+'Eingabedaten (berechnet)'!U31</f>
-        <v>97</v>
+        <v>98.5</v>
       </c>
       <c r="V32" s="10">
         <f>Eingabedaten!H32+'Eingabedaten (berechnet)'!V31</f>
@@ -11131,11 +11149,11 @@
       </c>
       <c r="W32" s="10">
         <f>Eingabedaten!I32+'Eingabedaten (berechnet)'!W31</f>
-        <v>104.75</v>
+        <v>115.25</v>
       </c>
       <c r="X32" s="10">
         <f t="shared" si="7"/>
-        <v>337.75</v>
+        <v>349.75</v>
       </c>
       <c r="Z32" s="10">
         <f>Z31+Eingabedaten!K32</f>
@@ -11151,19 +11169,19 @@
       </c>
       <c r="AC32" s="10">
         <f>AC31+Eingabedaten!N32</f>
-        <v>16.5</v>
+        <v>19.5</v>
       </c>
       <c r="AD32" s="10">
         <f>AD31+Eingabedaten!O32</f>
-        <v>43.75</v>
+        <v>46.25</v>
       </c>
       <c r="AE32" s="10">
         <f t="shared" si="8"/>
-        <v>352.75</v>
+        <v>358.25</v>
       </c>
       <c r="AG32" s="10">
         <f t="shared" si="9"/>
-        <v>690.5</v>
+        <v>708</v>
       </c>
     </row>
     <row r="33" spans="2:33">
@@ -11193,11 +11211,11 @@
       </c>
       <c r="I33" s="10">
         <f>Eingabedaten!I33+Eingabedaten!O33</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="J33" s="10">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="L33" s="10">
         <f t="shared" si="0"/>
@@ -11217,11 +11235,11 @@
       </c>
       <c r="P33" s="10">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="Q33" s="10">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="S33" s="10">
         <f>Eingabedaten!E33+'Eingabedaten (berechnet)'!S32</f>
@@ -11233,7 +11251,7 @@
       </c>
       <c r="U33" s="10">
         <f>Eingabedaten!G33+'Eingabedaten (berechnet)'!U32</f>
-        <v>97</v>
+        <v>98.5</v>
       </c>
       <c r="V33" s="10">
         <f>Eingabedaten!H33+'Eingabedaten (berechnet)'!V32</f>
@@ -11241,11 +11259,11 @@
       </c>
       <c r="W33" s="10">
         <f>Eingabedaten!I33+'Eingabedaten (berechnet)'!W32</f>
-        <v>104.75</v>
+        <v>126.25</v>
       </c>
       <c r="X33" s="10">
         <f t="shared" si="7"/>
-        <v>337.75</v>
+        <v>360.75</v>
       </c>
       <c r="Z33" s="10">
         <f>Z32+Eingabedaten!K33</f>
@@ -11261,19 +11279,19 @@
       </c>
       <c r="AC33" s="10">
         <f>AC32+Eingabedaten!N33</f>
-        <v>16.5</v>
+        <v>19.5</v>
       </c>
       <c r="AD33" s="10">
         <f>AD32+Eingabedaten!O33</f>
-        <v>43.75</v>
+        <v>49.25</v>
       </c>
       <c r="AE33" s="10">
         <f t="shared" si="8"/>
-        <v>352.75</v>
+        <v>361.25</v>
       </c>
       <c r="AG33" s="10">
         <f t="shared" si="9"/>
-        <v>690.5</v>
+        <v>722</v>
       </c>
     </row>
     <row r="35" spans="2:33">
@@ -11287,25 +11305,25 @@
       </c>
       <c r="G35" s="6">
         <f t="shared" si="12"/>
-        <v>244</v>
+        <v>245.5</v>
       </c>
       <c r="H35" s="6">
         <f t="shared" si="12"/>
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="I35" s="6">
         <f t="shared" si="12"/>
-        <v>148.5</v>
+        <v>175.5</v>
       </c>
       <c r="J35" s="6">
         <f t="shared" si="12"/>
-        <v>690.5</v>
+        <v>722</v>
       </c>
     </row>
     <row r="36" spans="2:33">
       <c r="E36" s="6">
         <f>SUM(E35:I35)</f>
-        <v>690.5</v>
+        <v>722</v>
       </c>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>

</xml_diff>